<commit_message>
Se incluye formula de creación de objetos
La formula para crear objetos de una manera facil y rapidoa
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="284">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -875,6 +875,9 @@
   </si>
   <si>
     <t>PagePagaTuFacturaMovil</t>
+  </si>
+  <si>
+    <t>Creación</t>
   </si>
 </sst>
 </file>
@@ -1398,6 +1401,12 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1484,12 +1493,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2080,78 +2083,78 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="89"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
+      <c r="A15" s="91"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="89"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="89"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="89"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="89"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="89"/>
-      <c r="B22" s="89"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="89"/>
+      <c r="A22" s="91"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2184,17 +2187,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -4440,14 +4443,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4470,7 +4473,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="105" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4490,7 +4493,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="104"/>
+      <c r="A4" s="106"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -4508,7 +4511,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="104"/>
+      <c r="A5" s="106"/>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -4526,7 +4529,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="104"/>
+      <c r="A6" s="106"/>
       <c r="B6" s="3" t="s">
         <v>101</v>
       </c>
@@ -4544,7 +4547,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
+      <c r="A7" s="106"/>
       <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
@@ -4565,7 +4568,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
+      <c r="A8" s="106"/>
       <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
@@ -4586,7 +4589,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="105"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="3" t="s">
         <v>229</v>
       </c>
@@ -4604,7 +4607,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="112" t="s">
+      <c r="A10" s="114" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -4624,7 +4627,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="113"/>
+      <c r="A11" s="115"/>
       <c r="B11" s="7" t="s">
         <v>124</v>
       </c>
@@ -4645,7 +4648,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="113"/>
+      <c r="A12" s="115"/>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -4663,7 +4666,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="113"/>
+      <c r="A13" s="115"/>
       <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
@@ -4684,7 +4687,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="113"/>
+      <c r="A14" s="115"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -4702,7 +4705,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
+      <c r="A15" s="115"/>
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -4720,7 +4723,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="113"/>
+      <c r="A16" s="115"/>
       <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
@@ -4738,7 +4741,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="113"/>
+      <c r="A17" s="115"/>
       <c r="B17" s="7" t="s">
         <v>101</v>
       </c>
@@ -4756,7 +4759,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="113"/>
+      <c r="A18" s="115"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -4774,7 +4777,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="114"/>
+      <c r="A19" s="116"/>
       <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
@@ -4792,7 +4795,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="99" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -4812,7 +4815,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="98"/>
+      <c r="A21" s="100"/>
       <c r="B21" s="4" t="s">
         <v>81</v>
       </c>
@@ -4837,7 +4840,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="98"/>
+      <c r="A22" s="100"/>
       <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
@@ -4855,7 +4858,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="98"/>
+      <c r="A23" s="100"/>
       <c r="B23" s="4" t="s">
         <v>82</v>
       </c>
@@ -4873,7 +4876,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="99"/>
+      <c r="A24" s="101"/>
       <c r="B24" s="4" t="s">
         <v>83</v>
       </c>
@@ -4898,7 +4901,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="102" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -4918,7 +4921,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="101"/>
+      <c r="A26" s="103"/>
       <c r="B26" s="13" t="s">
         <v>27</v>
       </c>
@@ -4936,7 +4939,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="102"/>
+      <c r="A27" s="104"/>
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -4954,7 +4957,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="115" t="s">
+      <c r="A28" s="117" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -4974,7 +4977,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="116"/>
+      <c r="A29" s="118"/>
       <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
@@ -4995,7 +4998,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="116"/>
+      <c r="A30" s="118"/>
       <c r="B30" s="15" t="s">
         <v>118</v>
       </c>
@@ -5016,7 +5019,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="116"/>
+      <c r="A31" s="118"/>
       <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
@@ -5034,7 +5037,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="116"/>
+      <c r="A32" s="118"/>
       <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
@@ -5052,7 +5055,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="116"/>
+      <c r="A33" s="118"/>
       <c r="B33" s="15" t="s">
         <v>35</v>
       </c>
@@ -5070,7 +5073,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="116"/>
+      <c r="A34" s="118"/>
       <c r="B34" s="15" t="s">
         <v>36</v>
       </c>
@@ -5088,7 +5091,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="116"/>
+      <c r="A35" s="118"/>
       <c r="B35" s="15" t="s">
         <v>39</v>
       </c>
@@ -5106,7 +5109,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="116"/>
+      <c r="A36" s="118"/>
       <c r="B36" s="15" t="s">
         <v>3</v>
       </c>
@@ -5124,7 +5127,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="116"/>
+      <c r="A37" s="118"/>
       <c r="B37" s="15" t="s">
         <v>42</v>
       </c>
@@ -5142,7 +5145,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="116"/>
+      <c r="A38" s="118"/>
       <c r="B38" s="15" t="s">
         <v>122</v>
       </c>
@@ -5163,7 +5166,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="116"/>
+      <c r="A39" s="118"/>
       <c r="B39" s="15" t="s">
         <v>44</v>
       </c>
@@ -5181,7 +5184,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="116"/>
+      <c r="A40" s="118"/>
       <c r="B40" s="15" t="s">
         <v>130</v>
       </c>
@@ -5202,7 +5205,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="116"/>
+      <c r="A41" s="118"/>
       <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
@@ -5220,7 +5223,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="116"/>
+      <c r="A42" s="118"/>
       <c r="B42" s="15" t="s">
         <v>110</v>
       </c>
@@ -5241,7 +5244,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="116"/>
+      <c r="A43" s="118"/>
       <c r="B43" s="15" t="s">
         <v>47</v>
       </c>
@@ -5257,7 +5260,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="116"/>
+      <c r="A44" s="118"/>
       <c r="B44" s="15" t="s">
         <v>101</v>
       </c>
@@ -5273,7 +5276,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="116"/>
+      <c r="A45" s="118"/>
       <c r="B45" s="15" t="s">
         <v>22</v>
       </c>
@@ -5291,7 +5294,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="117"/>
+      <c r="A46" s="119"/>
       <c r="B46" s="15" t="s">
         <v>51</v>
       </c>
@@ -5309,7 +5312,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="106" t="s">
+      <c r="A47" s="108" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -5329,7 +5332,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="107"/>
+      <c r="A48" s="109"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -5347,7 +5350,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="107"/>
+      <c r="A49" s="109"/>
       <c r="B49" s="5" t="s">
         <v>56</v>
       </c>
@@ -5365,7 +5368,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="107"/>
+      <c r="A50" s="109"/>
       <c r="B50" s="5" t="s">
         <v>3</v>
       </c>
@@ -5383,7 +5386,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="107"/>
+      <c r="A51" s="109"/>
       <c r="B51" s="5" t="s">
         <v>60</v>
       </c>
@@ -5401,7 +5404,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="107"/>
+      <c r="A52" s="109"/>
       <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
@@ -5419,7 +5422,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="107"/>
+      <c r="A53" s="109"/>
       <c r="B53" s="5" t="s">
         <v>101</v>
       </c>
@@ -5435,7 +5438,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="107"/>
+      <c r="A54" s="109"/>
       <c r="B54" s="5" t="s">
         <v>22</v>
       </c>
@@ -5453,7 +5456,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="108"/>
+      <c r="A55" s="110"/>
       <c r="B55" s="5" t="s">
         <v>64</v>
       </c>
@@ -5471,7 +5474,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="109" t="s">
+      <c r="A56" s="111" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -5491,7 +5494,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="110"/>
+      <c r="A57" s="112"/>
       <c r="B57" s="1" t="s">
         <v>101</v>
       </c>
@@ -5507,7 +5510,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="110"/>
+      <c r="A58" s="112"/>
       <c r="B58" s="1" t="s">
         <v>22</v>
       </c>
@@ -5525,7 +5528,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="111"/>
+      <c r="A59" s="113"/>
       <c r="B59" s="1" t="s">
         <v>48</v>
       </c>
@@ -5543,7 +5546,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="92" t="s">
+      <c r="A60" s="94" t="s">
         <v>136</v>
       </c>
       <c r="B60" s="23" t="s">
@@ -5566,7 +5569,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="93"/>
+      <c r="A61" s="95"/>
       <c r="B61" s="23" t="s">
         <v>137</v>
       </c>
@@ -5584,7 +5587,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="93"/>
+      <c r="A62" s="95"/>
       <c r="B62" s="23" t="s">
         <v>138</v>
       </c>
@@ -5602,7 +5605,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="93"/>
+      <c r="A63" s="95"/>
       <c r="B63" s="23" t="s">
         <v>139</v>
       </c>
@@ -5620,7 +5623,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="93"/>
+      <c r="A64" s="95"/>
       <c r="B64" s="23" t="s">
         <v>140</v>
       </c>
@@ -5638,7 +5641,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="93"/>
+      <c r="A65" s="95"/>
       <c r="B65" s="23" t="s">
         <v>141</v>
       </c>
@@ -5656,7 +5659,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="93"/>
+      <c r="A66" s="95"/>
       <c r="B66" s="23" t="s">
         <v>142</v>
       </c>
@@ -5674,7 +5677,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="93"/>
+      <c r="A67" s="95"/>
       <c r="B67" s="23" t="s">
         <v>143</v>
       </c>
@@ -5692,7 +5695,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="93"/>
+      <c r="A68" s="95"/>
       <c r="B68" s="23" t="s">
         <v>144</v>
       </c>
@@ -5710,7 +5713,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="93"/>
+      <c r="A69" s="95"/>
       <c r="B69" s="23" t="s">
         <v>145</v>
       </c>
@@ -5728,7 +5731,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="93"/>
+      <c r="A70" s="95"/>
       <c r="B70" s="23" t="s">
         <v>146</v>
       </c>
@@ -5746,7 +5749,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="93"/>
+      <c r="A71" s="95"/>
       <c r="B71" s="23" t="s">
         <v>147</v>
       </c>
@@ -5764,7 +5767,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="93"/>
+      <c r="A72" s="95"/>
       <c r="B72" s="23" t="s">
         <v>148</v>
       </c>
@@ -5782,7 +5785,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="93"/>
+      <c r="A73" s="95"/>
       <c r="B73" s="23" t="s">
         <v>149</v>
       </c>
@@ -5800,7 +5803,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="94"/>
+      <c r="A74" s="96"/>
       <c r="B74" s="23" t="s">
         <v>150</v>
       </c>
@@ -5969,28 +5972,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" style="39" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="39"/>
+    <col min="3" max="3" width="27.140625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="61" style="39" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="39"/>
+    <col min="6" max="6" width="11.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
@@ -6003,8 +6009,11 @@
       <c r="D2" s="47" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>282</v>
       </c>
@@ -6017,8 +6026,12 @@
       <c r="D3" s="48" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="39" t="str">
+        <f t="shared" ref="E3:E66" si="0">CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath("""),D3,""");")</f>
+        <v>public By btnMovil=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[1]/div/div/div[2]/p");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>282</v>
       </c>
@@ -6031,8 +6044,12 @@
       <c r="D4" s="48" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnHogar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[1]/div/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>282</v>
       </c>
@@ -6045,8 +6062,12 @@
       <c r="D5" s="48" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtTuLineaTigo=By.FALSOid="edit-candidate-number"");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>282</v>
       </c>
@@ -6059,8 +6080,12 @@
       <c r="D6" s="48" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.FALSOid="edit-email"");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>282</v>
       </c>
@@ -6073,8 +6098,12 @@
       <c r="D7" s="48" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosyCondiciones=By.xpath("//*[@id="tyc_Movil"]");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>282</v>
       </c>
@@ -6087,8 +6116,12 @@
       <c r="D8" s="48" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnConsultar=By.FALSOid="edit-consult"");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>282</v>
       </c>
@@ -6099,8 +6132,12 @@
         <v>229</v>
       </c>
       <c r="D9" s="48"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By CapcharCaptchar=By.FALSO");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>231</v>
       </c>
@@ -6113,8 +6150,12 @@
       <c r="D10" s="51" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="39" t="str">
+        <f>CONCATENATE("public By ",B10,C10,"=By.",IF(ISNUMBER(SEARCH("@id=",D10)),"xpath("""),D10,""");")</f>
+        <v>public By btnMovil=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[1]/div/div/div[2]/p");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>231</v>
       </c>
@@ -6127,8 +6168,12 @@
       <c r="D11" s="51" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnHogar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[1]/div/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>231</v>
       </c>
@@ -6141,8 +6186,12 @@
       <c r="D12" s="51" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipoDocumento=By.FALSOid="edit-document-type"");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>231</v>
       </c>
@@ -6155,8 +6204,12 @@
       <c r="D13" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumeroDocumento=By.FALSOid="edit-document"");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>231</v>
       </c>
@@ -6169,8 +6222,12 @@
       <c r="D14" s="51" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.xpath("//*[@id="content_right_forms_unified"]/div/div/label");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>231</v>
       </c>
@@ -6183,8 +6240,12 @@
       <c r="D15" s="51" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosyCondiciones=By.xpath("//*[@id="tyc_Fijo"]");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>231</v>
       </c>
@@ -6196,6 +6257,10 @@
       </c>
       <c r="D16" s="51" t="s">
         <v>203</v>
+      </c>
+      <c r="E16" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnConsultar=By.FALSOid="edit-consult--2"");</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6209,6 +6274,10 @@
         <v>229</v>
       </c>
       <c r="D17" s="51"/>
+      <c r="E17" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By CapcharCaptchar=By.FALSO");</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
@@ -6223,6 +6292,10 @@
       <c r="D18" s="53" t="s">
         <v>160</v>
       </c>
+      <c r="E18" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodeLinea=By.xpath("//*[@id='value']");</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
@@ -6237,6 +6310,10 @@
       <c r="D19" s="53" t="s">
         <v>161</v>
       </c>
+      <c r="E19" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtFechaLimitePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[1]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
@@ -6251,6 +6328,10 @@
       <c r="D20" s="53" t="s">
         <v>162</v>
       </c>
+      <c r="E20" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtReferentePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
@@ -6265,6 +6346,10 @@
       <c r="D21" s="53" t="s">
         <v>163</v>
       </c>
+      <c r="E21" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtPeriodoFacturacion=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
@@ -6279,6 +6364,10 @@
       <c r="D22" s="53" t="s">
         <v>164</v>
       </c>
+      <c r="E22" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtValorPagar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[4]/div[2]");</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
@@ -6293,6 +6382,10 @@
       <c r="D23" s="34" t="s">
         <v>87</v>
       </c>
+      <c r="E23" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTarjetaCredito=By.FALSOpayment-method-type-label-credit-payu");</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
@@ -6307,6 +6400,10 @@
       <c r="D24" s="34" t="s">
         <v>88</v>
       </c>
+      <c r="E24" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkDebitoBancarioPSE=By.FALSOpayment-method-type-label-debit-payu");</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
@@ -6321,6 +6418,10 @@
       <c r="D25" s="34" t="s">
         <v>89</v>
       </c>
+      <c r="E25" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkOtrosmediosdepago=By.FALSOpayment-method-type-label-others-pay-methods");</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
@@ -6335,6 +6436,10 @@
       <c r="D26" s="35" t="s">
         <v>29</v>
       </c>
+      <c r="E26" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodetarjeta=By.FALSOedit-cardnumber");</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
@@ -6349,8 +6454,9 @@
       <c r="D27" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="E27" s="39" t="s">
-        <v>119</v>
+      <c r="E27" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -6366,8 +6472,9 @@
       <c r="D28" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="E28" s="55" t="s">
-        <v>121</v>
+      <c r="E28" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -6383,6 +6490,10 @@
       <c r="D29" s="35" t="s">
         <v>31</v>
       </c>
+      <c r="E29" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCVV/CVC=By.FALSOedit-cvc");</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
@@ -6397,6 +6508,10 @@
       <c r="D30" s="35" t="s">
         <v>33</v>
       </c>
+      <c r="E30" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listFechaVencimiento-MM=By.FALSOedit-buyer-card-month-expiration");</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
@@ -6411,6 +6526,10 @@
       <c r="D31" s="35" t="s">
         <v>34</v>
       </c>
+      <c r="E31" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listFechaVencimiento-AA=By.FALSOedit-buyer-card-year-expiration");</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
@@ -6425,6 +6544,10 @@
       <c r="D32" s="35" t="s">
         <v>37</v>
       </c>
+      <c r="E32" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listCuotas=By.FALSOedit-cardnumber-quota");</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
@@ -6439,6 +6562,10 @@
       <c r="D33" s="35" t="s">
         <v>38</v>
       </c>
+      <c r="E33" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNombre=By.FALSOedit-ccname");</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
@@ -6453,6 +6580,10 @@
       <c r="D34" s="35" t="s">
         <v>40</v>
       </c>
+      <c r="E34" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipo=By.FALSOedit-buyer-document-type");</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
@@ -6467,6 +6598,10 @@
       <c r="D35" s="35" t="s">
         <v>41</v>
       </c>
+      <c r="E35" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodedocumento=By.FALSOedit-buyer-document");</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
@@ -6481,8 +6616,9 @@
       <c r="D36" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="E36" s="39" t="s">
-        <v>127</v>
+      <c r="E36" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -6498,6 +6634,10 @@
       <c r="D37" s="35" t="s">
         <v>43</v>
       </c>
+      <c r="E37" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.FALSOedit-buyer-phone");</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
@@ -6512,8 +6652,9 @@
       <c r="D38" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="39" t="s">
-        <v>131</v>
+      <c r="E38" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -6529,6 +6670,10 @@
       <c r="D39" s="35" t="s">
         <v>45</v>
       </c>
+      <c r="E39" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.FALSOedit-buyer-mail");</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
@@ -6543,8 +6688,9 @@
       <c r="D40" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="E40" s="55" t="s">
-        <v>129</v>
+      <c r="E40" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -6560,6 +6706,10 @@
       <c r="D41" s="35" t="s">
         <v>46</v>
       </c>
+      <c r="E41" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.FALSOedit-buyer-check-authorize");</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
@@ -6574,6 +6724,10 @@
       <c r="D42" s="35" t="s">
         <v>169</v>
       </c>
+      <c r="E42" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
@@ -6588,6 +6742,10 @@
       <c r="D43" s="35" t="s">
         <v>49</v>
       </c>
+      <c r="E43" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.FALSOedit-cancel");</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
@@ -6602,6 +6760,10 @@
       <c r="D44" s="35" t="s">
         <v>50</v>
       </c>
+      <c r="E44" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.FALSOedit-submit");</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
@@ -6616,6 +6778,10 @@
       <c r="D45" s="36" t="s">
         <v>53</v>
       </c>
+      <c r="E45" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listBanco=By.FALSOedit-bank");</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
@@ -6630,6 +6796,10 @@
       <c r="D46" s="36" t="s">
         <v>54</v>
       </c>
+      <c r="E46" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipodepersona=By.FALSOedit-buyer-type-person");</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
@@ -6644,6 +6814,10 @@
       <c r="D47" s="36" t="s">
         <v>57</v>
       </c>
+      <c r="E47" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNombresyapellidos=By.FALSOedit-buyer-name");</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
@@ -6658,6 +6832,10 @@
       <c r="D48" s="36" t="s">
         <v>58</v>
       </c>
+      <c r="E48" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipo=By.FALSOedit-buyer-document-type--2");</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
@@ -6672,6 +6850,10 @@
       <c r="D49" s="36" t="s">
         <v>59</v>
       </c>
+      <c r="E49" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodedocumento=By.FALSOedit-buyer-document--2");</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
@@ -6686,8 +6868,9 @@
       <c r="D50" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="E50" s="39" t="s">
-        <v>204</v>
+      <c r="E50" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id="edit-content-document--2"]/div/p");</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -6703,6 +6886,10 @@
       <c r="D51" s="36" t="s">
         <v>61</v>
       </c>
+      <c r="E51" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.FALSOedit-buyer-mail--2");</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
@@ -6717,6 +6904,10 @@
       <c r="D52" s="36" t="s">
         <v>207</v>
       </c>
+      <c r="E52" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id="edit-show-email--2"]/div/p");</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
@@ -6731,6 +6922,10 @@
       <c r="D53" s="36" t="s">
         <v>208</v>
       </c>
+      <c r="E53" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id="edit-terms--2"]/div/a");</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
@@ -6745,6 +6940,10 @@
       <c r="D54" s="36" t="s">
         <v>63</v>
       </c>
+      <c r="E54" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.FALSOedit-cancel--2");</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
@@ -6759,6 +6958,10 @@
       <c r="D55" s="36" t="s">
         <v>65</v>
       </c>
+      <c r="E55" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.FALSOedit-submit--2");</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
@@ -6773,6 +6976,10 @@
       <c r="D56" s="37" t="s">
         <v>66</v>
       </c>
+      <c r="E56" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.FALSOedit-nequi-account");</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
@@ -6787,6 +6994,10 @@
       <c r="D57" s="37" t="s">
         <v>223</v>
       </c>
+      <c r="E57" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id="edit-terms--3"]/div/a");</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
@@ -6801,6 +7012,10 @@
       <c r="D58" s="37" t="s">
         <v>68</v>
       </c>
+      <c r="E58" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.FALSOtigoune-nequi-button-cancel");</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
@@ -6815,6 +7030,10 @@
       <c r="D59" s="37" t="s">
         <v>69</v>
       </c>
+      <c r="E59" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar=By.FALSOtigoune-nequi-button-submit");</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="33" t="s">
@@ -6829,8 +7048,9 @@
       <c r="D60" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="E60" s="39" t="s">
-        <v>151</v>
+      <c r="E60" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedePagorealizado=By.FALSOgateway-content-alert-message");</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -6846,6 +7066,10 @@
       <c r="D61" s="38" t="s">
         <v>170</v>
       </c>
+      <c r="E61" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="33" t="s">
@@ -6860,6 +7084,10 @@
       <c r="D62" s="38" t="s">
         <v>171</v>
       </c>
+      <c r="E62" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
@@ -6874,6 +7102,10 @@
       <c r="D63" s="38" t="s">
         <v>172</v>
       </c>
+      <c r="E63" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="33" t="s">
@@ -6888,8 +7120,12 @@
       <c r="D64" s="38" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
         <v>136</v>
       </c>
@@ -6902,8 +7138,12 @@
       <c r="D65" s="38" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text()");</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
         <v>136</v>
       </c>
@@ -6916,8 +7156,12 @@
       <c r="D66" s="38" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbCodigo=By.xpath("//*[@id='transaction-description-error']");</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
         <v>136</v>
       </c>
@@ -6930,8 +7174,12 @@
       <c r="D67" s="38" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="39" t="str">
+        <f t="shared" ref="E67:E77" si="1">CONCATENATE("public By ",B67,C67,"=By.",IF(ISNUMBER(SEARCH("@id=",D67)),"xpath("""),D67,""");")</f>
+        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div");</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="33" t="s">
         <v>136</v>
       </c>
@@ -6944,8 +7192,12 @@
       <c r="D68" s="38" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2]");</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
         <v>136</v>
       </c>
@@ -6958,8 +7210,12 @@
       <c r="D69" s="38" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2]");</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="33" t="s">
         <v>136</v>
       </c>
@@ -6972,8 +7228,12 @@
       <c r="D70" s="38" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2]");</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
         <v>136</v>
       </c>
@@ -6986,8 +7246,12 @@
       <c r="D71" s="38" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2]");</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
         <v>136</v>
       </c>
@@ -7000,8 +7264,12 @@
       <c r="D72" s="38" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a");</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
         <v>136</v>
       </c>
@@ -7014,8 +7282,12 @@
       <c r="D73" s="38" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button");</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
         <v>136</v>
       </c>
@@ -7028,8 +7300,12 @@
       <c r="D74" s="38" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnPAGAROTRAFACTURA=By.xpath("//*[@id='details-transaction']/div[5]/a[2]/button");</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="46" t="s">
         <v>209</v>
       </c>
@@ -7042,8 +7318,12 @@
       <c r="D75" s="56" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By txtE-mail=By.FALSOid="PNEMail"");</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="46" t="s">
         <v>209</v>
       </c>
@@ -7056,8 +7336,12 @@
       <c r="D76" s="56" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnIralBanco=By.FALSOid="btnSeguir"");</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="46" t="s">
         <v>209</v>
       </c>
@@ -7069,6 +7353,10 @@
       </c>
       <c r="D77" s="56" t="s">
         <v>216</v>
+      </c>
+      <c r="E77" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnRegresaralcomercio=By.FALSOid="btnCancel"");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de formula de objetos. Corrección comillas
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="302">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -878,6 +878,60 @@
   </si>
   <si>
     <t>Creación</t>
+  </si>
+  <si>
+    <t>//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[2]/p</t>
+  </si>
+  <si>
+    <t>//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p</t>
+  </si>
+  <si>
+    <t>id='edit-candidate-number'</t>
+  </si>
+  <si>
+    <t>id='edit-email'</t>
+  </si>
+  <si>
+    <t>//*[@id='tyc_Movil']</t>
+  </si>
+  <si>
+    <t>id='edit-consult'</t>
+  </si>
+  <si>
+    <t>id='edit-document-type'</t>
+  </si>
+  <si>
+    <t>id='edit-document'</t>
+  </si>
+  <si>
+    <t>//*[@id='content_right_forms_unified']/div/div/label</t>
+  </si>
+  <si>
+    <t>id='edit-consult--2'</t>
+  </si>
+  <si>
+    <t>//*[@id='edit-content-document--2']/div/p</t>
+  </si>
+  <si>
+    <t>//*[@id='edit-show-email--2']/div/p</t>
+  </si>
+  <si>
+    <t>//*[@id='edit-terms--2']/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='edit-terms--3']/div/a</t>
+  </si>
+  <si>
+    <t>id='PNEMail'</t>
+  </si>
+  <si>
+    <t>id='btnSeguir'</t>
+  </si>
+  <si>
+    <t>id='btnCancel'</t>
+  </si>
+  <si>
+    <t>id='tyc_Fijo'</t>
   </si>
 </sst>
 </file>
@@ -888,7 +942,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -922,6 +976,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1171,7 +1233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1493,6 +1555,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5972,8 +6040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5982,7 +6050,7 @@
     <col min="2" max="2" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="39" customWidth="1"/>
     <col min="4" max="4" width="61" style="39" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="39"/>
+    <col min="5" max="5" width="134.5703125" style="39" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="39"/>
   </cols>
@@ -6024,11 +6092,11 @@
         <v>267</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="39" t="str">
-        <f t="shared" ref="E3:E66" si="0">CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath("""),D3,""");")</f>
-        <v>public By btnMovil=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[1]/div/div/div[2]/p");</v>
+        <v>284</v>
+      </c>
+      <c r="E3" s="48" t="str">
+        <f t="shared" ref="E3:E66" si="0">CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,")"";")</f>
+        <v>public By btnMovil=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[2]/p)";</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -6042,11 +6110,11 @@
         <v>268</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="39" t="str">
+        <v>285</v>
+      </c>
+      <c r="E4" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnHogar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[1]/div/div/div[1]/p");</v>
+        <v>public By btnHogar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p)";</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -6060,11 +6128,11 @@
         <v>269</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" s="39" t="str">
+        <v>286</v>
+      </c>
+      <c r="E5" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtTuLineaTigo=By.FALSOid="edit-candidate-number"");</v>
+        <v>public By txtTuLineaTigo=By.id("id='edit-candidate-number')";</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -6078,11 +6146,11 @@
         <v>255</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="E6" s="39" t="str">
+        <v>287</v>
+      </c>
+      <c r="E6" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico=By.FALSOid="edit-email"");</v>
+        <v>public By txtCorreoElectronico=By.id("id='edit-email')";</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -6096,11 +6164,11 @@
         <v>274</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="E7" s="39" t="str">
+        <v>288</v>
+      </c>
+      <c r="E7" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosyCondiciones=By.xpath("//*[@id="tyc_Movil"]");</v>
+        <v>public By linkTerminosyCondiciones=By.xpath("//*[@id='tyc_Movil'])";</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -6114,11 +6182,11 @@
         <v>7</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="E8" s="39" t="str">
+        <v>289</v>
+      </c>
+      <c r="E8" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnConsultar=By.FALSOid="edit-consult"");</v>
+        <v>public By btnConsultar=By.id("id='edit-consult')";</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6131,10 +6199,10 @@
       <c r="C9" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="39" t="str">
+      <c r="D9" s="121"/>
+      <c r="E9" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By CapcharCaptchar=By.FALSO");</v>
+        <v>public By CapcharCaptchar=By.id(")";</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -6148,11 +6216,11 @@
         <v>267</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="39" t="str">
-        <f>CONCATENATE("public By ",B10,C10,"=By.",IF(ISNUMBER(SEARCH("@id=",D10)),"xpath("""),D10,""");")</f>
-        <v>public By btnMovil=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[1]/div/div/div[2]/p");</v>
+        <v>284</v>
+      </c>
+      <c r="E10" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnMovil=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[2]/p)";</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -6166,11 +6234,11 @@
         <v>268</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="E11" s="39" t="str">
+        <v>285</v>
+      </c>
+      <c r="E11" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnHogar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[1]/div/div/div[1]/p");</v>
+        <v>public By btnHogar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p)";</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -6184,11 +6252,11 @@
         <v>275</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>198</v>
-      </c>
-      <c r="E12" s="39" t="str">
+        <v>290</v>
+      </c>
+      <c r="E12" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipoDocumento=By.FALSOid="edit-document-type"");</v>
+        <v>public By listTipoDocumento=By.id("id='edit-document-type')";</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -6202,11 +6270,11 @@
         <v>276</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>201</v>
-      </c>
-      <c r="E13" s="39" t="str">
+        <v>291</v>
+      </c>
+      <c r="E13" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumeroDocumento=By.FALSOid="edit-document"");</v>
+        <v>public By txtNumeroDocumento=By.id("id='edit-document')";</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6220,11 +6288,11 @@
         <v>255</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>202</v>
-      </c>
-      <c r="E14" s="39" t="str">
+        <v>292</v>
+      </c>
+      <c r="E14" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico=By.xpath("//*[@id="content_right_forms_unified"]/div/div/label");</v>
+        <v>public By txtCorreoElectronico=By.xpath("//*[@id='content_right_forms_unified']/div/div/label)";</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6238,11 +6306,11 @@
         <v>274</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" s="39" t="str">
+        <v>301</v>
+      </c>
+      <c r="E15" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosyCondiciones=By.xpath("//*[@id="tyc_Fijo"]");</v>
+        <v>public By linkTerminosyCondiciones=By.id("id='tyc_Fijo')";</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -6256,11 +6324,11 @@
         <v>7</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>203</v>
-      </c>
-      <c r="E16" s="39" t="str">
+        <v>293</v>
+      </c>
+      <c r="E16" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnConsultar=By.FALSOid="edit-consult--2"");</v>
+        <v>public By btnConsultar=By.id("id='edit-consult--2')";</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6274,9 +6342,9 @@
         <v>229</v>
       </c>
       <c r="D17" s="51"/>
-      <c r="E17" s="39" t="str">
+      <c r="E17" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By CapcharCaptchar=By.FALSO");</v>
+        <v>public By CapcharCaptchar=By.id(")";</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -6292,9 +6360,9 @@
       <c r="D18" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="E18" s="39" t="str">
+      <c r="E18" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodeLinea=By.xpath("//*[@id='value']");</v>
+        <v>public By txtNumerodeLinea=By.xpath("//*[@id='value'])";</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -6310,9 +6378,9 @@
       <c r="D19" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="E19" s="39" t="str">
+      <c r="E19" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtFechaLimitePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[1]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By txtFechaLimitePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[1]/div/table/tbody/tr[2]/td/div)";</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -6328,9 +6396,9 @@
       <c r="D20" s="53" t="s">
         <v>162</v>
       </c>
-      <c r="E20" s="39" t="str">
+      <c r="E20" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtReferentePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By txtReferentePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[2]/div/table/tbody/tr[2]/td/div)";</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -6346,9 +6414,9 @@
       <c r="D21" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="E21" s="39" t="str">
+      <c r="E21" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtPeriodoFacturacion=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By txtPeriodoFacturacion=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[3]/div/table/tbody/tr[2]/td/div)";</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -6364,9 +6432,9 @@
       <c r="D22" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="E22" s="39" t="str">
+      <c r="E22" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtValorPagar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[4]/div[2]");</v>
+        <v>public By txtValorPagar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[4]/div[2])";</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -6382,9 +6450,9 @@
       <c r="D23" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="39" t="str">
+      <c r="E23" s="34" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTarjetaCredito=By.FALSOpayment-method-type-label-credit-payu");</v>
+        <v>public By linkTarjetaCredito=By.id("payment-method-type-label-credit-payu)";</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -6400,9 +6468,9 @@
       <c r="D24" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="39" t="str">
+      <c r="E24" s="34" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkDebitoBancarioPSE=By.FALSOpayment-method-type-label-debit-payu");</v>
+        <v>public By linkDebitoBancarioPSE=By.id("payment-method-type-label-debit-payu)";</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -6418,9 +6486,9 @@
       <c r="D25" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="39" t="str">
+      <c r="E25" s="34" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkOtrosmediosdepago=By.FALSOpayment-method-type-label-others-pay-methods");</v>
+        <v>public By linkOtrosmediosdepago=By.id("payment-method-type-label-others-pay-methods)";</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -6436,9 +6504,9 @@
       <c r="D26" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="39" t="str">
+      <c r="E26" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodetarjeta=By.FALSOedit-cardnumber");</v>
+        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber)";</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -6454,9 +6522,9 @@
       <c r="D27" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="E27" s="39" t="str">
+      <c r="E27" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p)";</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -6472,9 +6540,9 @@
       <c r="D28" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="E28" s="39" t="str">
+      <c r="E28" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p)";</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -6490,9 +6558,9 @@
       <c r="D29" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="39" t="str">
+      <c r="E29" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCVV/CVC=By.FALSOedit-cvc");</v>
+        <v>public By txtCVV/CVC=By.id("edit-cvc)";</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -6508,9 +6576,9 @@
       <c r="D30" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="39" t="str">
+      <c r="E30" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listFechaVencimiento-MM=By.FALSOedit-buyer-card-month-expiration");</v>
+        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration)";</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -6526,9 +6594,9 @@
       <c r="D31" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="39" t="str">
+      <c r="E31" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listFechaVencimiento-AA=By.FALSOedit-buyer-card-year-expiration");</v>
+        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration)";</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -6544,9 +6612,9 @@
       <c r="D32" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="39" t="str">
+      <c r="E32" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listCuotas=By.FALSOedit-cardnumber-quota");</v>
+        <v>public By listCuotas=By.id("edit-cardnumber-quota)";</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -6562,9 +6630,9 @@
       <c r="D33" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="39" t="str">
+      <c r="E33" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNombre=By.FALSOedit-ccname");</v>
+        <v>public By txtNombre=By.id("edit-ccname)";</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -6580,9 +6648,9 @@
       <c r="D34" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="39" t="str">
+      <c r="E34" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipo=By.FALSOedit-buyer-document-type");</v>
+        <v>public By listTipo=By.id("edit-buyer-document-type)";</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -6598,9 +6666,9 @@
       <c r="D35" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="39" t="str">
+      <c r="E35" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodedocumento=By.FALSOedit-buyer-document");</v>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document)";</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -6616,9 +6684,9 @@
       <c r="D36" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="E36" s="39" t="str">
+      <c r="E36" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p)";</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -6634,9 +6702,9 @@
       <c r="D37" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="39" t="str">
+      <c r="E37" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.FALSOedit-buyer-phone");</v>
+        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone)";</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -6652,9 +6720,9 @@
       <c r="D38" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="39" t="str">
+      <c r="E38" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
+        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p)";</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -6670,9 +6738,9 @@
       <c r="D39" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="39" t="str">
+      <c r="E39" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico=By.FALSOedit-buyer-mail");</v>
+        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail)";</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -6688,9 +6756,9 @@
       <c r="D40" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="E40" s="39" t="str">
+      <c r="E40" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p)";</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -6706,9 +6774,9 @@
       <c r="D41" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="39" t="str">
+      <c r="E41" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.FALSOedit-buyer-check-authorize");</v>
+        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize)";</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -6724,9 +6792,9 @@
       <c r="D42" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="E42" s="39" t="str">
+      <c r="E42" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a)";</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -6742,9 +6810,9 @@
       <c r="D43" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="E43" s="39" t="str">
+      <c r="E43" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.FALSOedit-cancel");</v>
+        <v>public By btnCancelar=By.id("edit-cancel)";</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -6760,9 +6828,9 @@
       <c r="D44" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="E44" s="39" t="str">
+      <c r="E44" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.FALSOedit-submit");</v>
+        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit)";</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -6778,9 +6846,9 @@
       <c r="D45" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E45" s="39" t="str">
+      <c r="E45" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By listBanco=By.FALSOedit-bank");</v>
+        <v>public By listBanco=By.id("edit-bank)";</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -6796,9 +6864,9 @@
       <c r="D46" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="39" t="str">
+      <c r="E46" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipodepersona=By.FALSOedit-buyer-type-person");</v>
+        <v>public By listTipodepersona=By.id("edit-buyer-type-person)";</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -6814,9 +6882,9 @@
       <c r="D47" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="39" t="str">
+      <c r="E47" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNombresyapellidos=By.FALSOedit-buyer-name");</v>
+        <v>public By txtNombresyapellidos=By.id("edit-buyer-name)";</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -6832,9 +6900,9 @@
       <c r="D48" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E48" s="39" t="str">
+      <c r="E48" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipo=By.FALSOedit-buyer-document-type--2");</v>
+        <v>public By listTipo=By.id("edit-buyer-document-type--2)";</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -6850,9 +6918,9 @@
       <c r="D49" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E49" s="39" t="str">
+      <c r="E49" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodedocumento=By.FALSOedit-buyer-document--2");</v>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2)";</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -6866,11 +6934,11 @@
         <v>264</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>206</v>
-      </c>
-      <c r="E50" s="39" t="str">
+        <v>294</v>
+      </c>
+      <c r="E50" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id="edit-content-document--2"]/div/p");</v>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p)";</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -6886,9 +6954,9 @@
       <c r="D51" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="39" t="str">
+      <c r="E51" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.FALSOedit-buyer-mail--2");</v>
+        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2)";</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -6902,11 +6970,11 @@
         <v>256</v>
       </c>
       <c r="D52" s="36" t="s">
-        <v>207</v>
-      </c>
-      <c r="E52" s="39" t="str">
+        <v>295</v>
+      </c>
+      <c r="E52" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id="edit-show-email--2"]/div/p");</v>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p)";</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -6920,11 +6988,11 @@
         <v>270</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>208</v>
-      </c>
-      <c r="E53" s="39" t="str">
+        <v>296</v>
+      </c>
+      <c r="E53" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id="edit-terms--2"]/div/a");</v>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a)";</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -6940,9 +7008,9 @@
       <c r="D54" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E54" s="39" t="str">
+      <c r="E54" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.FALSOedit-cancel--2");</v>
+        <v>public By btnCancelar=By.id("edit-cancel--2)";</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -6958,9 +7026,9 @@
       <c r="D55" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="E55" s="39" t="str">
+      <c r="E55" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.FALSOedit-submit--2");</v>
+        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2)";</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -6976,9 +7044,9 @@
       <c r="D56" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E56" s="39" t="str">
+      <c r="E56" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.FALSOedit-nequi-account");</v>
+        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.id("edit-nequi-account)";</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -6992,11 +7060,11 @@
         <v>270</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="E57" s="39" t="str">
+        <v>297</v>
+      </c>
+      <c r="E57" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id="edit-terms--3"]/div/a");</v>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--3']/div/a)";</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -7012,9 +7080,9 @@
       <c r="D58" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E58" s="39" t="str">
+      <c r="E58" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.FALSOtigoune-nequi-button-cancel");</v>
+        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel)";</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -7030,9 +7098,9 @@
       <c r="D59" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E59" s="39" t="str">
+      <c r="E59" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnPagar=By.FALSOtigoune-nequi-button-submit");</v>
+        <v>public By btnPagar=By.id("tigoune-nequi-button-submit)";</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -7048,9 +7116,9 @@
       <c r="D60" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="E60" s="39" t="str">
+      <c r="E60" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedePagorealizado=By.FALSOgateway-content-alert-message");</v>
+        <v>public By lbMensajedePagorealizado=By.id("gateway-content-alert-message)";</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -7066,9 +7134,9 @@
       <c r="D61" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="E61" s="39" t="str">
+      <c r="E61" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div)";</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -7084,9 +7152,9 @@
       <c r="D62" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="E62" s="39" t="str">
+      <c r="E62" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div)";</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -7102,9 +7170,9 @@
       <c r="D63" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="E63" s="39" t="str">
+      <c r="E63" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div)";</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -7120,9 +7188,9 @@
       <c r="D64" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="E64" s="39" t="str">
+      <c r="E64" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div)";</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -7138,9 +7206,9 @@
       <c r="D65" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="E65" s="39" t="str">
+      <c r="E65" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text()");</v>
+        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text())";</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -7156,9 +7224,9 @@
       <c r="D66" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="E66" s="39" t="str">
+      <c r="E66" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbCodigo=By.xpath("//*[@id='transaction-description-error']");</v>
+        <v>public By lbCodigo=By.xpath("//*[@id='transaction-description-error'])";</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -7174,9 +7242,9 @@
       <c r="D67" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="E67" s="39" t="str">
-        <f t="shared" ref="E67:E77" si="1">CONCATENATE("public By ",B67,C67,"=By.",IF(ISNUMBER(SEARCH("@id=",D67)),"xpath("""),D67,""");")</f>
-        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div");</v>
+      <c r="E67" s="38" t="str">
+        <f t="shared" ref="E67:E77" si="1">CONCATENATE("public By ",B67,C67,"=By.",IF(ISNUMBER(SEARCH("@id=",D67)),"xpath(""","id("""),D67,")"";")</f>
+        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div)";</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -7192,9 +7260,9 @@
       <c r="D68" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="E68" s="39" t="str">
+      <c r="E68" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2]");</v>
+        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2])";</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -7210,9 +7278,9 @@
       <c r="D69" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="E69" s="39" t="str">
+      <c r="E69" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2]");</v>
+        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2])";</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -7228,9 +7296,9 @@
       <c r="D70" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="E70" s="39" t="str">
+      <c r="E70" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2]");</v>
+        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2])";</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -7246,9 +7314,9 @@
       <c r="D71" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="E71" s="39" t="str">
+      <c r="E71" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2]");</v>
+        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2])";</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -7264,9 +7332,9 @@
       <c r="D72" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="E72" s="39" t="str">
+      <c r="E72" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a");</v>
+        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a)";</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -7282,9 +7350,9 @@
       <c r="D73" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="E73" s="39" t="str">
+      <c r="E73" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button");</v>
+        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button)";</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -7300,9 +7368,9 @@
       <c r="D74" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="E74" s="39" t="str">
+      <c r="E74" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnPAGAROTRAFACTURA=By.xpath("//*[@id='details-transaction']/div[5]/a[2]/button");</v>
+        <v>public By btnPAGAROTRAFACTURA=By.xpath("//*[@id='details-transaction']/div[5]/a[2]/button)";</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -7316,11 +7384,11 @@
         <v>211</v>
       </c>
       <c r="D75" s="56" t="s">
-        <v>212</v>
-      </c>
-      <c r="E75" s="39" t="str">
+        <v>298</v>
+      </c>
+      <c r="E75" s="56" t="str">
         <f t="shared" si="1"/>
-        <v>public By txtE-mail=By.FALSOid="PNEMail"");</v>
+        <v>public By txtE-mail=By.id("id='PNEMail')";</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -7334,11 +7402,11 @@
         <v>253</v>
       </c>
       <c r="D76" s="56" t="s">
-        <v>214</v>
-      </c>
-      <c r="E76" s="39" t="str">
+        <v>299</v>
+      </c>
+      <c r="E76" s="56" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnIralBanco=By.FALSOid="btnSeguir"");</v>
+        <v>public By btnIralBanco=By.id("id='btnSeguir')";</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -7352,15 +7420,16 @@
         <v>254</v>
       </c>
       <c r="D77" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="E77" s="39" t="str">
+        <v>300</v>
+      </c>
+      <c r="E77" s="56" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnRegresaralcomercio=By.FALSOid="btnCancel"");</v>
+        <v>public By btnRegresaralcomercio=By.id("id='btnCancel')";</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D74"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel - Se realizan ajustes a los identificadores de los objetos de las paginas
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="301">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -886,30 +886,9 @@
     <t>//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p</t>
   </si>
   <si>
-    <t>id='edit-candidate-number'</t>
-  </si>
-  <si>
-    <t>id='edit-email'</t>
-  </si>
-  <si>
-    <t>//*[@id='tyc_Movil']</t>
-  </si>
-  <si>
-    <t>id='edit-consult'</t>
-  </si>
-  <si>
-    <t>id='edit-document-type'</t>
-  </si>
-  <si>
-    <t>id='edit-document'</t>
-  </si>
-  <si>
     <t>//*[@id='content_right_forms_unified']/div/div/label</t>
   </si>
   <si>
-    <t>id='edit-consult--2'</t>
-  </si>
-  <si>
     <t>//*[@id='edit-content-document--2']/div/p</t>
   </si>
   <si>
@@ -922,16 +901,34 @@
     <t>//*[@id='edit-terms--3']/div/a</t>
   </si>
   <si>
-    <t>id='PNEMail'</t>
-  </si>
-  <si>
-    <t>id='btnSeguir'</t>
-  </si>
-  <si>
-    <t>id='btnCancel'</t>
-  </si>
-  <si>
-    <t>id='tyc_Fijo'</t>
+    <t>edit-consult--2</t>
+  </si>
+  <si>
+    <t>tyc_Fijo</t>
+  </si>
+  <si>
+    <t>edit-document</t>
+  </si>
+  <si>
+    <t>edit-document-type</t>
+  </si>
+  <si>
+    <t>edit-consult</t>
+  </si>
+  <si>
+    <t>tyc_Movil</t>
+  </si>
+  <si>
+    <t>btnSeguir</t>
+  </si>
+  <si>
+    <t>btnCancel</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>transaction-description-error</t>
   </si>
 </sst>
 </file>
@@ -942,7 +939,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -976,14 +973,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1233,7 +1222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1469,6 +1458,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1555,12 +1547,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2151,78 +2137,78 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="92" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="91"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="91"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="92"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="91"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="91"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="91"/>
-      <c r="B18" s="91"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="91"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="91"/>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="91"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91"/>
+      <c r="A21" s="92"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="92"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="91"/>
-      <c r="B22" s="91"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2255,17 +2241,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -4511,14 +4497,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4541,7 +4527,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="106" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4561,7 +4547,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="106"/>
+      <c r="A4" s="107"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -4579,7 +4565,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -4597,7 +4583,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="3" t="s">
         <v>101</v>
       </c>
@@ -4615,7 +4601,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
@@ -4636,7 +4622,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="106"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
@@ -4657,7 +4643,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
+      <c r="A9" s="108"/>
       <c r="B9" s="3" t="s">
         <v>229</v>
       </c>
@@ -4675,7 +4661,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="114" t="s">
+      <c r="A10" s="115" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -4695,7 +4681,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="115"/>
+      <c r="A11" s="116"/>
       <c r="B11" s="7" t="s">
         <v>124</v>
       </c>
@@ -4716,7 +4702,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="115"/>
+      <c r="A12" s="116"/>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -4734,7 +4720,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="115"/>
+      <c r="A13" s="116"/>
       <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
@@ -4755,7 +4741,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="115"/>
+      <c r="A14" s="116"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -4773,7 +4759,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="115"/>
+      <c r="A15" s="116"/>
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -4791,7 +4777,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="115"/>
+      <c r="A16" s="116"/>
       <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
@@ -4809,7 +4795,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="115"/>
+      <c r="A17" s="116"/>
       <c r="B17" s="7" t="s">
         <v>101</v>
       </c>
@@ -4827,7 +4813,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="115"/>
+      <c r="A18" s="116"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -4845,7 +4831,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="116"/>
+      <c r="A19" s="117"/>
       <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
@@ -4863,7 +4849,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="99" t="s">
+      <c r="A20" s="100" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -4883,7 +4869,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="100"/>
+      <c r="A21" s="101"/>
       <c r="B21" s="4" t="s">
         <v>81</v>
       </c>
@@ -4908,7 +4894,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="100"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
@@ -4926,7 +4912,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="100"/>
+      <c r="A23" s="101"/>
       <c r="B23" s="4" t="s">
         <v>82</v>
       </c>
@@ -4944,7 +4930,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="101"/>
+      <c r="A24" s="102"/>
       <c r="B24" s="4" t="s">
         <v>83</v>
       </c>
@@ -4969,7 +4955,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="102" t="s">
+      <c r="A25" s="103" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -4989,7 +4975,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="103"/>
+      <c r="A26" s="104"/>
       <c r="B26" s="13" t="s">
         <v>27</v>
       </c>
@@ -5007,7 +4993,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="104"/>
+      <c r="A27" s="105"/>
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -5025,7 +5011,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="117" t="s">
+      <c r="A28" s="118" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5045,7 +5031,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="118"/>
+      <c r="A29" s="119"/>
       <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
@@ -5066,7 +5052,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="118"/>
+      <c r="A30" s="119"/>
       <c r="B30" s="15" t="s">
         <v>118</v>
       </c>
@@ -5087,7 +5073,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="118"/>
+      <c r="A31" s="119"/>
       <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
@@ -5105,7 +5091,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="118"/>
+      <c r="A32" s="119"/>
       <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
@@ -5123,7 +5109,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="118"/>
+      <c r="A33" s="119"/>
       <c r="B33" s="15" t="s">
         <v>35</v>
       </c>
@@ -5141,7 +5127,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="118"/>
+      <c r="A34" s="119"/>
       <c r="B34" s="15" t="s">
         <v>36</v>
       </c>
@@ -5159,7 +5145,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="118"/>
+      <c r="A35" s="119"/>
       <c r="B35" s="15" t="s">
         <v>39</v>
       </c>
@@ -5177,7 +5163,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="118"/>
+      <c r="A36" s="119"/>
       <c r="B36" s="15" t="s">
         <v>3</v>
       </c>
@@ -5195,7 +5181,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="118"/>
+      <c r="A37" s="119"/>
       <c r="B37" s="15" t="s">
         <v>42</v>
       </c>
@@ -5213,7 +5199,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="118"/>
+      <c r="A38" s="119"/>
       <c r="B38" s="15" t="s">
         <v>122</v>
       </c>
@@ -5234,7 +5220,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="118"/>
+      <c r="A39" s="119"/>
       <c r="B39" s="15" t="s">
         <v>44</v>
       </c>
@@ -5252,7 +5238,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="118"/>
+      <c r="A40" s="119"/>
       <c r="B40" s="15" t="s">
         <v>130</v>
       </c>
@@ -5273,7 +5259,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="118"/>
+      <c r="A41" s="119"/>
       <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
@@ -5291,7 +5277,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="118"/>
+      <c r="A42" s="119"/>
       <c r="B42" s="15" t="s">
         <v>110</v>
       </c>
@@ -5312,7 +5298,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="118"/>
+      <c r="A43" s="119"/>
       <c r="B43" s="15" t="s">
         <v>47</v>
       </c>
@@ -5328,7 +5314,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="118"/>
+      <c r="A44" s="119"/>
       <c r="B44" s="15" t="s">
         <v>101</v>
       </c>
@@ -5344,7 +5330,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="118"/>
+      <c r="A45" s="119"/>
       <c r="B45" s="15" t="s">
         <v>22</v>
       </c>
@@ -5362,7 +5348,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="119"/>
+      <c r="A46" s="120"/>
       <c r="B46" s="15" t="s">
         <v>51</v>
       </c>
@@ -5380,7 +5366,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="108" t="s">
+      <c r="A47" s="109" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -5400,7 +5386,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="109"/>
+      <c r="A48" s="110"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -5418,7 +5404,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="109"/>
+      <c r="A49" s="110"/>
       <c r="B49" s="5" t="s">
         <v>56</v>
       </c>
@@ -5436,7 +5422,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="109"/>
+      <c r="A50" s="110"/>
       <c r="B50" s="5" t="s">
         <v>3</v>
       </c>
@@ -5454,7 +5440,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="109"/>
+      <c r="A51" s="110"/>
       <c r="B51" s="5" t="s">
         <v>60</v>
       </c>
@@ -5472,7 +5458,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="109"/>
+      <c r="A52" s="110"/>
       <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
@@ -5490,7 +5476,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="109"/>
+      <c r="A53" s="110"/>
       <c r="B53" s="5" t="s">
         <v>101</v>
       </c>
@@ -5506,7 +5492,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="109"/>
+      <c r="A54" s="110"/>
       <c r="B54" s="5" t="s">
         <v>22</v>
       </c>
@@ -5524,7 +5510,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="110"/>
+      <c r="A55" s="111"/>
       <c r="B55" s="5" t="s">
         <v>64</v>
       </c>
@@ -5542,7 +5528,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="111" t="s">
+      <c r="A56" s="112" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -5562,7 +5548,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="112"/>
+      <c r="A57" s="113"/>
       <c r="B57" s="1" t="s">
         <v>101</v>
       </c>
@@ -5578,7 +5564,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="112"/>
+      <c r="A58" s="113"/>
       <c r="B58" s="1" t="s">
         <v>22</v>
       </c>
@@ -5596,7 +5582,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="113"/>
+      <c r="A59" s="114"/>
       <c r="B59" s="1" t="s">
         <v>48</v>
       </c>
@@ -5614,7 +5600,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="94" t="s">
+      <c r="A60" s="95" t="s">
         <v>136</v>
       </c>
       <c r="B60" s="23" t="s">
@@ -5637,7 +5623,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="95"/>
+      <c r="A61" s="96"/>
       <c r="B61" s="23" t="s">
         <v>137</v>
       </c>
@@ -5655,7 +5641,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="95"/>
+      <c r="A62" s="96"/>
       <c r="B62" s="23" t="s">
         <v>138</v>
       </c>
@@ -5673,7 +5659,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="95"/>
+      <c r="A63" s="96"/>
       <c r="B63" s="23" t="s">
         <v>139</v>
       </c>
@@ -5691,7 +5677,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="95"/>
+      <c r="A64" s="96"/>
       <c r="B64" s="23" t="s">
         <v>140</v>
       </c>
@@ -5709,7 +5695,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="95"/>
+      <c r="A65" s="96"/>
       <c r="B65" s="23" t="s">
         <v>141</v>
       </c>
@@ -5727,7 +5713,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="95"/>
+      <c r="A66" s="96"/>
       <c r="B66" s="23" t="s">
         <v>142</v>
       </c>
@@ -5745,7 +5731,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="95"/>
+      <c r="A67" s="96"/>
       <c r="B67" s="23" t="s">
         <v>143</v>
       </c>
@@ -5763,7 +5749,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="95"/>
+      <c r="A68" s="96"/>
       <c r="B68" s="23" t="s">
         <v>144</v>
       </c>
@@ -5781,7 +5767,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="95"/>
+      <c r="A69" s="96"/>
       <c r="B69" s="23" t="s">
         <v>145</v>
       </c>
@@ -5799,7 +5785,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="95"/>
+      <c r="A70" s="96"/>
       <c r="B70" s="23" t="s">
         <v>146</v>
       </c>
@@ -5817,7 +5803,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="95"/>
+      <c r="A71" s="96"/>
       <c r="B71" s="23" t="s">
         <v>147</v>
       </c>
@@ -5835,7 +5821,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="95"/>
+      <c r="A72" s="96"/>
       <c r="B72" s="23" t="s">
         <v>148</v>
       </c>
@@ -5853,7 +5839,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="95"/>
+      <c r="A73" s="96"/>
       <c r="B73" s="23" t="s">
         <v>149</v>
       </c>
@@ -5871,7 +5857,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="96"/>
+      <c r="A74" s="97"/>
       <c r="B74" s="23" t="s">
         <v>150</v>
       </c>
@@ -6040,8 +6026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6049,8 +6035,7 @@
     <col min="1" max="1" width="32.42578125" style="39" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="39" customWidth="1"/>
-    <col min="4" max="4" width="61" style="39" customWidth="1"/>
-    <col min="5" max="5" width="134.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="61" style="39" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="39"/>
   </cols>
@@ -6095,8 +6080,8 @@
         <v>284</v>
       </c>
       <c r="E3" s="48" t="str">
-        <f t="shared" ref="E3:E66" si="0">CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,")"";")</f>
-        <v>public By btnMovil=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[2]/p)";</v>
+        <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
+        <v>public By btnMovil=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[2]/p");</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -6113,8 +6098,8 @@
         <v>285</v>
       </c>
       <c r="E4" s="48" t="str">
-        <f t="shared" si="0"/>
-        <v>public By btnHogar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p)";</v>
+        <f t="shared" ref="E4:E67" si="0">CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
+        <v>public By btnHogar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p");</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -6128,11 +6113,11 @@
         <v>269</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>286</v>
+        <v>9</v>
       </c>
       <c r="E5" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtTuLineaTigo=By.id("id='edit-candidate-number')";</v>
+        <v>public By txtTuLineaTigo=By.id("edit-candidate-number");</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -6146,11 +6131,11 @@
         <v>255</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="E6" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico=By.id("id='edit-email')";</v>
+        <v>public By txtCorreoElectronico=By.id("edit-email");</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -6164,11 +6149,11 @@
         <v>274</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="E7" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosyCondiciones=By.xpath("//*[@id='tyc_Movil'])";</v>
+        <v>public By linkTerminosyCondiciones=By.id("tyc_Movil");</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -6182,11 +6167,11 @@
         <v>7</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="E8" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnConsultar=By.id("id='edit-consult')";</v>
+        <v>public By btnConsultar=By.id("edit-consult");</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6199,10 +6184,10 @@
       <c r="C9" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="D9" s="121"/>
-      <c r="E9" s="48" t="str">
+      <c r="D9" s="91"/>
+      <c r="E9" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>public By CapcharCaptchar=By.id(")";</v>
+        <v>public By CapcharCaptchar=By.id("");</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -6220,7 +6205,7 @@
       </c>
       <c r="E10" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnMovil=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[2]/p)";</v>
+        <v>public By btnMovil=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[2]/p");</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -6238,7 +6223,7 @@
       </c>
       <c r="E11" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnHogar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p)";</v>
+        <v>public By btnHogar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p");</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -6252,11 +6237,11 @@
         <v>275</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E12" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipoDocumento=By.id("id='edit-document-type')";</v>
+        <v>public By listTipoDocumento=By.id("edit-document-type");</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -6270,11 +6255,11 @@
         <v>276</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E13" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumeroDocumento=By.id("id='edit-document')";</v>
+        <v>public By txtNumeroDocumento=By.id("edit-document");</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6288,11 +6273,11 @@
         <v>255</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E14" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico=By.xpath("//*[@id='content_right_forms_unified']/div/div/label)";</v>
+        <v>public By txtCorreoElectronico=By.xpath("//*[@id='content_right_forms_unified']/div/div/label");</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6306,11 +6291,11 @@
         <v>274</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="E15" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosyCondiciones=By.id("id='tyc_Fijo')";</v>
+        <v>public By linkTerminosyCondiciones=By.id("tyc_Fijo");</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -6324,11 +6309,11 @@
         <v>7</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E16" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnConsultar=By.id("id='edit-consult--2')";</v>
+        <v>public By btnConsultar=By.id("edit-consult--2");</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6344,7 +6329,7 @@
       <c r="D17" s="51"/>
       <c r="E17" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By CapcharCaptchar=By.id(")";</v>
+        <v>public By CapcharCaptchar=By.id("");</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -6358,11 +6343,11 @@
         <v>262</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>160</v>
+        <v>299</v>
       </c>
       <c r="E18" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodeLinea=By.xpath("//*[@id='value'])";</v>
+        <v>public By txtNumerodeLinea=By.id("value");</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -6380,7 +6365,7 @@
       </c>
       <c r="E19" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtFechaLimitePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[1]/div/table/tbody/tr[2]/td/div)";</v>
+        <v>public By txtFechaLimitePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[1]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -6398,7 +6383,7 @@
       </c>
       <c r="E20" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtReferentePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[2]/div/table/tbody/tr[2]/td/div)";</v>
+        <v>public By txtReferentePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[2]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -6416,7 +6401,7 @@
       </c>
       <c r="E21" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtPeriodoFacturacion=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[3]/div/table/tbody/tr[2]/td/div)";</v>
+        <v>public By txtPeriodoFacturacion=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[3]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -6434,7 +6419,7 @@
       </c>
       <c r="E22" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtValorPagar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[4]/div[2])";</v>
+        <v>public By txtValorPagar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[4]/div[2]");</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -6452,7 +6437,7 @@
       </c>
       <c r="E23" s="34" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTarjetaCredito=By.id("payment-method-type-label-credit-payu)";</v>
+        <v>public By linkTarjetaCredito=By.id("payment-method-type-label-credit-payu");</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -6470,7 +6455,7 @@
       </c>
       <c r="E24" s="34" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkDebitoBancarioPSE=By.id("payment-method-type-label-debit-payu)";</v>
+        <v>public By linkDebitoBancarioPSE=By.id("payment-method-type-label-debit-payu");</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -6488,7 +6473,7 @@
       </c>
       <c r="E25" s="34" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkOtrosmediosdepago=By.id("payment-method-type-label-others-pay-methods)";</v>
+        <v>public By linkOtrosmediosdepago=By.id("payment-method-type-label-others-pay-methods");</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -6504,9 +6489,9 @@
       <c r="D26" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="120" t="str">
+      <c r="E26" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber)";</v>
+        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber");</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -6522,9 +6507,9 @@
       <c r="D27" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="E27" s="120" t="str">
+      <c r="E27" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p)";</v>
+        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -6542,7 +6527,7 @@
       </c>
       <c r="E28" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p)";</v>
+        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -6560,7 +6545,7 @@
       </c>
       <c r="E29" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCVV/CVC=By.id("edit-cvc)";</v>
+        <v>public By txtCVV/CVC=By.id("edit-cvc");</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -6578,7 +6563,7 @@
       </c>
       <c r="E30" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration)";</v>
+        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration");</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -6596,7 +6581,7 @@
       </c>
       <c r="E31" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration)";</v>
+        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration");</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -6614,7 +6599,7 @@
       </c>
       <c r="E32" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listCuotas=By.id("edit-cardnumber-quota)";</v>
+        <v>public By listCuotas=By.id("edit-cardnumber-quota");</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -6632,7 +6617,7 @@
       </c>
       <c r="E33" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNombre=By.id("edit-ccname)";</v>
+        <v>public By txtNombre=By.id("edit-ccname");</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -6650,7 +6635,7 @@
       </c>
       <c r="E34" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipo=By.id("edit-buyer-document-type)";</v>
+        <v>public By listTipo=By.id("edit-buyer-document-type");</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -6668,7 +6653,7 @@
       </c>
       <c r="E35" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodedocumento=By.id("edit-buyer-document)";</v>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document");</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -6686,7 +6671,7 @@
       </c>
       <c r="E36" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p)";</v>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -6704,7 +6689,7 @@
       </c>
       <c r="E37" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone)";</v>
+        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone");</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -6722,7 +6707,7 @@
       </c>
       <c r="E38" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p)";</v>
+        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -6740,7 +6725,7 @@
       </c>
       <c r="E39" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail)";</v>
+        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail");</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -6758,7 +6743,7 @@
       </c>
       <c r="E40" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p)";</v>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -6776,7 +6761,7 @@
       </c>
       <c r="E41" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize)";</v>
+        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize");</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -6794,7 +6779,7 @@
       </c>
       <c r="E42" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a)";</v>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -6812,7 +6797,7 @@
       </c>
       <c r="E43" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.id("edit-cancel)";</v>
+        <v>public By btnCancelar=By.id("edit-cancel");</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -6830,7 +6815,7 @@
       </c>
       <c r="E44" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit)";</v>
+        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit");</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -6848,7 +6833,7 @@
       </c>
       <c r="E45" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By listBanco=By.id("edit-bank)";</v>
+        <v>public By listBanco=By.id("edit-bank");</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -6866,7 +6851,7 @@
       </c>
       <c r="E46" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipodepersona=By.id("edit-buyer-type-person)";</v>
+        <v>public By listTipodepersona=By.id("edit-buyer-type-person");</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -6884,7 +6869,7 @@
       </c>
       <c r="E47" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNombresyapellidos=By.id("edit-buyer-name)";</v>
+        <v>public By txtNombresyapellidos=By.id("edit-buyer-name");</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -6902,7 +6887,7 @@
       </c>
       <c r="E48" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipo=By.id("edit-buyer-document-type--2)";</v>
+        <v>public By listTipo=By.id("edit-buyer-document-type--2");</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -6920,7 +6905,7 @@
       </c>
       <c r="E49" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2)";</v>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2");</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -6934,11 +6919,11 @@
         <v>264</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E50" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p)";</v>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p");</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -6956,7 +6941,7 @@
       </c>
       <c r="E51" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2)";</v>
+        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2");</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -6970,11 +6955,11 @@
         <v>256</v>
       </c>
       <c r="D52" s="36" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E52" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p)";</v>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p");</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -6988,11 +6973,11 @@
         <v>270</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E53" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a)";</v>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a");</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -7010,7 +6995,7 @@
       </c>
       <c r="E54" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.id("edit-cancel--2)";</v>
+        <v>public By btnCancelar=By.id("edit-cancel--2");</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -7028,7 +7013,7 @@
       </c>
       <c r="E55" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2)";</v>
+        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2");</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -7046,7 +7031,7 @@
       </c>
       <c r="E56" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.id("edit-nequi-account)";</v>
+        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.id("edit-nequi-account");</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -7060,11 +7045,11 @@
         <v>270</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E57" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--3']/div/a)";</v>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--3']/div/a");</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -7082,7 +7067,7 @@
       </c>
       <c r="E58" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel)";</v>
+        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel");</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -7100,7 +7085,7 @@
       </c>
       <c r="E59" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnPagar=By.id("tigoune-nequi-button-submit)";</v>
+        <v>public By btnPagar=By.id("tigoune-nequi-button-submit");</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -7118,7 +7103,7 @@
       </c>
       <c r="E60" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedePagorealizado=By.id("gateway-content-alert-message)";</v>
+        <v>public By lbMensajedePagorealizado=By.id("gateway-content-alert-message");</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -7136,7 +7121,7 @@
       </c>
       <c r="E61" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div)";</v>
+        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -7154,7 +7139,7 @@
       </c>
       <c r="E62" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div)";</v>
+        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -7172,7 +7157,7 @@
       </c>
       <c r="E63" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div)";</v>
+        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -7190,7 +7175,7 @@
       </c>
       <c r="E64" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div)";</v>
+        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -7208,7 +7193,7 @@
       </c>
       <c r="E65" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text())";</v>
+        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text()");</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -7222,11 +7207,11 @@
         <v>259</v>
       </c>
       <c r="D66" s="38" t="s">
-        <v>175</v>
+        <v>300</v>
       </c>
       <c r="E66" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbCodigo=By.xpath("//*[@id='transaction-description-error'])";</v>
+        <v>public By lbCodigo=By.id("transaction-description-error");</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -7243,8 +7228,8 @@
         <v>176</v>
       </c>
       <c r="E67" s="38" t="str">
-        <f t="shared" ref="E67:E77" si="1">CONCATENATE("public By ",B67,C67,"=By.",IF(ISNUMBER(SEARCH("@id=",D67)),"xpath(""","id("""),D67,")"";")</f>
-        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div)";</v>
+        <f t="shared" si="0"/>
+        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div");</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -7261,8 +7246,8 @@
         <v>177</v>
       </c>
       <c r="E68" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2])";</v>
+        <f t="shared" ref="E68:E77" si="1">CONCATENATE("public By ",B68,C68,"=By.",IF(ISNUMBER(SEARCH("@id=",D68)),"xpath(""","id("""),D68,""");")</f>
+        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2]");</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -7280,7 +7265,7 @@
       </c>
       <c r="E69" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2])";</v>
+        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2]");</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -7298,7 +7283,7 @@
       </c>
       <c r="E70" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2])";</v>
+        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2]");</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -7316,7 +7301,7 @@
       </c>
       <c r="E71" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2])";</v>
+        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2]");</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -7334,7 +7319,7 @@
       </c>
       <c r="E72" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a)";</v>
+        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a");</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -7352,7 +7337,7 @@
       </c>
       <c r="E73" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button)";</v>
+        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button");</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -7370,7 +7355,7 @@
       </c>
       <c r="E74" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnPAGAROTRAFACTURA=By.xpath("//*[@id='details-transaction']/div[5]/a[2]/button)";</v>
+        <v>public By btnPAGAROTRAFACTURA=By.xpath("//*[@id='details-transaction']/div[5]/a[2]/button");</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -7384,11 +7369,11 @@
         <v>211</v>
       </c>
       <c r="D75" s="56" t="s">
-        <v>298</v>
+        <v>210</v>
       </c>
       <c r="E75" s="56" t="str">
         <f t="shared" si="1"/>
-        <v>public By txtE-mail=By.id("id='PNEMail')";</v>
+        <v>public By txtE-mail=By.id("PNEMail");</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -7402,11 +7387,11 @@
         <v>253</v>
       </c>
       <c r="D76" s="56" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E76" s="56" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnIralBanco=By.id("id='btnSeguir')";</v>
+        <v>public By btnIralBanco=By.id("btnSeguir");</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -7420,11 +7405,11 @@
         <v>254</v>
       </c>
       <c r="D77" s="56" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E77" s="56" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnRegresaralcomercio=By.id("id='btnCancel')";</v>
+        <v>public By btnRegresaralcomercio=By.id("btnCancel");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalización de la HU009
All funcional
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Objetos" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Objetos!$A$2:$D$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Objetos!$A$2:$D$77</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Unificado!$A$2:$I$75</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="307">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -938,6 +938,15 @@
   </si>
   <si>
     <t>//*[@id='content_left_forms_unified']/div[1]/span</t>
+  </si>
+  <si>
+    <t>FacturasPendientes</t>
+  </si>
+  <si>
+    <t>//*[@id="content_list_invoices"]</t>
+  </si>
+  <si>
+    <t>alert_main</t>
   </si>
 </sst>
 </file>
@@ -948,7 +957,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -982,6 +991,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1231,7 +1248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1470,6 +1487,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1556,6 +1576,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2146,78 +2169,78 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="92" t="s">
+      <c r="A14" s="93" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
+      <c r="B14" s="93"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="92"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
-      <c r="B16" s="92"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
+      <c r="A16" s="93"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="92"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
+      <c r="F17" s="93"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
+      <c r="A18" s="93"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="92"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
+      <c r="A20" s="93"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="92"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="92"/>
-      <c r="E21" s="92"/>
-      <c r="F21" s="92"/>
+      <c r="A21" s="93"/>
+      <c r="B21" s="93"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="92"/>
-      <c r="B22" s="92"/>
-      <c r="C22" s="92"/>
-      <c r="D22" s="92"/>
-      <c r="E22" s="92"/>
-      <c r="F22" s="92"/>
+      <c r="A22" s="93"/>
+      <c r="B22" s="93"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2250,17 +2273,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -4535,14 +4558,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4565,7 +4588,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="107" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4585,7 +4608,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="107"/>
+      <c r="A4" s="108"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -4603,7 +4626,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="107"/>
+      <c r="A5" s="108"/>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -4621,7 +4644,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
+      <c r="A6" s="108"/>
       <c r="B6" s="3" t="s">
         <v>101</v>
       </c>
@@ -4639,7 +4662,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
@@ -4660,7 +4683,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
+      <c r="A8" s="108"/>
       <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
@@ -4681,7 +4704,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="108"/>
+      <c r="A9" s="109"/>
       <c r="B9" s="3" t="s">
         <v>229</v>
       </c>
@@ -4699,7 +4722,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="116" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -4719,7 +4742,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="116"/>
+      <c r="A11" s="117"/>
       <c r="B11" s="7" t="s">
         <v>124</v>
       </c>
@@ -4740,7 +4763,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="116"/>
+      <c r="A12" s="117"/>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -4758,7 +4781,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="116"/>
+      <c r="A13" s="117"/>
       <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
@@ -4779,7 +4802,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="116"/>
+      <c r="A14" s="117"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -4797,7 +4820,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="116"/>
+      <c r="A15" s="117"/>
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -4815,7 +4838,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="116"/>
+      <c r="A16" s="117"/>
       <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
@@ -4833,7 +4856,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="116"/>
+      <c r="A17" s="117"/>
       <c r="B17" s="7" t="s">
         <v>101</v>
       </c>
@@ -4851,7 +4874,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="116"/>
+      <c r="A18" s="117"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -4869,7 +4892,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="117"/>
+      <c r="A19" s="118"/>
       <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
@@ -4887,7 +4910,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="100" t="s">
+      <c r="A20" s="101" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -4907,7 +4930,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
+      <c r="A21" s="102"/>
       <c r="B21" s="4" t="s">
         <v>81</v>
       </c>
@@ -4932,7 +4955,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="101"/>
+      <c r="A22" s="102"/>
       <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
@@ -4950,7 +4973,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="101"/>
+      <c r="A23" s="102"/>
       <c r="B23" s="4" t="s">
         <v>82</v>
       </c>
@@ -4968,7 +4991,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="102"/>
+      <c r="A24" s="103"/>
       <c r="B24" s="4" t="s">
         <v>83</v>
       </c>
@@ -4993,7 +5016,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="103" t="s">
+      <c r="A25" s="104" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -5013,7 +5036,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="104"/>
+      <c r="A26" s="105"/>
       <c r="B26" s="13" t="s">
         <v>27</v>
       </c>
@@ -5031,7 +5054,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="105"/>
+      <c r="A27" s="106"/>
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -5049,7 +5072,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="119" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5069,7 +5092,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="119"/>
+      <c r="A29" s="120"/>
       <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
@@ -5090,7 +5113,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="119"/>
+      <c r="A30" s="120"/>
       <c r="B30" s="15" t="s">
         <v>118</v>
       </c>
@@ -5111,7 +5134,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="119"/>
+      <c r="A31" s="120"/>
       <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
@@ -5129,7 +5152,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="119"/>
+      <c r="A32" s="120"/>
       <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
@@ -5147,7 +5170,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="119"/>
+      <c r="A33" s="120"/>
       <c r="B33" s="15" t="s">
         <v>35</v>
       </c>
@@ -5165,7 +5188,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="119"/>
+      <c r="A34" s="120"/>
       <c r="B34" s="15" t="s">
         <v>36</v>
       </c>
@@ -5183,7 +5206,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="119"/>
+      <c r="A35" s="120"/>
       <c r="B35" s="15" t="s">
         <v>39</v>
       </c>
@@ -5201,7 +5224,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="119"/>
+      <c r="A36" s="120"/>
       <c r="B36" s="15" t="s">
         <v>3</v>
       </c>
@@ -5219,7 +5242,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="119"/>
+      <c r="A37" s="120"/>
       <c r="B37" s="15" t="s">
         <v>42</v>
       </c>
@@ -5237,7 +5260,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="119"/>
+      <c r="A38" s="120"/>
       <c r="B38" s="15" t="s">
         <v>122</v>
       </c>
@@ -5258,7 +5281,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="119"/>
+      <c r="A39" s="120"/>
       <c r="B39" s="15" t="s">
         <v>44</v>
       </c>
@@ -5276,7 +5299,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="119"/>
+      <c r="A40" s="120"/>
       <c r="B40" s="15" t="s">
         <v>130</v>
       </c>
@@ -5297,7 +5320,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="119"/>
+      <c r="A41" s="120"/>
       <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
@@ -5315,7 +5338,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="119"/>
+      <c r="A42" s="120"/>
       <c r="B42" s="15" t="s">
         <v>110</v>
       </c>
@@ -5336,7 +5359,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="119"/>
+      <c r="A43" s="120"/>
       <c r="B43" s="15" t="s">
         <v>47</v>
       </c>
@@ -5352,7 +5375,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="119"/>
+      <c r="A44" s="120"/>
       <c r="B44" s="15" t="s">
         <v>101</v>
       </c>
@@ -5368,7 +5391,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="119"/>
+      <c r="A45" s="120"/>
       <c r="B45" s="15" t="s">
         <v>22</v>
       </c>
@@ -5386,7 +5409,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="120"/>
+      <c r="A46" s="121"/>
       <c r="B46" s="15" t="s">
         <v>51</v>
       </c>
@@ -5404,7 +5427,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="109" t="s">
+      <c r="A47" s="110" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -5424,7 +5447,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="110"/>
+      <c r="A48" s="111"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -5442,7 +5465,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="110"/>
+      <c r="A49" s="111"/>
       <c r="B49" s="5" t="s">
         <v>56</v>
       </c>
@@ -5460,7 +5483,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="110"/>
+      <c r="A50" s="111"/>
       <c r="B50" s="5" t="s">
         <v>3</v>
       </c>
@@ -5478,7 +5501,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="110"/>
+      <c r="A51" s="111"/>
       <c r="B51" s="5" t="s">
         <v>60</v>
       </c>
@@ -5496,7 +5519,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="110"/>
+      <c r="A52" s="111"/>
       <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
@@ -5514,7 +5537,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="110"/>
+      <c r="A53" s="111"/>
       <c r="B53" s="5" t="s">
         <v>101</v>
       </c>
@@ -5530,7 +5553,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="110"/>
+      <c r="A54" s="111"/>
       <c r="B54" s="5" t="s">
         <v>22</v>
       </c>
@@ -5548,7 +5571,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="111"/>
+      <c r="A55" s="112"/>
       <c r="B55" s="5" t="s">
         <v>64</v>
       </c>
@@ -5566,7 +5589,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="112" t="s">
+      <c r="A56" s="113" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -5586,7 +5609,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="113"/>
+      <c r="A57" s="114"/>
       <c r="B57" s="1" t="s">
         <v>101</v>
       </c>
@@ -5602,7 +5625,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="113"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="1" t="s">
         <v>22</v>
       </c>
@@ -5620,7 +5643,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="114"/>
+      <c r="A59" s="115"/>
       <c r="B59" s="1" t="s">
         <v>48</v>
       </c>
@@ -5638,7 +5661,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="95" t="s">
+      <c r="A60" s="96" t="s">
         <v>136</v>
       </c>
       <c r="B60" s="23" t="s">
@@ -5661,7 +5684,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="96"/>
+      <c r="A61" s="97"/>
       <c r="B61" s="23" t="s">
         <v>137</v>
       </c>
@@ -5679,7 +5702,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="96"/>
+      <c r="A62" s="97"/>
       <c r="B62" s="23" t="s">
         <v>138</v>
       </c>
@@ -5697,7 +5720,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="96"/>
+      <c r="A63" s="97"/>
       <c r="B63" s="23" t="s">
         <v>139</v>
       </c>
@@ -5715,7 +5738,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="96"/>
+      <c r="A64" s="97"/>
       <c r="B64" s="23" t="s">
         <v>140</v>
       </c>
@@ -5733,7 +5756,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="96"/>
+      <c r="A65" s="97"/>
       <c r="B65" s="23" t="s">
         <v>141</v>
       </c>
@@ -5751,7 +5774,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="96"/>
+      <c r="A66" s="97"/>
       <c r="B66" s="23" t="s">
         <v>142</v>
       </c>
@@ -5769,7 +5792,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="96"/>
+      <c r="A67" s="97"/>
       <c r="B67" s="23" t="s">
         <v>143</v>
       </c>
@@ -5787,7 +5810,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="96"/>
+      <c r="A68" s="97"/>
       <c r="B68" s="23" t="s">
         <v>144</v>
       </c>
@@ -5805,7 +5828,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="96"/>
+      <c r="A69" s="97"/>
       <c r="B69" s="23" t="s">
         <v>145</v>
       </c>
@@ -5823,7 +5846,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="96"/>
+      <c r="A70" s="97"/>
       <c r="B70" s="23" t="s">
         <v>146</v>
       </c>
@@ -5841,7 +5864,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="96"/>
+      <c r="A71" s="97"/>
       <c r="B71" s="23" t="s">
         <v>147</v>
       </c>
@@ -5859,7 +5882,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="96"/>
+      <c r="A72" s="97"/>
       <c r="B72" s="23" t="s">
         <v>148</v>
       </c>
@@ -5877,7 +5900,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="96"/>
+      <c r="A73" s="97"/>
       <c r="B73" s="23" t="s">
         <v>149</v>
       </c>
@@ -5895,7 +5918,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="97"/>
+      <c r="A74" s="98"/>
       <c r="B74" s="23" t="s">
         <v>150</v>
       </c>
@@ -6062,10 +6085,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6136,7 +6159,7 @@
         <v>285</v>
       </c>
       <c r="E4" s="48" t="str">
-        <f t="shared" ref="E4:E68" si="0">CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
+        <f t="shared" ref="E4:E70" si="0">CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
         <v>public By btnHogar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p");</v>
       </c>
     </row>
@@ -6377,51 +6400,51 @@
         <v>231</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>229</v>
-      </c>
-      <c r="D18" s="51"/>
+        <v>304</v>
+      </c>
+      <c r="D18" s="92" t="s">
+        <v>306</v>
+      </c>
       <c r="E18" s="51" t="str">
         <f t="shared" si="0"/>
+        <v>public By lbFacturasPendientes=By.id("alert_main");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>304</v>
+      </c>
+      <c r="D19" s="122" t="s">
+        <v>305</v>
+      </c>
+      <c r="E19" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listFacturasPendientes=By.xpath("//*[@id="content_list_invoices"]");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51" t="str">
+        <f t="shared" si="0"/>
         <v>public By CapcharCaptchar=By.id("");</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="53" t="s">
-        <v>235</v>
-      </c>
-      <c r="C19" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D19" s="53" t="s">
-        <v>299</v>
-      </c>
-      <c r="E19" s="53" t="str">
-        <f t="shared" si="0"/>
-        <v>public By txtNumerodeLinea=By.id("value");</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="53" t="s">
-        <v>235</v>
-      </c>
-      <c r="C20" s="53" t="s">
-        <v>277</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" s="53" t="str">
-        <f t="shared" si="0"/>
-        <v>public By txtFechaLimitePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[1]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -6432,14 +6455,14 @@
         <v>235</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>162</v>
+        <v>299</v>
       </c>
       <c r="E21" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtReferentePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By txtNumerodeLinea=By.id("value");</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -6450,14 +6473,14 @@
         <v>235</v>
       </c>
       <c r="C22" s="53" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E22" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtPeriodoFacturacion=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By txtFechaLimitePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[1]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -6468,50 +6491,50 @@
         <v>235</v>
       </c>
       <c r="C23" s="53" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E23" s="53" t="str">
         <f t="shared" si="0"/>
+        <v>public By txtReferentePago=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="C24" s="53" t="s">
+        <v>279</v>
+      </c>
+      <c r="D24" s="53" t="s">
+        <v>163</v>
+      </c>
+      <c r="E24" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtPeriodoFacturacion=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[3]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>280</v>
+      </c>
+      <c r="D25" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="E25" s="53" t="str">
+        <f t="shared" si="0"/>
         <v>public By txtValorPagar=By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div[2]/div[4]/div[2]");</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>281</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>public By linkTarjetaCredito=By.id("payment-method-type-label-credit-payu");</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>271</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>public By linkDebitoBancarioPSE=By.id("payment-method-type-label-debit-payu");</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -6522,50 +6545,50 @@
         <v>233</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>237</v>
+        <v>281</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E26" s="34" t="str">
         <f t="shared" si="0"/>
+        <v>public By linkTarjetaCredito=By.id("payment-method-type-label-credit-payu");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkDebitoBancarioPSE=By.id("payment-method-type-label-debit-payu");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="34" t="str">
+        <f t="shared" si="0"/>
         <v>public By linkOtrosmediosdepago=By.id("payment-method-type-label-others-pay-methods");</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>263</v>
-      </c>
-      <c r="D27" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber");</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="35" t="s">
-        <v>236</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="E28" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -6573,17 +6596,17 @@
         <v>26</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>165</v>
+        <v>29</v>
       </c>
       <c r="E29" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber");</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -6591,17 +6614,17 @@
         <v>26</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>30</v>
+        <v>238</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="E30" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCVV/CVC=By.id("edit-cvc");</v>
+        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -6609,17 +6632,17 @@
         <v>26</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="E31" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration");</v>
+        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -6627,17 +6650,17 @@
         <v>26</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>241</v>
+        <v>30</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E32" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration");</v>
+        <v>public By txtCVV/CVC=By.id("edit-cvc");</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -6648,14 +6671,14 @@
         <v>234</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>36</v>
+        <v>240</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E33" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listCuotas=By.id("edit-cardnumber-quota");</v>
+        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration");</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -6663,17 +6686,17 @@
         <v>26</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>39</v>
+        <v>241</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E34" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNombre=By.id("edit-ccname");</v>
+        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration");</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -6684,14 +6707,14 @@
         <v>234</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E35" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipo=By.id("edit-buyer-document-type");</v>
+        <v>public By listCuotas=By.id("edit-cardnumber-quota");</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -6702,14 +6725,14 @@
         <v>235</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>246</v>
+        <v>39</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E36" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodedocumento=By.id("edit-buyer-document");</v>
+        <v>public By txtNombre=By.id("edit-ccname");</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -6717,17 +6740,17 @@
         <v>26</v>
       </c>
       <c r="B37" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>264</v>
+        <v>3</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>166</v>
+        <v>40</v>
       </c>
       <c r="E37" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
+        <v>public By listTipo=By.id("edit-buyer-document-type");</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -6738,14 +6761,14 @@
         <v>235</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E38" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone");</v>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document");</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -6756,14 +6779,14 @@
         <v>236</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E39" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -6774,14 +6797,14 @@
         <v>235</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E40" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail");</v>
+        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone");</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -6792,14 +6815,14 @@
         <v>236</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="D41" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E41" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
+        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -6807,17 +6830,17 @@
         <v>26</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>93</v>
+        <v>235</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E42" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize");</v>
+        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail");</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -6825,17 +6848,17 @@
         <v>26</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C43" s="35" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E43" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -6843,17 +6866,17 @@
         <v>26</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>232</v>
+        <v>93</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>22</v>
+        <v>242</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E44" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.id("edit-cancel");</v>
+        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize");</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -6861,53 +6884,53 @@
         <v>26</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C45" s="35" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="E45" s="35" t="str">
         <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("edit-cancel");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="35" t="str">
+        <f t="shared" si="0"/>
         <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit");</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="C46" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>public By listBanco=By.id("edit-bank");</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="C47" s="36" t="s">
-        <v>244</v>
-      </c>
-      <c r="D47" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>public By listTipodepersona=By.id("edit-buyer-type-person");</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -6915,17 +6938,17 @@
         <v>27</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C48" s="36" t="s">
-        <v>245</v>
+        <v>52</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E48" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNombresyapellidos=By.id("edit-buyer-name");</v>
+        <v>public By listBanco=By.id("edit-bank");</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -6936,14 +6959,14 @@
         <v>234</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>3</v>
+        <v>244</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E49" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By listTipo=By.id("edit-buyer-document-type--2");</v>
+        <v>public By listTipodepersona=By.id("edit-buyer-type-person");</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -6954,14 +6977,14 @@
         <v>235</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E50" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2");</v>
+        <v>public By txtNombresyapellidos=By.id("edit-buyer-name");</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -6969,17 +6992,17 @@
         <v>27</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>264</v>
+        <v>3</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>287</v>
+        <v>58</v>
       </c>
       <c r="E51" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p");</v>
+        <v>public By listTipo=By.id("edit-buyer-document-type--2");</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -6990,14 +7013,14 @@
         <v>235</v>
       </c>
       <c r="C52" s="36" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="D52" s="36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E52" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2");</v>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2");</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -7008,14 +7031,14 @@
         <v>236</v>
       </c>
       <c r="C53" s="36" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E53" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p");</v>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p");</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -7023,17 +7046,17 @@
         <v>27</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C54" s="36" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>289</v>
+        <v>61</v>
       </c>
       <c r="E54" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a");</v>
+        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2");</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -7041,17 +7064,17 @@
         <v>27</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C55" s="36" t="s">
-        <v>22</v>
+        <v>256</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>63</v>
+        <v>288</v>
       </c>
       <c r="E55" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.id("edit-cancel--2");</v>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p");</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -7059,53 +7082,53 @@
         <v>27</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C56" s="36" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="D56" s="36" t="s">
-        <v>65</v>
+        <v>289</v>
       </c>
       <c r="E56" s="36" t="str">
         <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a");</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="C57" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("edit-cancel--2");</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="D58" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E58" s="36" t="str">
+        <f t="shared" si="0"/>
         <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2");</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B57" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="C57" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="D57" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E57" s="37" t="str">
-        <f t="shared" si="0"/>
-        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.id("edit-nequi-account");</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B58" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="C58" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="D58" s="37" t="s">
-        <v>290</v>
-      </c>
-      <c r="E58" s="37" t="str">
-        <f t="shared" si="0"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--3']/div/a");</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -7113,17 +7136,17 @@
         <v>28</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>22</v>
+        <v>265</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E59" s="37" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel");</v>
+        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.id("edit-nequi-account");</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -7131,53 +7154,53 @@
         <v>28</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>48</v>
+        <v>270</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>69</v>
+        <v>290</v>
       </c>
       <c r="E60" s="37" t="str">
         <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--3']/div/a");</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel");</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E62" s="37" t="str">
+        <f t="shared" si="0"/>
         <v>public By btnPagar=By.id("tigoune-nequi-button-submit");</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B61" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="C61" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="D61" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="E61" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>public By lbMensajedePagorealizado=By.id("gateway-content-alert-message");</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B62" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="C62" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="D62" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="E62" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -7188,14 +7211,14 @@
         <v>236</v>
       </c>
       <c r="C63" s="38" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="E63" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By lbMensajedePagorealizado=By.id("gateway-content-alert-message");</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -7206,14 +7229,14 @@
         <v>236</v>
       </c>
       <c r="C64" s="38" t="s">
-        <v>258</v>
+        <v>137</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E64" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -7224,14 +7247,14 @@
         <v>236</v>
       </c>
       <c r="C65" s="38" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="D65" s="38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E65" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div");</v>
+        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -7242,14 +7265,14 @@
         <v>236</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>141</v>
+        <v>258</v>
       </c>
       <c r="D66" s="38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E66" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text()");</v>
+        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -7260,14 +7283,14 @@
         <v>236</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D67" s="38" t="s">
-        <v>300</v>
+        <v>173</v>
       </c>
       <c r="E67" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbCodigo=By.id("transaction-description-error");</v>
+        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div");</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -7278,14 +7301,14 @@
         <v>236</v>
       </c>
       <c r="C68" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E68" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div");</v>
+        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text()");</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -7296,14 +7319,14 @@
         <v>236</v>
       </c>
       <c r="C69" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D69" s="38" t="s">
-        <v>177</v>
+        <v>300</v>
       </c>
       <c r="E69" s="38" t="str">
-        <f t="shared" ref="E69:E78" si="1">CONCATENATE("public By ",B69,C69,"=By.",IF(ISNUMBER(SEARCH("@id=",D69)),"xpath(""","id("""),D69,""");")</f>
-        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2]");</v>
+        <f t="shared" si="0"/>
+        <v>public By lbCodigo=By.id("transaction-description-error");</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -7314,14 +7337,14 @@
         <v>236</v>
       </c>
       <c r="C70" s="38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D70" s="38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E70" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2]");</v>
+        <f t="shared" si="0"/>
+        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div");</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -7332,14 +7355,14 @@
         <v>236</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>146</v>
+        <v>260</v>
       </c>
       <c r="D71" s="38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E71" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2]");</v>
+        <f t="shared" ref="E71:E80" si="1">CONCATENATE("public By ",B71,C71,"=By.",IF(ISNUMBER(SEARCH("@id=",D71)),"xpath(""","id("""),D71,""");")</f>
+        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2]");</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -7350,14 +7373,14 @@
         <v>236</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>261</v>
+        <v>145</v>
       </c>
       <c r="D72" s="38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E72" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2]");</v>
+        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2]");</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -7365,17 +7388,17 @@
         <v>136</v>
       </c>
       <c r="B73" s="38" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C73" s="38" t="s">
-        <v>250</v>
+        <v>146</v>
       </c>
       <c r="D73" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E73" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a");</v>
+        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2]");</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -7383,17 +7406,17 @@
         <v>136</v>
       </c>
       <c r="B74" s="38" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C74" s="38" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="D74" s="38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E74" s="38" t="str">
         <f t="shared" si="1"/>
-        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button");</v>
+        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2]");</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -7401,53 +7424,53 @@
         <v>136</v>
       </c>
       <c r="B75" s="38" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D75" s="38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E75" s="38" t="str">
         <f t="shared" si="1"/>
+        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a");</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C76" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D76" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="E76" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button");</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B77" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C77" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="D77" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E77" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>public By btnPAGAROTRAFACTURA=By.xpath("//*[@id='details-transaction']/div[5]/a[2]/button");</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="46" t="s">
-        <v>209</v>
-      </c>
-      <c r="B76" s="56" t="s">
-        <v>235</v>
-      </c>
-      <c r="C76" s="56" t="s">
-        <v>211</v>
-      </c>
-      <c r="D76" s="56" t="s">
-        <v>210</v>
-      </c>
-      <c r="E76" s="56" t="str">
-        <f t="shared" si="1"/>
-        <v>public By txtE-mail=By.id("PNEMail");</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="46" t="s">
-        <v>209</v>
-      </c>
-      <c r="B77" s="56" t="s">
-        <v>232</v>
-      </c>
-      <c r="C77" s="56" t="s">
-        <v>253</v>
-      </c>
-      <c r="D77" s="56" t="s">
-        <v>297</v>
-      </c>
-      <c r="E77" s="56" t="str">
-        <f t="shared" si="1"/>
-        <v>public By btnIralBanco=By.id("btnSeguir");</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -7455,21 +7478,57 @@
         <v>209</v>
       </c>
       <c r="B78" s="56" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C78" s="56" t="s">
-        <v>254</v>
+        <v>211</v>
       </c>
       <c r="D78" s="56" t="s">
-        <v>298</v>
+        <v>210</v>
       </c>
       <c r="E78" s="56" t="str">
         <f t="shared" si="1"/>
+        <v>public By txtE-mail=By.id("PNEMail");</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="C79" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D79" s="56" t="s">
+        <v>297</v>
+      </c>
+      <c r="E79" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnIralBanco=By.id("btnSeguir");</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B80" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="C80" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="D80" s="56" t="s">
+        <v>298</v>
+      </c>
+      <c r="E80" s="56" t="str">
+        <f t="shared" si="1"/>
         <v>public By btnRegresaralcomercio=By.id("btnCancel");</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D75"/>
+  <autoFilter ref="A2:D77"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios en el archivo de excel que tiene los objetos
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -957,7 +957,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -991,14 +991,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1248,7 +1240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1487,7 +1479,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1576,9 +1568,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6088,7 +6077,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6423,7 +6412,7 @@
       <c r="C19" s="51" t="s">
         <v>304</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="92" t="s">
         <v>305</v>
       </c>
       <c r="E19" s="51" t="str">

</xml_diff>

<commit_message>
Arreglos para generar bien el reporte.
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -886,9 +886,6 @@
     <t>//*[@id='block-tigo-theme-content']/div/div[1]/div/div/div[1]/p</t>
   </si>
   <si>
-    <t>//*[@id='content_right_forms_unified']/div/div/label</t>
-  </si>
-  <si>
     <t>//*[@id='edit-content-document--2']/div/p</t>
   </si>
   <si>
@@ -947,6 +944,9 @@
   </si>
   <si>
     <t>alert_main</t>
+  </si>
+  <si>
+    <t>edit-email-fijo</t>
   </si>
 </sst>
 </file>
@@ -2712,13 +2712,13 @@
         <v>231</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>70</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E17" s="52" t="s">
         <v>76</v>
@@ -2733,7 +2733,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="51" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -6199,7 +6199,7 @@
         <v>274</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E7" s="48" t="str">
         <f t="shared" si="0"/>
@@ -6217,7 +6217,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E8" s="48" t="str">
         <f t="shared" si="0"/>
@@ -6287,7 +6287,7 @@
         <v>275</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E12" s="51" t="str">
         <f t="shared" si="0"/>
@@ -6305,7 +6305,7 @@
         <v>276</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E13" s="51" t="str">
         <f t="shared" si="0"/>
@@ -6323,11 +6323,11 @@
         <v>255</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="E14" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>public By txtCorreoElectronico=By.xpath("//*[@id='content_right_forms_unified']/div/div/label");</v>
+        <v>public By txtCorreoElectronico=By.id("edit-email-fijo");</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6341,7 +6341,7 @@
         <v>274</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E15" s="51" t="str">
         <f t="shared" si="0"/>
@@ -6359,7 +6359,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E16" s="51" t="str">
         <f t="shared" si="0"/>
@@ -6374,10 +6374,10 @@
         <v>236</v>
       </c>
       <c r="C17" s="51" t="s">
+        <v>301</v>
+      </c>
+      <c r="D17" s="51" t="s">
         <v>302</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>303</v>
       </c>
       <c r="E17" s="51" t="str">
         <f t="shared" si="0"/>
@@ -6392,10 +6392,10 @@
         <v>236</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D18" s="92" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E18" s="51" t="str">
         <f t="shared" si="0"/>
@@ -6410,10 +6410,10 @@
         <v>234</v>
       </c>
       <c r="C19" s="51" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="92" t="s">
         <v>304</v>
-      </c>
-      <c r="D19" s="92" t="s">
-        <v>305</v>
       </c>
       <c r="E19" s="51" t="str">
         <f t="shared" si="0"/>
@@ -6447,7 +6447,7 @@
         <v>262</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E21" s="53" t="str">
         <f t="shared" si="0"/>
@@ -7023,7 +7023,7 @@
         <v>264</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E53" s="36" t="str">
         <f t="shared" si="0"/>
@@ -7059,7 +7059,7 @@
         <v>256</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E55" s="36" t="str">
         <f t="shared" si="0"/>
@@ -7077,7 +7077,7 @@
         <v>270</v>
       </c>
       <c r="D56" s="36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E56" s="36" t="str">
         <f t="shared" si="0"/>
@@ -7149,7 +7149,7 @@
         <v>270</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E60" s="37" t="str">
         <f t="shared" si="0"/>
@@ -7311,7 +7311,7 @@
         <v>259</v>
       </c>
       <c r="D69" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E69" s="38" t="str">
         <f t="shared" si="0"/>
@@ -7491,7 +7491,7 @@
         <v>253</v>
       </c>
       <c r="D79" s="56" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E79" s="56" t="str">
         <f t="shared" si="1"/>
@@ -7509,7 +7509,7 @@
         <v>254</v>
       </c>
       <c r="D80" s="56" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E80" s="56" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Se actualiza el archivo del Mapeo de los objetos, dejandolos en 1 solo archivo
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -1,28 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasprilla\Documents\automatizacion_base\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B91DB4-8B3F-401D-87B1-5470BFBB51A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
     <sheet name="Unificado" sheetId="2" r:id="rId2"/>
     <sheet name="Pantallas Movil" sheetId="1" r:id="rId3"/>
     <sheet name="Plantilla estimación" sheetId="4" r:id="rId4"/>
-    <sheet name="Objetos" sheetId="5" r:id="rId5"/>
+    <sheet name="ObjetosPasarela" sheetId="5" r:id="rId5"/>
+    <sheet name="ObjetosMiCuenta" sheetId="6" r:id="rId6"/>
+    <sheet name="ObjetosRecargas" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Objetos!$A$2:$D$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ObjetosPasarela!$A$2:$D$77</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Unificado!$A$2:$I$75</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="416">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -947,12 +955,339 @@
   </si>
   <si>
     <t>edit-email-fijo</t>
+  </si>
+  <si>
+    <t>Listado de Objetos en el proceso Mi Cuenta Tigo</t>
+  </si>
+  <si>
+    <t>InicioMiCuentaTigo</t>
+  </si>
+  <si>
+    <t>IngresarAMiCuenta</t>
+  </si>
+  <si>
+    <t>//*[@id="top_menu_aside"]/nav/ul/li/a</t>
+  </si>
+  <si>
+    <t>IniciarSesion</t>
+  </si>
+  <si>
+    <t>//*[@id="top_menu_aside"]/nav/ul/li/ul/li/a</t>
+  </si>
+  <si>
+    <t>Registrarme</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[1]</t>
+  </si>
+  <si>
+    <t>Ingresar</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[2]</t>
+  </si>
+  <si>
+    <t>PagaTusFacturas</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[3]/div/div/div/div/a</t>
+  </si>
+  <si>
+    <t>RecargasYPaquetes</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[4]/div/div/div/div/a</t>
+  </si>
+  <si>
+    <t>RegistraTuEquipo</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[5]/div/div/div/div/a</t>
+  </si>
+  <si>
+    <t>ReponeTuSim</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[6]/div/div/div/div/a</t>
+  </si>
+  <si>
+    <t>CambiarMiClave</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[7]/div/div/div/div/div[2]/a</t>
+  </si>
+  <si>
+    <t>//*[@id="t_document"]/div/div/input</t>
+  </si>
+  <si>
+    <t>//*[@id="document"]</t>
+  </si>
+  <si>
+    <t>//*[@id="query-container"]/section/div[1]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="findagenda"]/div[2]/div[2]</t>
+  </si>
+  <si>
+    <t>ConsultaPQRUne</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[1]/p/a</t>
+  </si>
+  <si>
+    <t>ConsultaPQRTigo</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[2]/p/a</t>
+  </si>
+  <si>
+    <t>ConsultaSic</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[3]/p/a</t>
+  </si>
+  <si>
+    <t>ConoceNuestrasTiendas</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[4]/p/a</t>
+  </si>
+  <si>
+    <t>ChatYAyuda</t>
+  </si>
+  <si>
+    <t>//*[@id="Embed"]/button/span[2]</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>//*[@id="top_menu"]/nav/ul/li[1]/a</t>
+  </si>
+  <si>
+    <t>Empresas</t>
+  </si>
+  <si>
+    <t>//*[@id="top_menu"]/nav/ul/li[2]/a</t>
+  </si>
+  <si>
+    <t>DescubreloYa</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[1]/div/div/div/section/div/div/a</t>
+  </si>
+  <si>
+    <t>IngresaMiCuentaTigo</t>
+  </si>
+  <si>
+    <t>idEmail</t>
+  </si>
+  <si>
+    <t>ValidarCorreo</t>
+  </si>
+  <si>
+    <t>continueBtn</t>
+  </si>
+  <si>
+    <t>CrearTuCuenta</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/div[3]/div/p[2]/a</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Continuar</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[3]/button</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[4]/a</t>
+  </si>
+  <si>
+    <t>NumeroPlan</t>
+  </si>
+  <si>
+    <t>//*[@id="block-accountsblock-2"]/div/div/div/div/div/span</t>
+  </si>
+  <si>
+    <t>Resumen</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/div[2]/div/div/nav/div/div/ul/li[1]/a</t>
+  </si>
+  <si>
+    <t>CambiateYa</t>
+  </si>
+  <si>
+    <t>//*[@id="action_Cámbiate ya"]</t>
+  </si>
+  <si>
+    <t>CrearTuCuentaTigo</t>
+  </si>
+  <si>
+    <t>ConMiCorreo</t>
+  </si>
+  <si>
+    <t>//*[@id="addNew"]</t>
+  </si>
+  <si>
+    <t>ConFacebook</t>
+  </si>
+  <si>
+    <t>//*[@id="SLFacebook"]</t>
+  </si>
+  <si>
+    <t>ConGoogle</t>
+  </si>
+  <si>
+    <t>//*[@id="SLGoogle"]</t>
+  </si>
+  <si>
+    <t>IngresaAMiCuenta</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/div[1]/h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlvidasteContrasena </t>
+  </si>
+  <si>
+    <t>PQRUne</t>
+  </si>
+  <si>
+    <t>/html/body/div[4]/div/div/div/div[1]/h3</t>
+  </si>
+  <si>
+    <t>PQRTigo</t>
+  </si>
+  <si>
+    <t>//*[@id='formInicioPqr:panelBotonesInicio']/thead/tr/th/span</t>
+  </si>
+  <si>
+    <t>Sic</t>
+  </si>
+  <si>
+    <t>//*[@id=\'contenido_medio\']/div[1]/h1</t>
+  </si>
+  <si>
+    <t>PQR Tigo</t>
+  </si>
+  <si>
+    <t>PQR Une</t>
+  </si>
+  <si>
+    <t>Tiendas</t>
+  </si>
+  <si>
+    <t>/html/body/content/div[2]/div/section[1]/div/div/h3</t>
+  </si>
+  <si>
+    <t>VisitasPendientes</t>
+  </si>
+  <si>
+    <t>//*[@id=\'schedule-visits-container\']/div[2]/div[1]/div/p</t>
+  </si>
+  <si>
+    <t>MsgErrorDocumento</t>
+  </si>
+  <si>
+    <t>Listado de Objetos en el proceso Recargas y Paquetes</t>
+  </si>
+  <si>
+    <t>Recargas</t>
+  </si>
+  <si>
+    <t>Recarga</t>
+  </si>
+  <si>
+    <t>//*[@id="tap_selector"]/div[2]</t>
+  </si>
+  <si>
+    <t>TuLineaTigoR</t>
+  </si>
+  <si>
+    <t>//*[@id="num_lin"]</t>
+  </si>
+  <si>
+    <t>Valor3Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[1]</t>
+  </si>
+  <si>
+    <t>Valor6Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[2]</t>
+  </si>
+  <si>
+    <t>Valor15Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[3]</t>
+  </si>
+  <si>
+    <t>Valor 20Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[4]</t>
+  </si>
+  <si>
+    <t>Valor30Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[5]</t>
+  </si>
+  <si>
+    <t>OtroValor</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[6]</t>
+  </si>
+  <si>
+    <t>ValorRecargar</t>
+  </si>
+  <si>
+    <t>edit-otro-valor</t>
+  </si>
+  <si>
+    <t>ErrorValor</t>
+  </si>
+  <si>
+    <t>//*[@id="other_value"]/div/div/div[1]/p</t>
+  </si>
+  <si>
+    <t>Recargar</t>
+  </si>
+  <si>
+    <t>edit-button-recargar</t>
+  </si>
+  <si>
+    <t>ResumenTransaccion</t>
+  </si>
+  <si>
+    <t>//*[@id="title-detail"]</t>
+  </si>
+  <si>
+    <t>NumeroDelProducto</t>
+  </si>
+  <si>
+    <t>product-number</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -997,7 +1332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1088,8 +1423,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1235,12 +1588,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1569,10 +1937,43 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1580,12 +1981,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1627,7 +2031,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1660,9 +2064,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1695,6 +2116,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1870,14 +2308,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -1932,7 +2370,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>194</v>
       </c>
@@ -2240,14 +2678,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" style="39" customWidth="1"/>
     <col min="2" max="2" width="45" style="39" bestFit="1" customWidth="1"/>
@@ -3413,7 +3851,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>26</v>
       </c>
@@ -4519,7 +4957,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I75"/>
+  <autoFilter ref="A2:I75" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
@@ -4528,21 +4966,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F10" sqref="F10:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5942,14 +6380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" hidden="1" customWidth="1"/>
@@ -6073,19 +6511,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" style="39" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="39" customWidth="1"/>
-    <col min="4" max="5" width="61" style="39" customWidth="1"/>
+    <col min="4" max="4" width="61" style="39" customWidth="1"/>
+    <col min="5" max="5" width="135.42578125" style="39" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="39"/>
   </cols>
@@ -7517,8 +7956,2068 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D77"/>
+  <autoFilter ref="A2:D77" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDA504D-8FF2-405F-AE1B-22086E468A89}">
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" customWidth="1"/>
+    <col min="5" max="5" width="101.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>310</v>
+      </c>
+      <c r="E3" s="48" t="str">
+        <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
+        <v>public By btnIngresarAMiCuenta=By.xpath("//*[@id="top_menu_aside"]/nav/ul/li/a");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>312</v>
+      </c>
+      <c r="E4" s="48" t="str">
+        <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
+        <v>public By btnIniciarSesion=By.xpath("//*[@id="top_menu_aside"]/nav/ul/li/ul/li/a");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>314</v>
+      </c>
+      <c r="E5" s="48" t="str">
+        <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
+        <v>public By btnRegistrarme=By.xpath("//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[1]");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>316</v>
+      </c>
+      <c r="E6" s="48" t="str">
+        <f t="shared" ref="E6:E41" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <v>public By btnIngresar=By.xpath("//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[2]");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="E7" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagaTusFacturas=By.xpath("//*[@id="main-content"]/div[2]/div[3]/div/div/div/div/a");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnRecargasYPaquetes=By.xpath("//*[@id="main-content"]/div[2]/div[4]/div/div/div/div/a");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>322</v>
+      </c>
+      <c r="E9" s="91" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnRegistraTuEquipo=By.xpath("//*[@id="main-content"]/div[2]/div[5]/div/div/div/div/a");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B10" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="122" t="s">
+        <v>323</v>
+      </c>
+      <c r="D10" s="122" t="s">
+        <v>324</v>
+      </c>
+      <c r="E10" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnReponeTuSim=By.xpath("//*[@id="main-content"]/div[2]/div[6]/div/div/div/div/a");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B11" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="122" t="s">
+        <v>325</v>
+      </c>
+      <c r="D11" s="122" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCambiarMiClave=By.xpath("//*[@id="main-content"]/div[2]/div[7]/div/div/div/div/div[2]/a");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B12" s="122" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="122" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="122" t="s">
+        <v>327</v>
+      </c>
+      <c r="E12" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipo=By.xpath("//*[@id="t_document"]/div/div/input");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="122" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="122" t="s">
+        <v>328</v>
+      </c>
+      <c r="E13" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumeroDocumento=By.xpath("//*[@id="document"]");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B14" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="122" t="s">
+        <v>386</v>
+      </c>
+      <c r="D14" s="122" t="s">
+        <v>329</v>
+      </c>
+      <c r="E14" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMsgErrorDocumento=By.xpath("//*[@id="query-container"]/section/div[1]/span[2]");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="122" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="122" t="s">
+        <v>330</v>
+      </c>
+      <c r="E15" s="122" t="str">
+        <f t="shared" ref="E15" si="1">CONCATENATE("public By ",B15,C15,"=By.",IF(ISNUMBER(SEARCH("@id=",D15)),"xpath(""","id("""),D15,""");")</f>
+        <v>public By btnConsultar=By.xpath("//*[@id="findagenda"]/div[2]/div[2]");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="122" t="s">
+        <v>384</v>
+      </c>
+      <c r="D16" s="122" t="s">
+        <v>385</v>
+      </c>
+      <c r="E16" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbVisitasPendientes=By.xpath("//*[@id=\'schedule-visits-container\']/div[2]/div[1]/div/p");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" s="122" t="s">
+        <v>331</v>
+      </c>
+      <c r="D17" s="122" t="s">
+        <v>332</v>
+      </c>
+      <c r="E17" s="122" t="str">
+        <f t="shared" ref="E17" si="2">CONCATENATE("public By ",B17,C17,"=By.",IF(ISNUMBER(SEARCH("@id=",D17)),"xpath(""","id("""),D17,""");")</f>
+        <v>public By txtConsultaPQRUne=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[1]/p/a");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="B18" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="122" t="s">
+        <v>374</v>
+      </c>
+      <c r="D18" s="122" t="s">
+        <v>375</v>
+      </c>
+      <c r="E18" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbPQRUne=By.id("/html/body/div[4]/div/div/div/div[1]/h3");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B19" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C19" s="122" t="s">
+        <v>333</v>
+      </c>
+      <c r="D19" s="122" t="s">
+        <v>334</v>
+      </c>
+      <c r="E19" s="122" t="str">
+        <f t="shared" ref="E19" si="3">CONCATENATE("public By ",B19,C19,"=By.",IF(ISNUMBER(SEARCH("@id=",D19)),"xpath(""","id("""),D19,""");")</f>
+        <v>public By txtConsultaPQRTigo=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[2]/p/a");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="B20" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="122" t="s">
+        <v>376</v>
+      </c>
+      <c r="D20" s="122" t="s">
+        <v>377</v>
+      </c>
+      <c r="E20" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbPQRTigo=By.xpath("//*[@id='formInicioPqr:panelBotonesInicio']/thead/tr/th/span");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B21" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C21" s="122" t="s">
+        <v>335</v>
+      </c>
+      <c r="D21" s="122" t="s">
+        <v>336</v>
+      </c>
+      <c r="E21" s="122" t="str">
+        <f t="shared" ref="E21" si="4">CONCATENATE("public By ",B21,C21,"=By.",IF(ISNUMBER(SEARCH("@id=",D21)),"xpath(""","id("""),D21,""");")</f>
+        <v>public By txtConsultaSic=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[3]/p/a");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="B22" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="122" t="s">
+        <v>378</v>
+      </c>
+      <c r="D22" s="122" t="s">
+        <v>379</v>
+      </c>
+      <c r="E22" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbSic=By.xpath("//*[@id=\'contenido_medio\']/div[1]/h1");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B23" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C23" s="122" t="s">
+        <v>337</v>
+      </c>
+      <c r="D23" s="122" t="s">
+        <v>338</v>
+      </c>
+      <c r="E23" s="122" t="str">
+        <f t="shared" ref="E23" si="5">CONCATENATE("public By ",B23,C23,"=By.",IF(ISNUMBER(SEARCH("@id=",D23)),"xpath(""","id("""),D23,""");")</f>
+        <v>public By txtConoceNuestrasTiendas=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[4]/p/a");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="B24" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C24" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="D24" s="122" t="s">
+        <v>383</v>
+      </c>
+      <c r="E24" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbTiendas=By.id("/html/body/content/div[2]/div/section[1]/div/div/h3");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B25" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="122" t="s">
+        <v>339</v>
+      </c>
+      <c r="D25" s="122" t="s">
+        <v>340</v>
+      </c>
+      <c r="E25" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnChatYAyuda=By.xpath("//*[@id="Embed"]/button/span[2]");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B26" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="122" t="s">
+        <v>341</v>
+      </c>
+      <c r="D26" s="122" t="s">
+        <v>342</v>
+      </c>
+      <c r="E26" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtPersonas=By.xpath("//*[@id="top_menu"]/nav/ul/li[1]/a");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B27" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C27" s="122" t="s">
+        <v>343</v>
+      </c>
+      <c r="D27" s="122" t="s">
+        <v>344</v>
+      </c>
+      <c r="E27" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtEmpresas=By.xpath("//*[@id="top_menu"]/nav/ul/li[2]/a");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B28" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="122" t="s">
+        <v>345</v>
+      </c>
+      <c r="D28" s="122" t="s">
+        <v>346</v>
+      </c>
+      <c r="E28" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnDescubreloYa=By.xpath("//*[@id="main-content"]/div[2]/div[1]/div/div/div/section/div/div/a");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B29" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="124" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" s="124" t="s">
+        <v>348</v>
+      </c>
+      <c r="E29" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.id("idEmail");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B30" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="124" t="s">
+        <v>349</v>
+      </c>
+      <c r="D30" s="124" t="s">
+        <v>350</v>
+      </c>
+      <c r="E30" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnValidarCorreo=By.id("continueBtn");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B31" s="124" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="124" t="s">
+        <v>371</v>
+      </c>
+      <c r="D31" s="124" t="s">
+        <v>372</v>
+      </c>
+      <c r="E31" s="124" t="str">
+        <f t="shared" ref="E31" si="6">CONCATENATE("public By ",B31,C31,"=By.",IF(ISNUMBER(SEARCH("@id=",D31)),"xpath(""","id("""),D31,""");")</f>
+        <v>public By lbIngresaAMiCuenta=By.id("/html/body/div[2]/div/div[1]/h5");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B32" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C32" s="124" t="s">
+        <v>351</v>
+      </c>
+      <c r="D32" s="124" t="s">
+        <v>352</v>
+      </c>
+      <c r="E32" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCrearTuCuenta=By.id("/html/body/div[2]/div/div[3]/div/p[2]/a");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B33" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C33" s="124" t="s">
+        <v>353</v>
+      </c>
+      <c r="D33" s="124" t="s">
+        <v>354</v>
+      </c>
+      <c r="E33" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtContraseña=By.id("password");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B34" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="124" t="s">
+        <v>355</v>
+      </c>
+      <c r="D34" s="124" t="s">
+        <v>356</v>
+      </c>
+      <c r="E34" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnContinuar=By.id("/html/body/div[2]/div/form/div[3]/button");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B35" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C35" s="124" t="s">
+        <v>373</v>
+      </c>
+      <c r="D35" s="124" t="s">
+        <v>357</v>
+      </c>
+      <c r="E35" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtOlvidasteContrasena =By.id("/html/body/div[2]/div/form/div[4]/a");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B36" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="124" t="s">
+        <v>358</v>
+      </c>
+      <c r="D36" s="124" t="s">
+        <v>359</v>
+      </c>
+      <c r="E36" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listNumeroPlan=By.xpath("//*[@id="block-accountsblock-2"]/div/div/div/div/div/span");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B37" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="124" t="s">
+        <v>360</v>
+      </c>
+      <c r="D37" s="124" t="s">
+        <v>361</v>
+      </c>
+      <c r="E37" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtResumen=By.id("/html/body/div[3]/div[2]/div/div/nav/div/div/ul/li[1]/a");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B38" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="124" t="s">
+        <v>362</v>
+      </c>
+      <c r="D38" s="124" t="s">
+        <v>363</v>
+      </c>
+      <c r="E38" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCambiateYa=By.xpath("//*[@id="action_Cámbiate ya"]");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="125" t="s">
+        <v>364</v>
+      </c>
+      <c r="B39" s="126" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="126" t="s">
+        <v>365</v>
+      </c>
+      <c r="D39" s="126" t="s">
+        <v>366</v>
+      </c>
+      <c r="E39" s="126" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnConMiCorreo=By.xpath("//*[@id="addNew"]");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="125" t="s">
+        <v>364</v>
+      </c>
+      <c r="B40" s="126" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" s="126" t="s">
+        <v>367</v>
+      </c>
+      <c r="D40" s="126" t="s">
+        <v>368</v>
+      </c>
+      <c r="E40" s="126" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnConFacebook=By.xpath("//*[@id="SLFacebook"]");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="127" t="s">
+        <v>364</v>
+      </c>
+      <c r="B41" s="128" t="s">
+        <v>232</v>
+      </c>
+      <c r="C41" s="128" t="s">
+        <v>369</v>
+      </c>
+      <c r="D41" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="E41" s="128" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnConGoogle=By.xpath("//*[@id="SLGoogle"]");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E972679-EDA2-4ED9-97F5-E044AE9E5203}">
+  <dimension ref="A1:E72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="110.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>389</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="E3" s="48" t="str">
+        <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
+        <v>public By btnRecarga=By.xpath("//*[@id="tap_selector"]/div[2]");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>392</v>
+      </c>
+      <c r="E4" s="48" t="str">
+        <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
+        <v>public By txtTuLineaTigoR=By.xpath("//*[@id="num_lin"]");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>393</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>394</v>
+      </c>
+      <c r="E5" s="48" t="str">
+        <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
+        <v>public By btnValor3Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[1]");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>396</v>
+      </c>
+      <c r="E6" s="48" t="str">
+        <f t="shared" ref="E6:E69" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <v>public By btnValor6Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[2]");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="E7" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnValor15Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[3]");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>399</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="E8" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnValor 20Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[4]");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>401</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>402</v>
+      </c>
+      <c r="E9" s="91" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnValor30Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[5]");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B10" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="122" t="s">
+        <v>403</v>
+      </c>
+      <c r="D10" s="122" t="s">
+        <v>404</v>
+      </c>
+      <c r="E10" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnOtroValor=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[6]");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B11" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="122" t="s">
+        <v>405</v>
+      </c>
+      <c r="D11" s="122" t="s">
+        <v>406</v>
+      </c>
+      <c r="E11" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtValorRecargar=By.id("edit-otro-valor");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B12" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" s="122" t="s">
+        <v>407</v>
+      </c>
+      <c r="D12" s="122" t="s">
+        <v>408</v>
+      </c>
+      <c r="E12" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbErrorValor=By.xpath("//*[@id="other_value"]/div/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B13" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="122" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.id("edit-email");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B14" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="122" t="s">
+        <v>409</v>
+      </c>
+      <c r="D14" s="122" t="s">
+        <v>410</v>
+      </c>
+      <c r="E14" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnRecargar=By.id("edit-button-recargar");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="130" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="D15" s="130" t="s">
+        <v>412</v>
+      </c>
+      <c r="E15" s="130" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbResumenTransaccion=By.xpath("//*[@id="title-detail"]");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="130" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="130" t="s">
+        <v>413</v>
+      </c>
+      <c r="D16" s="130" t="s">
+        <v>414</v>
+      </c>
+      <c r="E16" s="130" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNumeroDelProducto=By.id("product-number");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="131" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="132" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="132" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E17" s="132" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbValorPagar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTarjetaCredito=By.id("payment-method-type-label-credit-payu");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkDebitoBancarioPSE=By.id("payment-method-type-label-debit-payu");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkOtrosmediosdepago=By.id("payment-method-type-label-others-pay-methods");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCVV/CVC=By.id("edit-cvc");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listCuotas=By.id("edit-cardnumber-quota");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNombre=By.id("edit-ccname");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipo=By.id("edit-buyer-document-type");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("edit-cancel");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listBanco=By.id("edit-bank");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipodepersona=By.id("edit-buyer-type-person");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNombresyapellidos=By.id("edit-buyer-name");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipo=By.id("edit-buyer-document-type--2");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="E45" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="D47" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="E47" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="D48" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="E48" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a");</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="C49" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("edit-cancel--2");</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="C50" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="D50" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2");</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.id("edit-nequi-account");</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="E52" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--3']/div/a");</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel");</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar=By.id("tigoune-nequi-button-submit");</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedePagorealizado=By.id("gateway-content-alert-message");</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C56" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>266</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E57" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C58" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="E58" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C59" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="D59" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E59" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C60" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D60" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text()");</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="D61" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="E61" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbCodigo=By.id("transaction-description-error");</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="E62" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div");</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="D63" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="E63" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2]");</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C64" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="D64" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="E64" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2]");</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C65" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="E65" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2]");</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C66" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="E66" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2]");</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="C67" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="D67" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="E67" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a");</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D68" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="E68" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button");</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C69" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E69" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPAGAROTRAFACTURA=By.xpath("//*[@id='details-transaction']/div[5]/a[2]/button");</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B70" s="56" t="s">
+        <v>235</v>
+      </c>
+      <c r="C70" s="56" t="s">
+        <v>211</v>
+      </c>
+      <c r="D70" s="56" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" s="56" t="str">
+        <f t="shared" ref="E70:E72" si="1">CONCATENATE("public By ",B70,C70,"=By.",IF(ISNUMBER(SEARCH("@id=",D70)),"xpath(""","id("""),D70,""");")</f>
+        <v>public By txtE-mail=By.id("PNEMail");</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B71" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="C71" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D71" s="56" t="s">
+        <v>296</v>
+      </c>
+      <c r="E71" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnIralBanco=By.id("btnSeguir");</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B72" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="C72" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="D72" s="56" t="s">
+        <v>297</v>
+      </c>
+      <c r="E72" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnRegresaralcomercio=By.id("btnCancel");</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Adherencia Pasarela de pagos.xlsx
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -1,28 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasprilla\Documents\automatizacion_base\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B91DB4-8B3F-401D-87B1-5470BFBB51A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
     <sheet name="Unificado" sheetId="2" r:id="rId2"/>
     <sheet name="Pantallas Movil" sheetId="1" r:id="rId3"/>
     <sheet name="Plantilla estimación" sheetId="4" r:id="rId4"/>
-    <sheet name="Objetos" sheetId="5" r:id="rId5"/>
+    <sheet name="ObjetosPasarela" sheetId="5" r:id="rId5"/>
+    <sheet name="ObjetosMiCuenta" sheetId="6" r:id="rId6"/>
+    <sheet name="ObjetosRecargas" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Objetos!$A$2:$D$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ObjetosPasarela!$A$2:$D$77</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Unificado!$A$2:$I$75</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="416">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -947,12 +955,339 @@
   </si>
   <si>
     <t>edit-email-fijo</t>
+  </si>
+  <si>
+    <t>Listado de Objetos en el proceso Mi Cuenta Tigo</t>
+  </si>
+  <si>
+    <t>InicioMiCuentaTigo</t>
+  </si>
+  <si>
+    <t>IngresarAMiCuenta</t>
+  </si>
+  <si>
+    <t>//*[@id="top_menu_aside"]/nav/ul/li/a</t>
+  </si>
+  <si>
+    <t>IniciarSesion</t>
+  </si>
+  <si>
+    <t>//*[@id="top_menu_aside"]/nav/ul/li/ul/li/a</t>
+  </si>
+  <si>
+    <t>Registrarme</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[1]</t>
+  </si>
+  <si>
+    <t>Ingresar</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[2]</t>
+  </si>
+  <si>
+    <t>PagaTusFacturas</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[3]/div/div/div/div/a</t>
+  </si>
+  <si>
+    <t>RecargasYPaquetes</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[4]/div/div/div/div/a</t>
+  </si>
+  <si>
+    <t>RegistraTuEquipo</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[5]/div/div/div/div/a</t>
+  </si>
+  <si>
+    <t>ReponeTuSim</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[6]/div/div/div/div/a</t>
+  </si>
+  <si>
+    <t>CambiarMiClave</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[7]/div/div/div/div/div[2]/a</t>
+  </si>
+  <si>
+    <t>//*[@id="t_document"]/div/div/input</t>
+  </si>
+  <si>
+    <t>//*[@id="document"]</t>
+  </si>
+  <si>
+    <t>//*[@id="query-container"]/section/div[1]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="findagenda"]/div[2]/div[2]</t>
+  </si>
+  <si>
+    <t>ConsultaPQRUne</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[1]/p/a</t>
+  </si>
+  <si>
+    <t>ConsultaPQRTigo</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[2]/p/a</t>
+  </si>
+  <si>
+    <t>ConsultaSic</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[3]/p/a</t>
+  </si>
+  <si>
+    <t>ConoceNuestrasTiendas</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[4]/p/a</t>
+  </si>
+  <si>
+    <t>ChatYAyuda</t>
+  </si>
+  <si>
+    <t>//*[@id="Embed"]/button/span[2]</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>//*[@id="top_menu"]/nav/ul/li[1]/a</t>
+  </si>
+  <si>
+    <t>Empresas</t>
+  </si>
+  <si>
+    <t>//*[@id="top_menu"]/nav/ul/li[2]/a</t>
+  </si>
+  <si>
+    <t>DescubreloYa</t>
+  </si>
+  <si>
+    <t>//*[@id="main-content"]/div[2]/div[1]/div/div/div/section/div/div/a</t>
+  </si>
+  <si>
+    <t>IngresaMiCuentaTigo</t>
+  </si>
+  <si>
+    <t>idEmail</t>
+  </si>
+  <si>
+    <t>ValidarCorreo</t>
+  </si>
+  <si>
+    <t>continueBtn</t>
+  </si>
+  <si>
+    <t>CrearTuCuenta</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/div[3]/div/p[2]/a</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Continuar</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[3]/button</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[4]/a</t>
+  </si>
+  <si>
+    <t>NumeroPlan</t>
+  </si>
+  <si>
+    <t>//*[@id="block-accountsblock-2"]/div/div/div/div/div/span</t>
+  </si>
+  <si>
+    <t>Resumen</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/div[2]/div/div/nav/div/div/ul/li[1]/a</t>
+  </si>
+  <si>
+    <t>CambiateYa</t>
+  </si>
+  <si>
+    <t>//*[@id="action_Cámbiate ya"]</t>
+  </si>
+  <si>
+    <t>CrearTuCuentaTigo</t>
+  </si>
+  <si>
+    <t>ConMiCorreo</t>
+  </si>
+  <si>
+    <t>//*[@id="addNew"]</t>
+  </si>
+  <si>
+    <t>ConFacebook</t>
+  </si>
+  <si>
+    <t>//*[@id="SLFacebook"]</t>
+  </si>
+  <si>
+    <t>ConGoogle</t>
+  </si>
+  <si>
+    <t>//*[@id="SLGoogle"]</t>
+  </si>
+  <si>
+    <t>IngresaAMiCuenta</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/div[1]/h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlvidasteContrasena </t>
+  </si>
+  <si>
+    <t>PQRUne</t>
+  </si>
+  <si>
+    <t>/html/body/div[4]/div/div/div/div[1]/h3</t>
+  </si>
+  <si>
+    <t>PQRTigo</t>
+  </si>
+  <si>
+    <t>//*[@id='formInicioPqr:panelBotonesInicio']/thead/tr/th/span</t>
+  </si>
+  <si>
+    <t>Sic</t>
+  </si>
+  <si>
+    <t>//*[@id=\'contenido_medio\']/div[1]/h1</t>
+  </si>
+  <si>
+    <t>PQR Tigo</t>
+  </si>
+  <si>
+    <t>PQR Une</t>
+  </si>
+  <si>
+    <t>Tiendas</t>
+  </si>
+  <si>
+    <t>/html/body/content/div[2]/div/section[1]/div/div/h3</t>
+  </si>
+  <si>
+    <t>VisitasPendientes</t>
+  </si>
+  <si>
+    <t>//*[@id=\'schedule-visits-container\']/div[2]/div[1]/div/p</t>
+  </si>
+  <si>
+    <t>MsgErrorDocumento</t>
+  </si>
+  <si>
+    <t>Listado de Objetos en el proceso Recargas y Paquetes</t>
+  </si>
+  <si>
+    <t>Recargas</t>
+  </si>
+  <si>
+    <t>Recarga</t>
+  </si>
+  <si>
+    <t>//*[@id="tap_selector"]/div[2]</t>
+  </si>
+  <si>
+    <t>TuLineaTigoR</t>
+  </si>
+  <si>
+    <t>//*[@id="num_lin"]</t>
+  </si>
+  <si>
+    <t>Valor3Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[1]</t>
+  </si>
+  <si>
+    <t>Valor6Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[2]</t>
+  </si>
+  <si>
+    <t>Valor15Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[3]</t>
+  </si>
+  <si>
+    <t>Valor 20Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[4]</t>
+  </si>
+  <si>
+    <t>Valor30Mil</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[5]</t>
+  </si>
+  <si>
+    <t>OtroValor</t>
+  </si>
+  <si>
+    <t>//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[6]</t>
+  </si>
+  <si>
+    <t>ValorRecargar</t>
+  </si>
+  <si>
+    <t>edit-otro-valor</t>
+  </si>
+  <si>
+    <t>ErrorValor</t>
+  </si>
+  <si>
+    <t>//*[@id="other_value"]/div/div/div[1]/p</t>
+  </si>
+  <si>
+    <t>Recargar</t>
+  </si>
+  <si>
+    <t>edit-button-recargar</t>
+  </si>
+  <si>
+    <t>ResumenTransaccion</t>
+  </si>
+  <si>
+    <t>//*[@id="title-detail"]</t>
+  </si>
+  <si>
+    <t>NumeroDelProducto</t>
+  </si>
+  <si>
+    <t>product-number</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -997,7 +1332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1088,8 +1423,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1235,12 +1588,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1569,10 +1937,43 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1580,12 +1981,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1627,7 +2031,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1660,9 +2064,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1695,6 +2116,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1870,14 +2308,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -1932,7 +2370,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>194</v>
       </c>
@@ -2240,14 +2678,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" style="39" customWidth="1"/>
     <col min="2" max="2" width="45" style="39" bestFit="1" customWidth="1"/>
@@ -3413,7 +3851,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>26</v>
       </c>
@@ -4519,7 +4957,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I75"/>
+  <autoFilter ref="A2:I75" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
@@ -4528,21 +4966,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F10" sqref="F10:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5942,14 +6380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" hidden="1" customWidth="1"/>
@@ -6073,19 +6511,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" style="39" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="39" customWidth="1"/>
-    <col min="4" max="5" width="61" style="39" customWidth="1"/>
+    <col min="4" max="4" width="61" style="39" customWidth="1"/>
+    <col min="5" max="5" width="135.42578125" style="39" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="39"/>
   </cols>
@@ -7517,8 +7956,2068 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D77"/>
+  <autoFilter ref="A2:D77" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDA504D-8FF2-405F-AE1B-22086E468A89}">
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" customWidth="1"/>
+    <col min="5" max="5" width="101.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>310</v>
+      </c>
+      <c r="E3" s="48" t="str">
+        <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
+        <v>public By btnIngresarAMiCuenta=By.xpath("//*[@id="top_menu_aside"]/nav/ul/li/a");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>312</v>
+      </c>
+      <c r="E4" s="48" t="str">
+        <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
+        <v>public By btnIniciarSesion=By.xpath("//*[@id="top_menu_aside"]/nav/ul/li/ul/li/a");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>314</v>
+      </c>
+      <c r="E5" s="48" t="str">
+        <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
+        <v>public By btnRegistrarme=By.xpath("//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[1]");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>316</v>
+      </c>
+      <c r="E6" s="48" t="str">
+        <f t="shared" ref="E6:E41" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <v>public By btnIngresar=By.xpath("//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[2]");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="E7" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagaTusFacturas=By.xpath("//*[@id="main-content"]/div[2]/div[3]/div/div/div/div/a");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnRecargasYPaquetes=By.xpath("//*[@id="main-content"]/div[2]/div[4]/div/div/div/div/a");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>322</v>
+      </c>
+      <c r="E9" s="91" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnRegistraTuEquipo=By.xpath("//*[@id="main-content"]/div[2]/div[5]/div/div/div/div/a");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B10" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="122" t="s">
+        <v>323</v>
+      </c>
+      <c r="D10" s="122" t="s">
+        <v>324</v>
+      </c>
+      <c r="E10" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnReponeTuSim=By.xpath("//*[@id="main-content"]/div[2]/div[6]/div/div/div/div/a");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B11" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="122" t="s">
+        <v>325</v>
+      </c>
+      <c r="D11" s="122" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCambiarMiClave=By.xpath("//*[@id="main-content"]/div[2]/div[7]/div/div/div/div/div[2]/a");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B12" s="122" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="122" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="122" t="s">
+        <v>327</v>
+      </c>
+      <c r="E12" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipo=By.xpath("//*[@id="t_document"]/div/div/input");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="122" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="122" t="s">
+        <v>328</v>
+      </c>
+      <c r="E13" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumeroDocumento=By.xpath("//*[@id="document"]");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B14" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="122" t="s">
+        <v>386</v>
+      </c>
+      <c r="D14" s="122" t="s">
+        <v>329</v>
+      </c>
+      <c r="E14" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMsgErrorDocumento=By.xpath("//*[@id="query-container"]/section/div[1]/span[2]");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="122" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="122" t="s">
+        <v>330</v>
+      </c>
+      <c r="E15" s="122" t="str">
+        <f t="shared" ref="E15" si="1">CONCATENATE("public By ",B15,C15,"=By.",IF(ISNUMBER(SEARCH("@id=",D15)),"xpath(""","id("""),D15,""");")</f>
+        <v>public By btnConsultar=By.xpath("//*[@id="findagenda"]/div[2]/div[2]");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="122" t="s">
+        <v>384</v>
+      </c>
+      <c r="D16" s="122" t="s">
+        <v>385</v>
+      </c>
+      <c r="E16" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbVisitasPendientes=By.xpath("//*[@id=\'schedule-visits-container\']/div[2]/div[1]/div/p");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" s="122" t="s">
+        <v>331</v>
+      </c>
+      <c r="D17" s="122" t="s">
+        <v>332</v>
+      </c>
+      <c r="E17" s="122" t="str">
+        <f t="shared" ref="E17" si="2">CONCATENATE("public By ",B17,C17,"=By.",IF(ISNUMBER(SEARCH("@id=",D17)),"xpath(""","id("""),D17,""");")</f>
+        <v>public By txtConsultaPQRUne=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[1]/p/a");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="B18" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="122" t="s">
+        <v>374</v>
+      </c>
+      <c r="D18" s="122" t="s">
+        <v>375</v>
+      </c>
+      <c r="E18" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbPQRUne=By.id("/html/body/div[4]/div/div/div/div[1]/h3");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B19" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C19" s="122" t="s">
+        <v>333</v>
+      </c>
+      <c r="D19" s="122" t="s">
+        <v>334</v>
+      </c>
+      <c r="E19" s="122" t="str">
+        <f t="shared" ref="E19" si="3">CONCATENATE("public By ",B19,C19,"=By.",IF(ISNUMBER(SEARCH("@id=",D19)),"xpath(""","id("""),D19,""");")</f>
+        <v>public By txtConsultaPQRTigo=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[2]/p/a");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="B20" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="122" t="s">
+        <v>376</v>
+      </c>
+      <c r="D20" s="122" t="s">
+        <v>377</v>
+      </c>
+      <c r="E20" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbPQRTigo=By.xpath("//*[@id='formInicioPqr:panelBotonesInicio']/thead/tr/th/span");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B21" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C21" s="122" t="s">
+        <v>335</v>
+      </c>
+      <c r="D21" s="122" t="s">
+        <v>336</v>
+      </c>
+      <c r="E21" s="122" t="str">
+        <f t="shared" ref="E21" si="4">CONCATENATE("public By ",B21,C21,"=By.",IF(ISNUMBER(SEARCH("@id=",D21)),"xpath(""","id("""),D21,""");")</f>
+        <v>public By txtConsultaSic=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[3]/p/a");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="B22" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="122" t="s">
+        <v>378</v>
+      </c>
+      <c r="D22" s="122" t="s">
+        <v>379</v>
+      </c>
+      <c r="E22" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbSic=By.xpath("//*[@id=\'contenido_medio\']/div[1]/h1");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B23" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C23" s="122" t="s">
+        <v>337</v>
+      </c>
+      <c r="D23" s="122" t="s">
+        <v>338</v>
+      </c>
+      <c r="E23" s="122" t="str">
+        <f t="shared" ref="E23" si="5">CONCATENATE("public By ",B23,C23,"=By.",IF(ISNUMBER(SEARCH("@id=",D23)),"xpath(""","id("""),D23,""");")</f>
+        <v>public By txtConoceNuestrasTiendas=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[4]/p/a");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="B24" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C24" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="D24" s="122" t="s">
+        <v>383</v>
+      </c>
+      <c r="E24" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbTiendas=By.id("/html/body/content/div[2]/div/section[1]/div/div/h3");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B25" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="122" t="s">
+        <v>339</v>
+      </c>
+      <c r="D25" s="122" t="s">
+        <v>340</v>
+      </c>
+      <c r="E25" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnChatYAyuda=By.xpath("//*[@id="Embed"]/button/span[2]");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B26" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="122" t="s">
+        <v>341</v>
+      </c>
+      <c r="D26" s="122" t="s">
+        <v>342</v>
+      </c>
+      <c r="E26" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtPersonas=By.xpath("//*[@id="top_menu"]/nav/ul/li[1]/a");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B27" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C27" s="122" t="s">
+        <v>343</v>
+      </c>
+      <c r="D27" s="122" t="s">
+        <v>344</v>
+      </c>
+      <c r="E27" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtEmpresas=By.xpath("//*[@id="top_menu"]/nav/ul/li[2]/a");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B28" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="122" t="s">
+        <v>345</v>
+      </c>
+      <c r="D28" s="122" t="s">
+        <v>346</v>
+      </c>
+      <c r="E28" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnDescubreloYa=By.xpath("//*[@id="main-content"]/div[2]/div[1]/div/div/div/section/div/div/a");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B29" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="124" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" s="124" t="s">
+        <v>348</v>
+      </c>
+      <c r="E29" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.id("idEmail");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B30" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="124" t="s">
+        <v>349</v>
+      </c>
+      <c r="D30" s="124" t="s">
+        <v>350</v>
+      </c>
+      <c r="E30" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnValidarCorreo=By.id("continueBtn");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B31" s="124" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="124" t="s">
+        <v>371</v>
+      </c>
+      <c r="D31" s="124" t="s">
+        <v>372</v>
+      </c>
+      <c r="E31" s="124" t="str">
+        <f t="shared" ref="E31" si="6">CONCATENATE("public By ",B31,C31,"=By.",IF(ISNUMBER(SEARCH("@id=",D31)),"xpath(""","id("""),D31,""");")</f>
+        <v>public By lbIngresaAMiCuenta=By.id("/html/body/div[2]/div/div[1]/h5");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B32" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C32" s="124" t="s">
+        <v>351</v>
+      </c>
+      <c r="D32" s="124" t="s">
+        <v>352</v>
+      </c>
+      <c r="E32" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCrearTuCuenta=By.id("/html/body/div[2]/div/div[3]/div/p[2]/a");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B33" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C33" s="124" t="s">
+        <v>353</v>
+      </c>
+      <c r="D33" s="124" t="s">
+        <v>354</v>
+      </c>
+      <c r="E33" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtContraseña=By.id("password");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B34" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="124" t="s">
+        <v>355</v>
+      </c>
+      <c r="D34" s="124" t="s">
+        <v>356</v>
+      </c>
+      <c r="E34" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnContinuar=By.id("/html/body/div[2]/div/form/div[3]/button");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B35" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C35" s="124" t="s">
+        <v>373</v>
+      </c>
+      <c r="D35" s="124" t="s">
+        <v>357</v>
+      </c>
+      <c r="E35" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtOlvidasteContrasena =By.id("/html/body/div[2]/div/form/div[4]/a");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B36" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="124" t="s">
+        <v>358</v>
+      </c>
+      <c r="D36" s="124" t="s">
+        <v>359</v>
+      </c>
+      <c r="E36" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listNumeroPlan=By.xpath("//*[@id="block-accountsblock-2"]/div/div/div/div/div/span");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B37" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="124" t="s">
+        <v>360</v>
+      </c>
+      <c r="D37" s="124" t="s">
+        <v>361</v>
+      </c>
+      <c r="E37" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtResumen=By.id("/html/body/div[3]/div[2]/div/div/nav/div/div/ul/li[1]/a");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="B38" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="124" t="s">
+        <v>362</v>
+      </c>
+      <c r="D38" s="124" t="s">
+        <v>363</v>
+      </c>
+      <c r="E38" s="124" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCambiateYa=By.xpath("//*[@id="action_Cámbiate ya"]");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="125" t="s">
+        <v>364</v>
+      </c>
+      <c r="B39" s="126" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="126" t="s">
+        <v>365</v>
+      </c>
+      <c r="D39" s="126" t="s">
+        <v>366</v>
+      </c>
+      <c r="E39" s="126" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnConMiCorreo=By.xpath("//*[@id="addNew"]");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="125" t="s">
+        <v>364</v>
+      </c>
+      <c r="B40" s="126" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" s="126" t="s">
+        <v>367</v>
+      </c>
+      <c r="D40" s="126" t="s">
+        <v>368</v>
+      </c>
+      <c r="E40" s="126" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnConFacebook=By.xpath("//*[@id="SLFacebook"]");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="127" t="s">
+        <v>364</v>
+      </c>
+      <c r="B41" s="128" t="s">
+        <v>232</v>
+      </c>
+      <c r="C41" s="128" t="s">
+        <v>369</v>
+      </c>
+      <c r="D41" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="E41" s="128" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnConGoogle=By.xpath("//*[@id="SLGoogle"]");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E972679-EDA2-4ED9-97F5-E044AE9E5203}">
+  <dimension ref="A1:E72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="110.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>389</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="E3" s="48" t="str">
+        <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
+        <v>public By btnRecarga=By.xpath("//*[@id="tap_selector"]/div[2]");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>392</v>
+      </c>
+      <c r="E4" s="48" t="str">
+        <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
+        <v>public By txtTuLineaTigoR=By.xpath("//*[@id="num_lin"]");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>393</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>394</v>
+      </c>
+      <c r="E5" s="48" t="str">
+        <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
+        <v>public By btnValor3Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[1]");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>396</v>
+      </c>
+      <c r="E6" s="48" t="str">
+        <f t="shared" ref="E6:E69" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <v>public By btnValor6Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[2]");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="E7" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnValor15Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[3]");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>399</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="E8" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnValor 20Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[4]");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>401</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>402</v>
+      </c>
+      <c r="E9" s="91" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnValor30Mil=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[5]");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B10" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="122" t="s">
+        <v>403</v>
+      </c>
+      <c r="D10" s="122" t="s">
+        <v>404</v>
+      </c>
+      <c r="E10" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnOtroValor=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[6]");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B11" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="122" t="s">
+        <v>405</v>
+      </c>
+      <c r="D11" s="122" t="s">
+        <v>406</v>
+      </c>
+      <c r="E11" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtValorRecargar=By.id("edit-otro-valor");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B12" s="122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" s="122" t="s">
+        <v>407</v>
+      </c>
+      <c r="D12" s="122" t="s">
+        <v>408</v>
+      </c>
+      <c r="E12" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbErrorValor=By.xpath("//*[@id="other_value"]/div/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B13" s="122" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="122" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.id("edit-email");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B14" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="122" t="s">
+        <v>409</v>
+      </c>
+      <c r="D14" s="122" t="s">
+        <v>410</v>
+      </c>
+      <c r="E14" s="122" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnRecargar=By.id("edit-button-recargar");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="130" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="D15" s="130" t="s">
+        <v>412</v>
+      </c>
+      <c r="E15" s="130" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbResumenTransaccion=By.xpath("//*[@id="title-detail"]");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="130" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="130" t="s">
+        <v>413</v>
+      </c>
+      <c r="D16" s="130" t="s">
+        <v>414</v>
+      </c>
+      <c r="E16" s="130" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNumeroDelProducto=By.id("product-number");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="131" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="132" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="132" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E17" s="132" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbValorPagar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTarjetaCredito=By.id("payment-method-type-label-credit-payu");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkDebitoBancarioPSE=By.id("payment-method-type-label-debit-payu");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkOtrosmediosdepago=By.id("payment-method-type-label-others-pay-methods");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCVV/CVC=By.id("edit-cvc");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listCuotas=By.id("edit-cardnumber-quota");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNombre=By.id("edit-ccname");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipo=By.id("edit-buyer-document-type");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("edit-cancel");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listBanco=By.id("edit-bank");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipodepersona=By.id("edit-buyer-type-person");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNombresyapellidos=By.id("edit-buyer-name");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By listTipo=By.id("edit-buyer-document-type--2");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="E45" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="D47" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="E47" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="D48" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="E48" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a");</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="C49" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("edit-cancel--2");</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="C50" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="D50" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2");</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By txtNumeroNequi(Cargaunvalorpordefecto)=By.id("edit-nequi-account");</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="E52" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--3']/div/a");</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel");</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPagar=By.id("tigoune-nequi-button-submit");</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbMensajedePagorealizado=By.id("gateway-content-alert-message");</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C56" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbValor=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[1]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>266</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E57" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNumeroCelular=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[2]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C58" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="E58" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNºtransaccion=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[3]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C59" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="D59" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E59" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbFechadepago=By.xpath("//*[@id='details-transaction']/div[2]/div[1]/div[4]/div/table/tbody/tr[2]/td/div");</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C60" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D60" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbEstado=By.xpath("//*[@id='details-transaction']/div[2]/div[2]/div/text()");</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="D61" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="E61" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbCodigo=By.id("transaction-description-error");</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="E62" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbCorreo=By.xpath("//*[@id='details-transaction']/div[2]/div[3]/div");</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="D63" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="E63" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbID.Transaccion=By.xpath("//*[@id='details_pse']/div/div[1]/span[2]");</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C64" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="D64" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="E64" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbEmpresa=By.xpath("//*[@id='details_pse']/div/div[2]/span[2]");</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C65" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="E65" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNIT=By.xpath("//*[@id='details_pse']/div/div[3]/span[2]");</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C66" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="E66" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbDireccion=By.xpath("//*[@id='details_pse']/div/div[4]/span[2]");</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="C67" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="D67" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="E67" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By linkDescargarComprobante=By.xpath("//*[@id='details-transaction']/div[3]/div[3]/a");</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D68" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="E68" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnVolveralinicio=By.xpath("//*[@id='details-transaction']/div[5]/a[1]/button");</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C69" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E69" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnPAGAROTRAFACTURA=By.xpath("//*[@id='details-transaction']/div[5]/a[2]/button");</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B70" s="56" t="s">
+        <v>235</v>
+      </c>
+      <c r="C70" s="56" t="s">
+        <v>211</v>
+      </c>
+      <c r="D70" s="56" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" s="56" t="str">
+        <f t="shared" ref="E70:E72" si="1">CONCATENATE("public By ",B70,C70,"=By.",IF(ISNUMBER(SEARCH("@id=",D70)),"xpath(""","id("""),D70,""");")</f>
+        <v>public By txtE-mail=By.id("PNEMail");</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B71" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="C71" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D71" s="56" t="s">
+        <v>296</v>
+      </c>
+      <c r="E71" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnIralBanco=By.id("btnSeguir");</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B72" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="C72" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="D72" s="56" t="s">
+        <v>297</v>
+      </c>
+      <c r="E72" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnRegresaralcomercio=By.id("btnCancel");</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se añaden campos de Mi Cuenta a el archivo de Mapeo
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasprilla\Documents\automatizacion_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B91DB4-8B3F-401D-87B1-5470BFBB51A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391733F1-CCED-4BE4-BD82-A9A8811F524B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="434">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -1282,6 +1282,60 @@
   </si>
   <si>
     <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]</t>
+  </si>
+  <si>
+    <t>LineaPruebasJuanca</t>
+  </si>
+  <si>
+    <t>(((//*[@id='lines'])//a[contains(@href,'')]))[11]</t>
+  </si>
+  <si>
+    <t>LineaHibridoMariana</t>
+  </si>
+  <si>
+    <t>(((((//*[@id='lines'])//a[contains(@href,'')])))//*[contains(text(),'Mariana')])[2]</t>
+  </si>
+  <si>
+    <t>LineaHibridoAna</t>
+  </si>
+  <si>
+    <t>(((//*[@id='lines'])//a[contains(@href,'')]))[9]</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>//*[@id='top_menu_aside']/nav/ul/li/a</t>
+  </si>
+  <si>
+    <t>CerrarSesion</t>
+  </si>
+  <si>
+    <t>//*[@id='top_menu_aside']/nav/ul/li/ul/li[2]/a</t>
+  </si>
+  <si>
+    <t>CambiarCuenta</t>
+  </si>
+  <si>
+    <t>//*[@id='addNew']</t>
+  </si>
+  <si>
+    <t>Planes</t>
+  </si>
+  <si>
+    <t>//*[@id='main-content']/div[2]</t>
+  </si>
+  <si>
+    <t>MejorarPlan</t>
+  </si>
+  <si>
+    <t>//*[@id='compras-noplan-container']/h3</t>
+  </si>
+  <si>
+    <t>DetallePlan</t>
+  </si>
+  <si>
+    <t>//*[@id='compras-noplan-container']/p</t>
   </si>
 </sst>
 </file>
@@ -1850,6 +1904,39 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1936,39 +2023,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2596,78 +2650,78 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="104" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="93"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="93"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="93"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="93"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="93"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="93"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
+      <c r="A20" s="104"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="93"/>
-      <c r="B21" s="93"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2700,17 +2754,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -4985,14 +5039,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5015,7 +5069,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="118" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -5035,7 +5089,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="108"/>
+      <c r="A4" s="119"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -5053,7 +5107,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="108"/>
+      <c r="A5" s="119"/>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -5071,7 +5125,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
+      <c r="A6" s="119"/>
       <c r="B6" s="3" t="s">
         <v>101</v>
       </c>
@@ -5089,7 +5143,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="108"/>
+      <c r="A7" s="119"/>
       <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
@@ -5110,7 +5164,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="108"/>
+      <c r="A8" s="119"/>
       <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
@@ -5131,7 +5185,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="109"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="3" t="s">
         <v>229</v>
       </c>
@@ -5149,7 +5203,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="127" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -5169,7 +5223,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="117"/>
+      <c r="A11" s="128"/>
       <c r="B11" s="7" t="s">
         <v>124</v>
       </c>
@@ -5190,7 +5244,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="117"/>
+      <c r="A12" s="128"/>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -5208,7 +5262,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="117"/>
+      <c r="A13" s="128"/>
       <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
@@ -5229,7 +5283,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
+      <c r="A14" s="128"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -5247,7 +5301,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+      <c r="A15" s="128"/>
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -5265,7 +5319,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="117"/>
+      <c r="A16" s="128"/>
       <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
@@ -5283,7 +5337,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="117"/>
+      <c r="A17" s="128"/>
       <c r="B17" s="7" t="s">
         <v>101</v>
       </c>
@@ -5301,7 +5355,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="117"/>
+      <c r="A18" s="128"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -5319,7 +5373,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
+      <c r="A19" s="129"/>
       <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
@@ -5337,7 +5391,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="101" t="s">
+      <c r="A20" s="112" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -5357,7 +5411,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="102"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="4" t="s">
         <v>81</v>
       </c>
@@ -5382,7 +5436,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="102"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
@@ -5400,7 +5454,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="102"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="4" t="s">
         <v>82</v>
       </c>
@@ -5418,7 +5472,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
+      <c r="A24" s="114"/>
       <c r="B24" s="4" t="s">
         <v>83</v>
       </c>
@@ -5443,7 +5497,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="104" t="s">
+      <c r="A25" s="115" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -5463,7 +5517,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="105"/>
+      <c r="A26" s="116"/>
       <c r="B26" s="13" t="s">
         <v>27</v>
       </c>
@@ -5481,7 +5535,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="106"/>
+      <c r="A27" s="117"/>
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -5499,7 +5553,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="130" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5519,7 +5573,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="120"/>
+      <c r="A29" s="131"/>
       <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
@@ -5540,7 +5594,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="120"/>
+      <c r="A30" s="131"/>
       <c r="B30" s="15" t="s">
         <v>118</v>
       </c>
@@ -5561,7 +5615,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="120"/>
+      <c r="A31" s="131"/>
       <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
@@ -5579,7 +5633,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="120"/>
+      <c r="A32" s="131"/>
       <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
@@ -5597,7 +5651,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="120"/>
+      <c r="A33" s="131"/>
       <c r="B33" s="15" t="s">
         <v>35</v>
       </c>
@@ -5615,7 +5669,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="120"/>
+      <c r="A34" s="131"/>
       <c r="B34" s="15" t="s">
         <v>36</v>
       </c>
@@ -5633,7 +5687,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="120"/>
+      <c r="A35" s="131"/>
       <c r="B35" s="15" t="s">
         <v>39</v>
       </c>
@@ -5651,7 +5705,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="120"/>
+      <c r="A36" s="131"/>
       <c r="B36" s="15" t="s">
         <v>3</v>
       </c>
@@ -5669,7 +5723,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="120"/>
+      <c r="A37" s="131"/>
       <c r="B37" s="15" t="s">
         <v>42</v>
       </c>
@@ -5687,7 +5741,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="120"/>
+      <c r="A38" s="131"/>
       <c r="B38" s="15" t="s">
         <v>122</v>
       </c>
@@ -5708,7 +5762,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="120"/>
+      <c r="A39" s="131"/>
       <c r="B39" s="15" t="s">
         <v>44</v>
       </c>
@@ -5726,7 +5780,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="120"/>
+      <c r="A40" s="131"/>
       <c r="B40" s="15" t="s">
         <v>130</v>
       </c>
@@ -5747,7 +5801,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="120"/>
+      <c r="A41" s="131"/>
       <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
@@ -5765,7 +5819,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="120"/>
+      <c r="A42" s="131"/>
       <c r="B42" s="15" t="s">
         <v>110</v>
       </c>
@@ -5786,7 +5840,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="120"/>
+      <c r="A43" s="131"/>
       <c r="B43" s="15" t="s">
         <v>47</v>
       </c>
@@ -5802,7 +5856,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="120"/>
+      <c r="A44" s="131"/>
       <c r="B44" s="15" t="s">
         <v>101</v>
       </c>
@@ -5818,7 +5872,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="120"/>
+      <c r="A45" s="131"/>
       <c r="B45" s="15" t="s">
         <v>22</v>
       </c>
@@ -5836,7 +5890,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="121"/>
+      <c r="A46" s="132"/>
       <c r="B46" s="15" t="s">
         <v>51</v>
       </c>
@@ -5854,7 +5908,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="110" t="s">
+      <c r="A47" s="121" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -5874,7 +5928,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="111"/>
+      <c r="A48" s="122"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -5892,7 +5946,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="111"/>
+      <c r="A49" s="122"/>
       <c r="B49" s="5" t="s">
         <v>56</v>
       </c>
@@ -5910,7 +5964,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="111"/>
+      <c r="A50" s="122"/>
       <c r="B50" s="5" t="s">
         <v>3</v>
       </c>
@@ -5928,7 +5982,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="111"/>
+      <c r="A51" s="122"/>
       <c r="B51" s="5" t="s">
         <v>60</v>
       </c>
@@ -5946,7 +6000,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="111"/>
+      <c r="A52" s="122"/>
       <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
@@ -5964,7 +6018,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="111"/>
+      <c r="A53" s="122"/>
       <c r="B53" s="5" t="s">
         <v>101</v>
       </c>
@@ -5980,7 +6034,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="111"/>
+      <c r="A54" s="122"/>
       <c r="B54" s="5" t="s">
         <v>22</v>
       </c>
@@ -5998,7 +6052,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="112"/>
+      <c r="A55" s="123"/>
       <c r="B55" s="5" t="s">
         <v>64</v>
       </c>
@@ -6016,7 +6070,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="113" t="s">
+      <c r="A56" s="124" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -6036,7 +6090,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="114"/>
+      <c r="A57" s="125"/>
       <c r="B57" s="1" t="s">
         <v>101</v>
       </c>
@@ -6052,7 +6106,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="114"/>
+      <c r="A58" s="125"/>
       <c r="B58" s="1" t="s">
         <v>22</v>
       </c>
@@ -6070,7 +6124,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="115"/>
+      <c r="A59" s="126"/>
       <c r="B59" s="1" t="s">
         <v>48</v>
       </c>
@@ -6088,7 +6142,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="96" t="s">
+      <c r="A60" s="107" t="s">
         <v>136</v>
       </c>
       <c r="B60" s="23" t="s">
@@ -6111,7 +6165,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="97"/>
+      <c r="A61" s="108"/>
       <c r="B61" s="23" t="s">
         <v>137</v>
       </c>
@@ -6129,7 +6183,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="97"/>
+      <c r="A62" s="108"/>
       <c r="B62" s="23" t="s">
         <v>138</v>
       </c>
@@ -6147,7 +6201,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="97"/>
+      <c r="A63" s="108"/>
       <c r="B63" s="23" t="s">
         <v>139</v>
       </c>
@@ -6165,7 +6219,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="97"/>
+      <c r="A64" s="108"/>
       <c r="B64" s="23" t="s">
         <v>140</v>
       </c>
@@ -6183,7 +6237,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="97"/>
+      <c r="A65" s="108"/>
       <c r="B65" s="23" t="s">
         <v>141</v>
       </c>
@@ -6201,7 +6255,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="97"/>
+      <c r="A66" s="108"/>
       <c r="B66" s="23" t="s">
         <v>142</v>
       </c>
@@ -6219,7 +6273,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="97"/>
+      <c r="A67" s="108"/>
       <c r="B67" s="23" t="s">
         <v>143</v>
       </c>
@@ -6237,7 +6291,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="97"/>
+      <c r="A68" s="108"/>
       <c r="B68" s="23" t="s">
         <v>144</v>
       </c>
@@ -6255,7 +6309,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="97"/>
+      <c r="A69" s="108"/>
       <c r="B69" s="23" t="s">
         <v>145</v>
       </c>
@@ -6273,7 +6327,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="97"/>
+      <c r="A70" s="108"/>
       <c r="B70" s="23" t="s">
         <v>146</v>
       </c>
@@ -6291,7 +6345,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="97"/>
+      <c r="A71" s="108"/>
       <c r="B71" s="23" t="s">
         <v>147</v>
       </c>
@@ -6309,7 +6363,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="97"/>
+      <c r="A72" s="108"/>
       <c r="B72" s="23" t="s">
         <v>148</v>
       </c>
@@ -6327,7 +6381,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="97"/>
+      <c r="A73" s="108"/>
       <c r="B73" s="23" t="s">
         <v>149</v>
       </c>
@@ -6345,7 +6399,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="98"/>
+      <c r="A74" s="109"/>
       <c r="B74" s="23" t="s">
         <v>150</v>
       </c>
@@ -7964,10 +8018,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDA504D-8FF2-405F-AE1B-22086E468A89}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7976,7 +8030,7 @@
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="75.42578125" customWidth="1"/>
-    <col min="5" max="5" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="114.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8073,7 +8127,7 @@
         <v>316</v>
       </c>
       <c r="E6" s="48" t="str">
-        <f t="shared" ref="E6:E41" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <f t="shared" ref="E6:E50" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
         <v>public By btnIngresar=By.xpath("//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[2]");</v>
       </c>
     </row>
@@ -8135,16 +8189,16 @@
       <c r="A10" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="93" t="s">
         <v>323</v>
       </c>
-      <c r="D10" s="122" t="s">
+      <c r="D10" s="93" t="s">
         <v>324</v>
       </c>
-      <c r="E10" s="122" t="str">
+      <c r="E10" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnReponeTuSim=By.xpath("//*[@id="main-content"]/div[2]/div[6]/div/div/div/div/a");</v>
       </c>
@@ -8153,16 +8207,16 @@
       <c r="A11" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="93" t="s">
         <v>325</v>
       </c>
-      <c r="D11" s="122" t="s">
+      <c r="D11" s="93" t="s">
         <v>326</v>
       </c>
-      <c r="E11" s="122" t="str">
+      <c r="E11" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCambiarMiClave=By.xpath("//*[@id="main-content"]/div[2]/div[7]/div/div/div/div/div[2]/a");</v>
       </c>
@@ -8171,16 +8225,16 @@
       <c r="A12" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="93" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="122" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="122" t="s">
+      <c r="C12" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="93" t="s">
         <v>327</v>
       </c>
-      <c r="E12" s="122" t="str">
+      <c r="E12" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By listTipo=By.xpath("//*[@id="t_document"]/div/div/input");</v>
       </c>
@@ -8189,16 +8243,16 @@
       <c r="A13" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="93" t="s">
         <v>276</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="93" t="s">
         <v>328</v>
       </c>
-      <c r="E13" s="122" t="str">
+      <c r="E13" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtNumeroDocumento=By.xpath("//*[@id="document"]");</v>
       </c>
@@ -8207,16 +8261,16 @@
       <c r="A14" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B14" s="122" t="s">
+      <c r="B14" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="93" t="s">
         <v>386</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="D14" s="93" t="s">
         <v>329</v>
       </c>
-      <c r="E14" s="122" t="str">
+      <c r="E14" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbMsgErrorDocumento=By.xpath("//*[@id="query-container"]/section/div[1]/span[2]");</v>
       </c>
@@ -8225,16 +8279,16 @@
       <c r="A15" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C15" s="122" t="s">
+      <c r="C15" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="122" t="s">
+      <c r="D15" s="93" t="s">
         <v>330</v>
       </c>
-      <c r="E15" s="122" t="str">
+      <c r="E15" s="93" t="str">
         <f t="shared" ref="E15" si="1">CONCATENATE("public By ",B15,C15,"=By.",IF(ISNUMBER(SEARCH("@id=",D15)),"xpath(""","id("""),D15,""");")</f>
         <v>public By btnConsultar=By.xpath("//*[@id="findagenda"]/div[2]/div[2]");</v>
       </c>
@@ -8243,16 +8297,16 @@
       <c r="A16" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B16" s="122" t="s">
+      <c r="B16" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="122" t="s">
+      <c r="C16" s="93" t="s">
         <v>384</v>
       </c>
-      <c r="D16" s="122" t="s">
+      <c r="D16" s="93" t="s">
         <v>385</v>
       </c>
-      <c r="E16" s="122" t="str">
+      <c r="E16" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbVisitasPendientes=By.xpath("//*[@id=\'schedule-visits-container\']/div[2]/div[1]/div/p");</v>
       </c>
@@ -8261,16 +8315,16 @@
       <c r="A17" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B17" s="122" t="s">
+      <c r="B17" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C17" s="122" t="s">
+      <c r="C17" s="93" t="s">
         <v>331</v>
       </c>
-      <c r="D17" s="122" t="s">
+      <c r="D17" s="93" t="s">
         <v>332</v>
       </c>
-      <c r="E17" s="122" t="str">
+      <c r="E17" s="93" t="str">
         <f t="shared" ref="E17" si="2">CONCATENATE("public By ",B17,C17,"=By.",IF(ISNUMBER(SEARCH("@id=",D17)),"xpath(""","id("""),D17,""");")</f>
         <v>public By txtConsultaPQRUne=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[1]/p/a");</v>
       </c>
@@ -8279,16 +8333,16 @@
       <c r="A18" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="93" t="s">
         <v>374</v>
       </c>
-      <c r="D18" s="122" t="s">
+      <c r="D18" s="93" t="s">
         <v>375</v>
       </c>
-      <c r="E18" s="122" t="str">
+      <c r="E18" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbPQRUne=By.id("/html/body/div[4]/div/div/div/div[1]/h3");</v>
       </c>
@@ -8297,16 +8351,16 @@
       <c r="A19" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="93" t="s">
         <v>333</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="93" t="s">
         <v>334</v>
       </c>
-      <c r="E19" s="122" t="str">
+      <c r="E19" s="93" t="str">
         <f t="shared" ref="E19" si="3">CONCATENATE("public By ",B19,C19,"=By.",IF(ISNUMBER(SEARCH("@id=",D19)),"xpath(""","id("""),D19,""");")</f>
         <v>public By txtConsultaPQRTigo=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[2]/p/a");</v>
       </c>
@@ -8315,16 +8369,16 @@
       <c r="A20" s="26" t="s">
         <v>380</v>
       </c>
-      <c r="B20" s="122" t="s">
+      <c r="B20" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C20" s="122" t="s">
+      <c r="C20" s="93" t="s">
         <v>376</v>
       </c>
-      <c r="D20" s="122" t="s">
+      <c r="D20" s="93" t="s">
         <v>377</v>
       </c>
-      <c r="E20" s="122" t="str">
+      <c r="E20" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbPQRTigo=By.xpath("//*[@id='formInicioPqr:panelBotonesInicio']/thead/tr/th/span");</v>
       </c>
@@ -8333,16 +8387,16 @@
       <c r="A21" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="122" t="s">
+      <c r="C21" s="93" t="s">
         <v>335</v>
       </c>
-      <c r="D21" s="122" t="s">
+      <c r="D21" s="93" t="s">
         <v>336</v>
       </c>
-      <c r="E21" s="122" t="str">
+      <c r="E21" s="93" t="str">
         <f t="shared" ref="E21" si="4">CONCATENATE("public By ",B21,C21,"=By.",IF(ISNUMBER(SEARCH("@id=",D21)),"xpath(""","id("""),D21,""");")</f>
         <v>public By txtConsultaSic=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[3]/p/a");</v>
       </c>
@@ -8351,16 +8405,16 @@
       <c r="A22" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="B22" s="122" t="s">
+      <c r="B22" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="93" t="s">
         <v>378</v>
       </c>
-      <c r="D22" s="122" t="s">
+      <c r="D22" s="93" t="s">
         <v>379</v>
       </c>
-      <c r="E22" s="122" t="str">
+      <c r="E22" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbSic=By.xpath("//*[@id=\'contenido_medio\']/div[1]/h1");</v>
       </c>
@@ -8369,16 +8423,16 @@
       <c r="A23" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B23" s="122" t="s">
+      <c r="B23" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C23" s="122" t="s">
+      <c r="C23" s="93" t="s">
         <v>337</v>
       </c>
-      <c r="D23" s="122" t="s">
+      <c r="D23" s="93" t="s">
         <v>338</v>
       </c>
-      <c r="E23" s="122" t="str">
+      <c r="E23" s="93" t="str">
         <f t="shared" ref="E23" si="5">CONCATENATE("public By ",B23,C23,"=By.",IF(ISNUMBER(SEARCH("@id=",D23)),"xpath(""","id("""),D23,""");")</f>
         <v>public By txtConoceNuestrasTiendas=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[4]/p/a");</v>
       </c>
@@ -8387,16 +8441,16 @@
       <c r="A24" s="26" t="s">
         <v>382</v>
       </c>
-      <c r="B24" s="122" t="s">
+      <c r="B24" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C24" s="122" t="s">
+      <c r="C24" s="93" t="s">
         <v>382</v>
       </c>
-      <c r="D24" s="122" t="s">
+      <c r="D24" s="93" t="s">
         <v>383</v>
       </c>
-      <c r="E24" s="122" t="str">
+      <c r="E24" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbTiendas=By.id("/html/body/content/div[2]/div/section[1]/div/div/h3");</v>
       </c>
@@ -8405,16 +8459,16 @@
       <c r="A25" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B25" s="122" t="s">
+      <c r="B25" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C25" s="122" t="s">
+      <c r="C25" s="93" t="s">
         <v>339</v>
       </c>
-      <c r="D25" s="122" t="s">
+      <c r="D25" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="E25" s="122" t="str">
+      <c r="E25" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnChatYAyuda=By.xpath("//*[@id="Embed"]/button/span[2]");</v>
       </c>
@@ -8423,16 +8477,16 @@
       <c r="A26" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B26" s="122" t="s">
+      <c r="B26" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C26" s="122" t="s">
+      <c r="C26" s="93" t="s">
         <v>341</v>
       </c>
-      <c r="D26" s="122" t="s">
+      <c r="D26" s="93" t="s">
         <v>342</v>
       </c>
-      <c r="E26" s="122" t="str">
+      <c r="E26" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtPersonas=By.xpath("//*[@id="top_menu"]/nav/ul/li[1]/a");</v>
       </c>
@@ -8441,16 +8495,16 @@
       <c r="A27" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B27" s="122" t="s">
+      <c r="B27" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C27" s="122" t="s">
+      <c r="C27" s="93" t="s">
         <v>343</v>
       </c>
-      <c r="D27" s="122" t="s">
+      <c r="D27" s="93" t="s">
         <v>344</v>
       </c>
-      <c r="E27" s="122" t="str">
+      <c r="E27" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtEmpresas=By.xpath("//*[@id="top_menu"]/nav/ul/li[2]/a");</v>
       </c>
@@ -8459,255 +8513,417 @@
       <c r="A28" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="122" t="s">
+      <c r="C28" s="93" t="s">
         <v>345</v>
       </c>
-      <c r="D28" s="122" t="s">
+      <c r="D28" s="93" t="s">
         <v>346</v>
       </c>
-      <c r="E28" s="122" t="str">
+      <c r="E28" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnDescubreloYa=By.xpath("//*[@id="main-content"]/div[2]/div[1]/div/div/div/section/div/div/a");</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B29" s="124" t="s">
+      <c r="B29" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C29" s="124" t="s">
+      <c r="C29" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="D29" s="124" t="s">
+      <c r="D29" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="E29" s="124" t="str">
+      <c r="E29" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCorreoElectronico=By.id("idEmail");</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="123" t="s">
+      <c r="A30" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B30" s="124" t="s">
+      <c r="B30" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="C30" s="124" t="s">
+      <c r="C30" s="95" t="s">
         <v>349</v>
       </c>
-      <c r="D30" s="124" t="s">
+      <c r="D30" s="95" t="s">
         <v>350</v>
       </c>
-      <c r="E30" s="124" t="str">
+      <c r="E30" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By btnValidarCorreo=By.id("continueBtn");</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="123" t="s">
+      <c r="A31" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="95" t="s">
         <v>236</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="95" t="s">
         <v>371</v>
       </c>
-      <c r="D31" s="124" t="s">
+      <c r="D31" s="95" t="s">
         <v>372</v>
       </c>
-      <c r="E31" s="124" t="str">
+      <c r="E31" s="95" t="str">
         <f t="shared" ref="E31" si="6">CONCATENATE("public By ",B31,C31,"=By.",IF(ISNUMBER(SEARCH("@id=",D31)),"xpath(""","id("""),D31,""");")</f>
         <v>public By lbIngresaAMiCuenta=By.id("/html/body/div[2]/div/div[1]/h5");</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="123" t="s">
+      <c r="A32" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B32" s="124" t="s">
+      <c r="B32" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C32" s="124" t="s">
+      <c r="C32" s="95" t="s">
         <v>351</v>
       </c>
-      <c r="D32" s="124" t="s">
+      <c r="D32" s="95" t="s">
         <v>352</v>
       </c>
-      <c r="E32" s="124" t="str">
+      <c r="E32" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCrearTuCuenta=By.id("/html/body/div[2]/div/div[3]/div/p[2]/a");</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="123" t="s">
+      <c r="A33" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B33" s="124" t="s">
+      <c r="B33" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C33" s="124" t="s">
+      <c r="C33" s="95" t="s">
         <v>353</v>
       </c>
-      <c r="D33" s="124" t="s">
+      <c r="D33" s="95" t="s">
         <v>354</v>
       </c>
-      <c r="E33" s="124" t="str">
+      <c r="E33" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtContraseña=By.id("password");</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="123" t="s">
+      <c r="A34" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B34" s="124" t="s">
+      <c r="B34" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="C34" s="124" t="s">
+      <c r="C34" s="95" t="s">
         <v>355</v>
       </c>
-      <c r="D34" s="124" t="s">
+      <c r="D34" s="95" t="s">
         <v>356</v>
       </c>
-      <c r="E34" s="124" t="str">
+      <c r="E34" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By btnContinuar=By.id("/html/body/div[2]/div/form/div[3]/button");</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="123" t="s">
+      <c r="A35" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B35" s="124" t="s">
+      <c r="B35" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C35" s="124" t="s">
+      <c r="C35" s="95" t="s">
         <v>373</v>
       </c>
-      <c r="D35" s="124" t="s">
+      <c r="D35" s="95" t="s">
         <v>357</v>
       </c>
-      <c r="E35" s="124" t="str">
+      <c r="E35" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtOlvidasteContrasena =By.id("/html/body/div[2]/div/form/div[4]/a");</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="123" t="s">
+      <c r="A36" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B36" s="124" t="s">
+      <c r="B36" s="95" t="s">
         <v>234</v>
       </c>
-      <c r="C36" s="124" t="s">
+      <c r="C36" s="95" t="s">
         <v>358</v>
       </c>
-      <c r="D36" s="124" t="s">
+      <c r="D36" s="95" t="s">
         <v>359</v>
       </c>
-      <c r="E36" s="124" t="str">
-        <f t="shared" si="0"/>
+      <c r="E36" s="95" t="str">
+        <f t="shared" ref="E36:E39" si="7">CONCATENATE("public By ",B36,C36,"=By.",IF(ISNUMBER(SEARCH("@id=",D36)),"xpath(""","id("""),D36,""");")</f>
         <v>public By listNumeroPlan=By.xpath("//*[@id="block-accountsblock-2"]/div/div/div/div/div/span");</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="123" t="s">
+      <c r="A37" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B37" s="124" t="s">
+      <c r="B37" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="95" t="s">
+        <v>416</v>
+      </c>
+      <c r="D37" s="95" t="s">
+        <v>417</v>
+      </c>
+      <c r="E37" s="95" t="str">
+        <f t="shared" si="7"/>
+        <v>public By listLineaPruebasJuanca=By.xpath("(((//*[@id='lines'])//a[contains(@href,'')]))[11]");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B38" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C38" s="95" t="s">
+        <v>418</v>
+      </c>
+      <c r="D38" s="95" t="s">
+        <v>419</v>
+      </c>
+      <c r="E38" s="95" t="str">
+        <f t="shared" ref="E38" si="8">CONCATENATE("public By ",B38,C38,"=By.",IF(ISNUMBER(SEARCH("@id=",D38)),"xpath(""","id("""),D38,""");")</f>
+        <v>public By listLineaHibridoMariana=By.xpath("(((((//*[@id='lines'])//a[contains(@href,'')])))//*[contains(text(),'Mariana')])[2]");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B39" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" s="95" t="s">
+        <v>420</v>
+      </c>
+      <c r="D39" s="95" t="s">
+        <v>421</v>
+      </c>
+      <c r="E39" s="95" t="str">
+        <f t="shared" si="7"/>
+        <v>public By listLineaHibridoAna=By.xpath("(((//*[@id='lines'])//a[contains(@href,'')]))[9]");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B40" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C37" s="124" t="s">
+      <c r="C40" s="95" t="s">
         <v>360</v>
       </c>
-      <c r="D37" s="124" t="s">
+      <c r="D40" s="95" t="s">
         <v>361</v>
       </c>
-      <c r="E37" s="124" t="str">
+      <c r="E40" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtResumen=By.id("/html/body/div[3]/div[2]/div/div/nav/div/div/ul/li[1]/a");</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="123" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B38" s="124" t="s">
+      <c r="B41" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C38" s="124" t="s">
+      <c r="C41" s="95" t="s">
         <v>362</v>
       </c>
-      <c r="D38" s="124" t="s">
+      <c r="D41" s="95" t="s">
         <v>363</v>
       </c>
-      <c r="E38" s="124" t="str">
-        <f t="shared" si="0"/>
+      <c r="E41" s="95" t="str">
+        <f t="shared" ref="E41:E46" si="9">CONCATENATE("public By ",B41,C41,"=By.",IF(ISNUMBER(SEARCH("@id=",D41)),"xpath(""","id("""),D41,""");")</f>
         <v>public By txtCambiateYa=By.xpath("//*[@id="action_Cámbiate ya"]");</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="125" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B42" s="95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="95" t="s">
+        <v>422</v>
+      </c>
+      <c r="D42" s="95" t="s">
+        <v>423</v>
+      </c>
+      <c r="E42" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By txtUsuario=By.xpath("//*[@id='top_menu_aside']/nav/ul/li/a");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B43" s="95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="95" t="s">
+        <v>424</v>
+      </c>
+      <c r="D43" s="95" t="s">
+        <v>425</v>
+      </c>
+      <c r="E43" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By txtCerrarSesion=By.xpath("//*[@id='top_menu_aside']/nav/ul/li/ul/li[2]/a");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B44" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C44" s="95" t="s">
+        <v>426</v>
+      </c>
+      <c r="D44" s="95" t="s">
+        <v>427</v>
+      </c>
+      <c r="E44" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By btnCambiarCuenta=By.xpath("//*[@id='addNew']");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B45" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C45" s="95" t="s">
+        <v>428</v>
+      </c>
+      <c r="D45" s="95" t="s">
+        <v>429</v>
+      </c>
+      <c r="E45" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By lbPlanes=By.xpath("//*[@id='main-content']/div[2]");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B46" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C46" s="95" t="s">
+        <v>430</v>
+      </c>
+      <c r="D46" s="95" t="s">
+        <v>431</v>
+      </c>
+      <c r="E46" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By lbMejorarPlan=By.xpath("//*[@id='compras-noplan-container']/h3");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B47" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C47" s="95" t="s">
+        <v>432</v>
+      </c>
+      <c r="D47" s="95" t="s">
+        <v>433</v>
+      </c>
+      <c r="E47" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbDetallePlan=By.xpath("//*[@id='compras-noplan-container']/p");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="B39" s="126" t="s">
+      <c r="B48" s="97" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="126" t="s">
+      <c r="C48" s="97" t="s">
         <v>365</v>
       </c>
-      <c r="D39" s="126" t="s">
+      <c r="D48" s="97" t="s">
         <v>366</v>
       </c>
-      <c r="E39" s="126" t="str">
+      <c r="E48" s="97" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConMiCorreo=By.xpath("//*[@id="addNew"]");</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="125" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="B40" s="126" t="s">
+      <c r="B49" s="97" t="s">
         <v>232</v>
       </c>
-      <c r="C40" s="126" t="s">
+      <c r="C49" s="97" t="s">
         <v>367</v>
       </c>
-      <c r="D40" s="126" t="s">
+      <c r="D49" s="97" t="s">
         <v>368</v>
       </c>
-      <c r="E40" s="126" t="str">
+      <c r="E49" s="97" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConFacebook=By.xpath("//*[@id="SLFacebook"]");</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="127" t="s">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="98" t="s">
         <v>364</v>
       </c>
-      <c r="B41" s="128" t="s">
+      <c r="B50" s="99" t="s">
         <v>232</v>
       </c>
-      <c r="C41" s="128" t="s">
+      <c r="C50" s="99" t="s">
         <v>369</v>
       </c>
-      <c r="D41" s="128" t="s">
+      <c r="D50" s="99" t="s">
         <v>370</v>
       </c>
-      <c r="E41" s="128" t="str">
+      <c r="E50" s="99" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConGoogle=By.xpath("//*[@id="SLGoogle"]");</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8718,7 +8934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E972679-EDA2-4ED9-97F5-E044AE9E5203}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -8887,16 +9103,16 @@
       <c r="A10" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="93" t="s">
         <v>403</v>
       </c>
-      <c r="D10" s="122" t="s">
+      <c r="D10" s="93" t="s">
         <v>404</v>
       </c>
-      <c r="E10" s="122" t="str">
+      <c r="E10" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnOtroValor=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[6]");</v>
       </c>
@@ -8905,16 +9121,16 @@
       <c r="A11" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="93" t="s">
         <v>405</v>
       </c>
-      <c r="D11" s="122" t="s">
+      <c r="D11" s="93" t="s">
         <v>406</v>
       </c>
-      <c r="E11" s="122" t="str">
+      <c r="E11" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtValorRecargar=By.id("edit-otro-valor");</v>
       </c>
@@ -8923,16 +9139,16 @@
       <c r="A12" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="93" t="s">
         <v>407</v>
       </c>
-      <c r="D12" s="122" t="s">
+      <c r="D12" s="93" t="s">
         <v>408</v>
       </c>
-      <c r="E12" s="122" t="str">
+      <c r="E12" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbErrorValor=By.xpath("//*[@id="other_value"]/div/div/div[1]/p");</v>
       </c>
@@ -8941,16 +9157,16 @@
       <c r="A13" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="93" t="s">
         <v>255</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="122" t="str">
+      <c r="E13" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCorreoElectronico=By.id("edit-email");</v>
       </c>
@@ -8959,70 +9175,70 @@
       <c r="A14" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B14" s="122" t="s">
+      <c r="B14" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="93" t="s">
         <v>409</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="D14" s="93" t="s">
         <v>410</v>
       </c>
-      <c r="E14" s="122" t="str">
+      <c r="E14" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnRecargar=By.id("edit-button-recargar");</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="101" t="s">
         <v>411</v>
       </c>
-      <c r="D15" s="130" t="s">
+      <c r="D15" s="101" t="s">
         <v>412</v>
       </c>
-      <c r="E15" s="130" t="str">
+      <c r="E15" s="101" t="str">
         <f t="shared" si="0"/>
         <v>public By lbResumenTransaccion=By.xpath("//*[@id="title-detail"]");</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="130" t="s">
+      <c r="B16" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="130" t="s">
+      <c r="C16" s="101" t="s">
         <v>413</v>
       </c>
-      <c r="D16" s="130" t="s">
+      <c r="D16" s="101" t="s">
         <v>414</v>
       </c>
-      <c r="E16" s="130" t="str">
+      <c r="E16" s="101" t="str">
         <f t="shared" si="0"/>
         <v>public By lbNumeroDelProducto=By.id("product-number");</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="131" t="s">
+      <c r="A17" s="102" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="132" t="s">
+      <c r="B17" s="103" t="s">
         <v>236</v>
       </c>
-      <c r="C17" s="132" t="s">
+      <c r="C17" s="103" t="s">
         <v>280</v>
       </c>
-      <c r="D17" s="132" t="s">
+      <c r="D17" s="103" t="s">
         <v>415</v>
       </c>
-      <c r="E17" s="132" t="str">
+      <c r="E17" s="103" t="str">
         <f t="shared" si="0"/>
         <v>public By lbValorPagar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]");</v>
       </c>

</xml_diff>

<commit_message>
Se actualiza el archivo del Mapeo de los Campos (Mi Cuenta)
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasprilla\Documents\automatizacion_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B91DB4-8B3F-401D-87B1-5470BFBB51A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391733F1-CCED-4BE4-BD82-A9A8811F524B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="434">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -1282,6 +1282,60 @@
   </si>
   <si>
     <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]</t>
+  </si>
+  <si>
+    <t>LineaPruebasJuanca</t>
+  </si>
+  <si>
+    <t>(((//*[@id='lines'])//a[contains(@href,'')]))[11]</t>
+  </si>
+  <si>
+    <t>LineaHibridoMariana</t>
+  </si>
+  <si>
+    <t>(((((//*[@id='lines'])//a[contains(@href,'')])))//*[contains(text(),'Mariana')])[2]</t>
+  </si>
+  <si>
+    <t>LineaHibridoAna</t>
+  </si>
+  <si>
+    <t>(((//*[@id='lines'])//a[contains(@href,'')]))[9]</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>//*[@id='top_menu_aside']/nav/ul/li/a</t>
+  </si>
+  <si>
+    <t>CerrarSesion</t>
+  </si>
+  <si>
+    <t>//*[@id='top_menu_aside']/nav/ul/li/ul/li[2]/a</t>
+  </si>
+  <si>
+    <t>CambiarCuenta</t>
+  </si>
+  <si>
+    <t>//*[@id='addNew']</t>
+  </si>
+  <si>
+    <t>Planes</t>
+  </si>
+  <si>
+    <t>//*[@id='main-content']/div[2]</t>
+  </si>
+  <si>
+    <t>MejorarPlan</t>
+  </si>
+  <si>
+    <t>//*[@id='compras-noplan-container']/h3</t>
+  </si>
+  <si>
+    <t>DetallePlan</t>
+  </si>
+  <si>
+    <t>//*[@id='compras-noplan-container']/p</t>
   </si>
 </sst>
 </file>
@@ -1850,6 +1904,39 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1936,39 +2023,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2596,78 +2650,78 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="104" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="93"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="93"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="93"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="93"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="93"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="93"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
+      <c r="A20" s="104"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="93"/>
-      <c r="B21" s="93"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2700,17 +2754,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -4985,14 +5039,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5015,7 +5069,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="118" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -5035,7 +5089,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="108"/>
+      <c r="A4" s="119"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -5053,7 +5107,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="108"/>
+      <c r="A5" s="119"/>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -5071,7 +5125,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
+      <c r="A6" s="119"/>
       <c r="B6" s="3" t="s">
         <v>101</v>
       </c>
@@ -5089,7 +5143,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="108"/>
+      <c r="A7" s="119"/>
       <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
@@ -5110,7 +5164,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="108"/>
+      <c r="A8" s="119"/>
       <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
@@ -5131,7 +5185,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="109"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="3" t="s">
         <v>229</v>
       </c>
@@ -5149,7 +5203,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="127" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -5169,7 +5223,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="117"/>
+      <c r="A11" s="128"/>
       <c r="B11" s="7" t="s">
         <v>124</v>
       </c>
@@ -5190,7 +5244,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="117"/>
+      <c r="A12" s="128"/>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -5208,7 +5262,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="117"/>
+      <c r="A13" s="128"/>
       <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
@@ -5229,7 +5283,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
+      <c r="A14" s="128"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -5247,7 +5301,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+      <c r="A15" s="128"/>
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -5265,7 +5319,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="117"/>
+      <c r="A16" s="128"/>
       <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
@@ -5283,7 +5337,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="117"/>
+      <c r="A17" s="128"/>
       <c r="B17" s="7" t="s">
         <v>101</v>
       </c>
@@ -5301,7 +5355,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="117"/>
+      <c r="A18" s="128"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -5319,7 +5373,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
+      <c r="A19" s="129"/>
       <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
@@ -5337,7 +5391,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="101" t="s">
+      <c r="A20" s="112" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -5357,7 +5411,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="102"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="4" t="s">
         <v>81</v>
       </c>
@@ -5382,7 +5436,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="102"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
@@ -5400,7 +5454,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="102"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="4" t="s">
         <v>82</v>
       </c>
@@ -5418,7 +5472,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
+      <c r="A24" s="114"/>
       <c r="B24" s="4" t="s">
         <v>83</v>
       </c>
@@ -5443,7 +5497,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="104" t="s">
+      <c r="A25" s="115" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -5463,7 +5517,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="105"/>
+      <c r="A26" s="116"/>
       <c r="B26" s="13" t="s">
         <v>27</v>
       </c>
@@ -5481,7 +5535,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="106"/>
+      <c r="A27" s="117"/>
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -5499,7 +5553,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="130" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5519,7 +5573,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="120"/>
+      <c r="A29" s="131"/>
       <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
@@ -5540,7 +5594,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="120"/>
+      <c r="A30" s="131"/>
       <c r="B30" s="15" t="s">
         <v>118</v>
       </c>
@@ -5561,7 +5615,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="120"/>
+      <c r="A31" s="131"/>
       <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
@@ -5579,7 +5633,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="120"/>
+      <c r="A32" s="131"/>
       <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
@@ -5597,7 +5651,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="120"/>
+      <c r="A33" s="131"/>
       <c r="B33" s="15" t="s">
         <v>35</v>
       </c>
@@ -5615,7 +5669,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="120"/>
+      <c r="A34" s="131"/>
       <c r="B34" s="15" t="s">
         <v>36</v>
       </c>
@@ -5633,7 +5687,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="120"/>
+      <c r="A35" s="131"/>
       <c r="B35" s="15" t="s">
         <v>39</v>
       </c>
@@ -5651,7 +5705,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="120"/>
+      <c r="A36" s="131"/>
       <c r="B36" s="15" t="s">
         <v>3</v>
       </c>
@@ -5669,7 +5723,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="120"/>
+      <c r="A37" s="131"/>
       <c r="B37" s="15" t="s">
         <v>42</v>
       </c>
@@ -5687,7 +5741,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="120"/>
+      <c r="A38" s="131"/>
       <c r="B38" s="15" t="s">
         <v>122</v>
       </c>
@@ -5708,7 +5762,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="120"/>
+      <c r="A39" s="131"/>
       <c r="B39" s="15" t="s">
         <v>44</v>
       </c>
@@ -5726,7 +5780,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="120"/>
+      <c r="A40" s="131"/>
       <c r="B40" s="15" t="s">
         <v>130</v>
       </c>
@@ -5747,7 +5801,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="120"/>
+      <c r="A41" s="131"/>
       <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
@@ -5765,7 +5819,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="120"/>
+      <c r="A42" s="131"/>
       <c r="B42" s="15" t="s">
         <v>110</v>
       </c>
@@ -5786,7 +5840,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="120"/>
+      <c r="A43" s="131"/>
       <c r="B43" s="15" t="s">
         <v>47</v>
       </c>
@@ -5802,7 +5856,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="120"/>
+      <c r="A44" s="131"/>
       <c r="B44" s="15" t="s">
         <v>101</v>
       </c>
@@ -5818,7 +5872,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="120"/>
+      <c r="A45" s="131"/>
       <c r="B45" s="15" t="s">
         <v>22</v>
       </c>
@@ -5836,7 +5890,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="121"/>
+      <c r="A46" s="132"/>
       <c r="B46" s="15" t="s">
         <v>51</v>
       </c>
@@ -5854,7 +5908,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="110" t="s">
+      <c r="A47" s="121" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -5874,7 +5928,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="111"/>
+      <c r="A48" s="122"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -5892,7 +5946,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="111"/>
+      <c r="A49" s="122"/>
       <c r="B49" s="5" t="s">
         <v>56</v>
       </c>
@@ -5910,7 +5964,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="111"/>
+      <c r="A50" s="122"/>
       <c r="B50" s="5" t="s">
         <v>3</v>
       </c>
@@ -5928,7 +5982,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="111"/>
+      <c r="A51" s="122"/>
       <c r="B51" s="5" t="s">
         <v>60</v>
       </c>
@@ -5946,7 +6000,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="111"/>
+      <c r="A52" s="122"/>
       <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
@@ -5964,7 +6018,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="111"/>
+      <c r="A53" s="122"/>
       <c r="B53" s="5" t="s">
         <v>101</v>
       </c>
@@ -5980,7 +6034,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="111"/>
+      <c r="A54" s="122"/>
       <c r="B54" s="5" t="s">
         <v>22</v>
       </c>
@@ -5998,7 +6052,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="112"/>
+      <c r="A55" s="123"/>
       <c r="B55" s="5" t="s">
         <v>64</v>
       </c>
@@ -6016,7 +6070,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="113" t="s">
+      <c r="A56" s="124" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -6036,7 +6090,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="114"/>
+      <c r="A57" s="125"/>
       <c r="B57" s="1" t="s">
         <v>101</v>
       </c>
@@ -6052,7 +6106,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="114"/>
+      <c r="A58" s="125"/>
       <c r="B58" s="1" t="s">
         <v>22</v>
       </c>
@@ -6070,7 +6124,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="115"/>
+      <c r="A59" s="126"/>
       <c r="B59" s="1" t="s">
         <v>48</v>
       </c>
@@ -6088,7 +6142,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="96" t="s">
+      <c r="A60" s="107" t="s">
         <v>136</v>
       </c>
       <c r="B60" s="23" t="s">
@@ -6111,7 +6165,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="97"/>
+      <c r="A61" s="108"/>
       <c r="B61" s="23" t="s">
         <v>137</v>
       </c>
@@ -6129,7 +6183,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="97"/>
+      <c r="A62" s="108"/>
       <c r="B62" s="23" t="s">
         <v>138</v>
       </c>
@@ -6147,7 +6201,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="97"/>
+      <c r="A63" s="108"/>
       <c r="B63" s="23" t="s">
         <v>139</v>
       </c>
@@ -6165,7 +6219,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="97"/>
+      <c r="A64" s="108"/>
       <c r="B64" s="23" t="s">
         <v>140</v>
       </c>
@@ -6183,7 +6237,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="97"/>
+      <c r="A65" s="108"/>
       <c r="B65" s="23" t="s">
         <v>141</v>
       </c>
@@ -6201,7 +6255,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="97"/>
+      <c r="A66" s="108"/>
       <c r="B66" s="23" t="s">
         <v>142</v>
       </c>
@@ -6219,7 +6273,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="97"/>
+      <c r="A67" s="108"/>
       <c r="B67" s="23" t="s">
         <v>143</v>
       </c>
@@ -6237,7 +6291,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="97"/>
+      <c r="A68" s="108"/>
       <c r="B68" s="23" t="s">
         <v>144</v>
       </c>
@@ -6255,7 +6309,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="97"/>
+      <c r="A69" s="108"/>
       <c r="B69" s="23" t="s">
         <v>145</v>
       </c>
@@ -6273,7 +6327,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="97"/>
+      <c r="A70" s="108"/>
       <c r="B70" s="23" t="s">
         <v>146</v>
       </c>
@@ -6291,7 +6345,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="97"/>
+      <c r="A71" s="108"/>
       <c r="B71" s="23" t="s">
         <v>147</v>
       </c>
@@ -6309,7 +6363,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="97"/>
+      <c r="A72" s="108"/>
       <c r="B72" s="23" t="s">
         <v>148</v>
       </c>
@@ -6327,7 +6381,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="97"/>
+      <c r="A73" s="108"/>
       <c r="B73" s="23" t="s">
         <v>149</v>
       </c>
@@ -6345,7 +6399,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="98"/>
+      <c r="A74" s="109"/>
       <c r="B74" s="23" t="s">
         <v>150</v>
       </c>
@@ -7964,10 +8018,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDA504D-8FF2-405F-AE1B-22086E468A89}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7976,7 +8030,7 @@
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="75.42578125" customWidth="1"/>
-    <col min="5" max="5" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="114.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8073,7 +8127,7 @@
         <v>316</v>
       </c>
       <c r="E6" s="48" t="str">
-        <f t="shared" ref="E6:E41" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <f t="shared" ref="E6:E50" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
         <v>public By btnIngresar=By.xpath("//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[2]");</v>
       </c>
     </row>
@@ -8135,16 +8189,16 @@
       <c r="A10" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="93" t="s">
         <v>323</v>
       </c>
-      <c r="D10" s="122" t="s">
+      <c r="D10" s="93" t="s">
         <v>324</v>
       </c>
-      <c r="E10" s="122" t="str">
+      <c r="E10" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnReponeTuSim=By.xpath("//*[@id="main-content"]/div[2]/div[6]/div/div/div/div/a");</v>
       </c>
@@ -8153,16 +8207,16 @@
       <c r="A11" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="93" t="s">
         <v>325</v>
       </c>
-      <c r="D11" s="122" t="s">
+      <c r="D11" s="93" t="s">
         <v>326</v>
       </c>
-      <c r="E11" s="122" t="str">
+      <c r="E11" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCambiarMiClave=By.xpath("//*[@id="main-content"]/div[2]/div[7]/div/div/div/div/div[2]/a");</v>
       </c>
@@ -8171,16 +8225,16 @@
       <c r="A12" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="93" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="122" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="122" t="s">
+      <c r="C12" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="93" t="s">
         <v>327</v>
       </c>
-      <c r="E12" s="122" t="str">
+      <c r="E12" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By listTipo=By.xpath("//*[@id="t_document"]/div/div/input");</v>
       </c>
@@ -8189,16 +8243,16 @@
       <c r="A13" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="93" t="s">
         <v>276</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="93" t="s">
         <v>328</v>
       </c>
-      <c r="E13" s="122" t="str">
+      <c r="E13" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtNumeroDocumento=By.xpath("//*[@id="document"]");</v>
       </c>
@@ -8207,16 +8261,16 @@
       <c r="A14" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B14" s="122" t="s">
+      <c r="B14" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="93" t="s">
         <v>386</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="D14" s="93" t="s">
         <v>329</v>
       </c>
-      <c r="E14" s="122" t="str">
+      <c r="E14" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbMsgErrorDocumento=By.xpath("//*[@id="query-container"]/section/div[1]/span[2]");</v>
       </c>
@@ -8225,16 +8279,16 @@
       <c r="A15" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C15" s="122" t="s">
+      <c r="C15" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="122" t="s">
+      <c r="D15" s="93" t="s">
         <v>330</v>
       </c>
-      <c r="E15" s="122" t="str">
+      <c r="E15" s="93" t="str">
         <f t="shared" ref="E15" si="1">CONCATENATE("public By ",B15,C15,"=By.",IF(ISNUMBER(SEARCH("@id=",D15)),"xpath(""","id("""),D15,""");")</f>
         <v>public By btnConsultar=By.xpath("//*[@id="findagenda"]/div[2]/div[2]");</v>
       </c>
@@ -8243,16 +8297,16 @@
       <c r="A16" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B16" s="122" t="s">
+      <c r="B16" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="122" t="s">
+      <c r="C16" s="93" t="s">
         <v>384</v>
       </c>
-      <c r="D16" s="122" t="s">
+      <c r="D16" s="93" t="s">
         <v>385</v>
       </c>
-      <c r="E16" s="122" t="str">
+      <c r="E16" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbVisitasPendientes=By.xpath("//*[@id=\'schedule-visits-container\']/div[2]/div[1]/div/p");</v>
       </c>
@@ -8261,16 +8315,16 @@
       <c r="A17" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B17" s="122" t="s">
+      <c r="B17" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C17" s="122" t="s">
+      <c r="C17" s="93" t="s">
         <v>331</v>
       </c>
-      <c r="D17" s="122" t="s">
+      <c r="D17" s="93" t="s">
         <v>332</v>
       </c>
-      <c r="E17" s="122" t="str">
+      <c r="E17" s="93" t="str">
         <f t="shared" ref="E17" si="2">CONCATENATE("public By ",B17,C17,"=By.",IF(ISNUMBER(SEARCH("@id=",D17)),"xpath(""","id("""),D17,""");")</f>
         <v>public By txtConsultaPQRUne=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[1]/p/a");</v>
       </c>
@@ -8279,16 +8333,16 @@
       <c r="A18" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="93" t="s">
         <v>374</v>
       </c>
-      <c r="D18" s="122" t="s">
+      <c r="D18" s="93" t="s">
         <v>375</v>
       </c>
-      <c r="E18" s="122" t="str">
+      <c r="E18" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbPQRUne=By.id("/html/body/div[4]/div/div/div/div[1]/h3");</v>
       </c>
@@ -8297,16 +8351,16 @@
       <c r="A19" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="93" t="s">
         <v>333</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="93" t="s">
         <v>334</v>
       </c>
-      <c r="E19" s="122" t="str">
+      <c r="E19" s="93" t="str">
         <f t="shared" ref="E19" si="3">CONCATENATE("public By ",B19,C19,"=By.",IF(ISNUMBER(SEARCH("@id=",D19)),"xpath(""","id("""),D19,""");")</f>
         <v>public By txtConsultaPQRTigo=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[2]/p/a");</v>
       </c>
@@ -8315,16 +8369,16 @@
       <c r="A20" s="26" t="s">
         <v>380</v>
       </c>
-      <c r="B20" s="122" t="s">
+      <c r="B20" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C20" s="122" t="s">
+      <c r="C20" s="93" t="s">
         <v>376</v>
       </c>
-      <c r="D20" s="122" t="s">
+      <c r="D20" s="93" t="s">
         <v>377</v>
       </c>
-      <c r="E20" s="122" t="str">
+      <c r="E20" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbPQRTigo=By.xpath("//*[@id='formInicioPqr:panelBotonesInicio']/thead/tr/th/span");</v>
       </c>
@@ -8333,16 +8387,16 @@
       <c r="A21" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="122" t="s">
+      <c r="C21" s="93" t="s">
         <v>335</v>
       </c>
-      <c r="D21" s="122" t="s">
+      <c r="D21" s="93" t="s">
         <v>336</v>
       </c>
-      <c r="E21" s="122" t="str">
+      <c r="E21" s="93" t="str">
         <f t="shared" ref="E21" si="4">CONCATENATE("public By ",B21,C21,"=By.",IF(ISNUMBER(SEARCH("@id=",D21)),"xpath(""","id("""),D21,""");")</f>
         <v>public By txtConsultaSic=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[3]/p/a");</v>
       </c>
@@ -8351,16 +8405,16 @@
       <c r="A22" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="B22" s="122" t="s">
+      <c r="B22" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="93" t="s">
         <v>378</v>
       </c>
-      <c r="D22" s="122" t="s">
+      <c r="D22" s="93" t="s">
         <v>379</v>
       </c>
-      <c r="E22" s="122" t="str">
+      <c r="E22" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbSic=By.xpath("//*[@id=\'contenido_medio\']/div[1]/h1");</v>
       </c>
@@ -8369,16 +8423,16 @@
       <c r="A23" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B23" s="122" t="s">
+      <c r="B23" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C23" s="122" t="s">
+      <c r="C23" s="93" t="s">
         <v>337</v>
       </c>
-      <c r="D23" s="122" t="s">
+      <c r="D23" s="93" t="s">
         <v>338</v>
       </c>
-      <c r="E23" s="122" t="str">
+      <c r="E23" s="93" t="str">
         <f t="shared" ref="E23" si="5">CONCATENATE("public By ",B23,C23,"=By.",IF(ISNUMBER(SEARCH("@id=",D23)),"xpath(""","id("""),D23,""");")</f>
         <v>public By txtConoceNuestrasTiendas=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[4]/p/a");</v>
       </c>
@@ -8387,16 +8441,16 @@
       <c r="A24" s="26" t="s">
         <v>382</v>
       </c>
-      <c r="B24" s="122" t="s">
+      <c r="B24" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C24" s="122" t="s">
+      <c r="C24" s="93" t="s">
         <v>382</v>
       </c>
-      <c r="D24" s="122" t="s">
+      <c r="D24" s="93" t="s">
         <v>383</v>
       </c>
-      <c r="E24" s="122" t="str">
+      <c r="E24" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbTiendas=By.id("/html/body/content/div[2]/div/section[1]/div/div/h3");</v>
       </c>
@@ -8405,16 +8459,16 @@
       <c r="A25" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B25" s="122" t="s">
+      <c r="B25" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C25" s="122" t="s">
+      <c r="C25" s="93" t="s">
         <v>339</v>
       </c>
-      <c r="D25" s="122" t="s">
+      <c r="D25" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="E25" s="122" t="str">
+      <c r="E25" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnChatYAyuda=By.xpath("//*[@id="Embed"]/button/span[2]");</v>
       </c>
@@ -8423,16 +8477,16 @@
       <c r="A26" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B26" s="122" t="s">
+      <c r="B26" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C26" s="122" t="s">
+      <c r="C26" s="93" t="s">
         <v>341</v>
       </c>
-      <c r="D26" s="122" t="s">
+      <c r="D26" s="93" t="s">
         <v>342</v>
       </c>
-      <c r="E26" s="122" t="str">
+      <c r="E26" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtPersonas=By.xpath("//*[@id="top_menu"]/nav/ul/li[1]/a");</v>
       </c>
@@ -8441,16 +8495,16 @@
       <c r="A27" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B27" s="122" t="s">
+      <c r="B27" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C27" s="122" t="s">
+      <c r="C27" s="93" t="s">
         <v>343</v>
       </c>
-      <c r="D27" s="122" t="s">
+      <c r="D27" s="93" t="s">
         <v>344</v>
       </c>
-      <c r="E27" s="122" t="str">
+      <c r="E27" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtEmpresas=By.xpath("//*[@id="top_menu"]/nav/ul/li[2]/a");</v>
       </c>
@@ -8459,255 +8513,417 @@
       <c r="A28" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="122" t="s">
+      <c r="C28" s="93" t="s">
         <v>345</v>
       </c>
-      <c r="D28" s="122" t="s">
+      <c r="D28" s="93" t="s">
         <v>346</v>
       </c>
-      <c r="E28" s="122" t="str">
+      <c r="E28" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnDescubreloYa=By.xpath("//*[@id="main-content"]/div[2]/div[1]/div/div/div/section/div/div/a");</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B29" s="124" t="s">
+      <c r="B29" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C29" s="124" t="s">
+      <c r="C29" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="D29" s="124" t="s">
+      <c r="D29" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="E29" s="124" t="str">
+      <c r="E29" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCorreoElectronico=By.id("idEmail");</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="123" t="s">
+      <c r="A30" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B30" s="124" t="s">
+      <c r="B30" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="C30" s="124" t="s">
+      <c r="C30" s="95" t="s">
         <v>349</v>
       </c>
-      <c r="D30" s="124" t="s">
+      <c r="D30" s="95" t="s">
         <v>350</v>
       </c>
-      <c r="E30" s="124" t="str">
+      <c r="E30" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By btnValidarCorreo=By.id("continueBtn");</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="123" t="s">
+      <c r="A31" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="95" t="s">
         <v>236</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="95" t="s">
         <v>371</v>
       </c>
-      <c r="D31" s="124" t="s">
+      <c r="D31" s="95" t="s">
         <v>372</v>
       </c>
-      <c r="E31" s="124" t="str">
+      <c r="E31" s="95" t="str">
         <f t="shared" ref="E31" si="6">CONCATENATE("public By ",B31,C31,"=By.",IF(ISNUMBER(SEARCH("@id=",D31)),"xpath(""","id("""),D31,""");")</f>
         <v>public By lbIngresaAMiCuenta=By.id("/html/body/div[2]/div/div[1]/h5");</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="123" t="s">
+      <c r="A32" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B32" s="124" t="s">
+      <c r="B32" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C32" s="124" t="s">
+      <c r="C32" s="95" t="s">
         <v>351</v>
       </c>
-      <c r="D32" s="124" t="s">
+      <c r="D32" s="95" t="s">
         <v>352</v>
       </c>
-      <c r="E32" s="124" t="str">
+      <c r="E32" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCrearTuCuenta=By.id("/html/body/div[2]/div/div[3]/div/p[2]/a");</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="123" t="s">
+      <c r="A33" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B33" s="124" t="s">
+      <c r="B33" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C33" s="124" t="s">
+      <c r="C33" s="95" t="s">
         <v>353</v>
       </c>
-      <c r="D33" s="124" t="s">
+      <c r="D33" s="95" t="s">
         <v>354</v>
       </c>
-      <c r="E33" s="124" t="str">
+      <c r="E33" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtContraseña=By.id("password");</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="123" t="s">
+      <c r="A34" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B34" s="124" t="s">
+      <c r="B34" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="C34" s="124" t="s">
+      <c r="C34" s="95" t="s">
         <v>355</v>
       </c>
-      <c r="D34" s="124" t="s">
+      <c r="D34" s="95" t="s">
         <v>356</v>
       </c>
-      <c r="E34" s="124" t="str">
+      <c r="E34" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By btnContinuar=By.id("/html/body/div[2]/div/form/div[3]/button");</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="123" t="s">
+      <c r="A35" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B35" s="124" t="s">
+      <c r="B35" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C35" s="124" t="s">
+      <c r="C35" s="95" t="s">
         <v>373</v>
       </c>
-      <c r="D35" s="124" t="s">
+      <c r="D35" s="95" t="s">
         <v>357</v>
       </c>
-      <c r="E35" s="124" t="str">
+      <c r="E35" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtOlvidasteContrasena =By.id("/html/body/div[2]/div/form/div[4]/a");</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="123" t="s">
+      <c r="A36" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B36" s="124" t="s">
+      <c r="B36" s="95" t="s">
         <v>234</v>
       </c>
-      <c r="C36" s="124" t="s">
+      <c r="C36" s="95" t="s">
         <v>358</v>
       </c>
-      <c r="D36" s="124" t="s">
+      <c r="D36" s="95" t="s">
         <v>359</v>
       </c>
-      <c r="E36" s="124" t="str">
-        <f t="shared" si="0"/>
+      <c r="E36" s="95" t="str">
+        <f t="shared" ref="E36:E39" si="7">CONCATENATE("public By ",B36,C36,"=By.",IF(ISNUMBER(SEARCH("@id=",D36)),"xpath(""","id("""),D36,""");")</f>
         <v>public By listNumeroPlan=By.xpath("//*[@id="block-accountsblock-2"]/div/div/div/div/div/span");</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="123" t="s">
+      <c r="A37" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B37" s="124" t="s">
+      <c r="B37" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="95" t="s">
+        <v>416</v>
+      </c>
+      <c r="D37" s="95" t="s">
+        <v>417</v>
+      </c>
+      <c r="E37" s="95" t="str">
+        <f t="shared" si="7"/>
+        <v>public By listLineaPruebasJuanca=By.xpath("(((//*[@id='lines'])//a[contains(@href,'')]))[11]");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B38" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C38" s="95" t="s">
+        <v>418</v>
+      </c>
+      <c r="D38" s="95" t="s">
+        <v>419</v>
+      </c>
+      <c r="E38" s="95" t="str">
+        <f t="shared" ref="E38" si="8">CONCATENATE("public By ",B38,C38,"=By.",IF(ISNUMBER(SEARCH("@id=",D38)),"xpath(""","id("""),D38,""");")</f>
+        <v>public By listLineaHibridoMariana=By.xpath("(((((//*[@id='lines'])//a[contains(@href,'')])))//*[contains(text(),'Mariana')])[2]");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B39" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" s="95" t="s">
+        <v>420</v>
+      </c>
+      <c r="D39" s="95" t="s">
+        <v>421</v>
+      </c>
+      <c r="E39" s="95" t="str">
+        <f t="shared" si="7"/>
+        <v>public By listLineaHibridoAna=By.xpath("(((//*[@id='lines'])//a[contains(@href,'')]))[9]");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B40" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C37" s="124" t="s">
+      <c r="C40" s="95" t="s">
         <v>360</v>
       </c>
-      <c r="D37" s="124" t="s">
+      <c r="D40" s="95" t="s">
         <v>361</v>
       </c>
-      <c r="E37" s="124" t="str">
+      <c r="E40" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtResumen=By.id("/html/body/div[3]/div[2]/div/div/nav/div/div/ul/li[1]/a");</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="123" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B38" s="124" t="s">
+      <c r="B41" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C38" s="124" t="s">
+      <c r="C41" s="95" t="s">
         <v>362</v>
       </c>
-      <c r="D38" s="124" t="s">
+      <c r="D41" s="95" t="s">
         <v>363</v>
       </c>
-      <c r="E38" s="124" t="str">
-        <f t="shared" si="0"/>
+      <c r="E41" s="95" t="str">
+        <f t="shared" ref="E41:E46" si="9">CONCATENATE("public By ",B41,C41,"=By.",IF(ISNUMBER(SEARCH("@id=",D41)),"xpath(""","id("""),D41,""");")</f>
         <v>public By txtCambiateYa=By.xpath("//*[@id="action_Cámbiate ya"]");</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="125" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B42" s="95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="95" t="s">
+        <v>422</v>
+      </c>
+      <c r="D42" s="95" t="s">
+        <v>423</v>
+      </c>
+      <c r="E42" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By txtUsuario=By.xpath("//*[@id='top_menu_aside']/nav/ul/li/a");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B43" s="95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="95" t="s">
+        <v>424</v>
+      </c>
+      <c r="D43" s="95" t="s">
+        <v>425</v>
+      </c>
+      <c r="E43" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By txtCerrarSesion=By.xpath("//*[@id='top_menu_aside']/nav/ul/li/ul/li[2]/a");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B44" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C44" s="95" t="s">
+        <v>426</v>
+      </c>
+      <c r="D44" s="95" t="s">
+        <v>427</v>
+      </c>
+      <c r="E44" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By btnCambiarCuenta=By.xpath("//*[@id='addNew']");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B45" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C45" s="95" t="s">
+        <v>428</v>
+      </c>
+      <c r="D45" s="95" t="s">
+        <v>429</v>
+      </c>
+      <c r="E45" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By lbPlanes=By.xpath("//*[@id='main-content']/div[2]");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B46" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C46" s="95" t="s">
+        <v>430</v>
+      </c>
+      <c r="D46" s="95" t="s">
+        <v>431</v>
+      </c>
+      <c r="E46" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By lbMejorarPlan=By.xpath("//*[@id='compras-noplan-container']/h3");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B47" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C47" s="95" t="s">
+        <v>432</v>
+      </c>
+      <c r="D47" s="95" t="s">
+        <v>433</v>
+      </c>
+      <c r="E47" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbDetallePlan=By.xpath("//*[@id='compras-noplan-container']/p");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="B39" s="126" t="s">
+      <c r="B48" s="97" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="126" t="s">
+      <c r="C48" s="97" t="s">
         <v>365</v>
       </c>
-      <c r="D39" s="126" t="s">
+      <c r="D48" s="97" t="s">
         <v>366</v>
       </c>
-      <c r="E39" s="126" t="str">
+      <c r="E48" s="97" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConMiCorreo=By.xpath("//*[@id="addNew"]");</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="125" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="B40" s="126" t="s">
+      <c r="B49" s="97" t="s">
         <v>232</v>
       </c>
-      <c r="C40" s="126" t="s">
+      <c r="C49" s="97" t="s">
         <v>367</v>
       </c>
-      <c r="D40" s="126" t="s">
+      <c r="D49" s="97" t="s">
         <v>368</v>
       </c>
-      <c r="E40" s="126" t="str">
+      <c r="E49" s="97" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConFacebook=By.xpath("//*[@id="SLFacebook"]");</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="127" t="s">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="98" t="s">
         <v>364</v>
       </c>
-      <c r="B41" s="128" t="s">
+      <c r="B50" s="99" t="s">
         <v>232</v>
       </c>
-      <c r="C41" s="128" t="s">
+      <c r="C50" s="99" t="s">
         <v>369</v>
       </c>
-      <c r="D41" s="128" t="s">
+      <c r="D50" s="99" t="s">
         <v>370</v>
       </c>
-      <c r="E41" s="128" t="str">
+      <c r="E50" s="99" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConGoogle=By.xpath("//*[@id="SLGoogle"]");</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8718,7 +8934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E972679-EDA2-4ED9-97F5-E044AE9E5203}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -8887,16 +9103,16 @@
       <c r="A10" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="93" t="s">
         <v>403</v>
       </c>
-      <c r="D10" s="122" t="s">
+      <c r="D10" s="93" t="s">
         <v>404</v>
       </c>
-      <c r="E10" s="122" t="str">
+      <c r="E10" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnOtroValor=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[6]");</v>
       </c>
@@ -8905,16 +9121,16 @@
       <c r="A11" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="93" t="s">
         <v>405</v>
       </c>
-      <c r="D11" s="122" t="s">
+      <c r="D11" s="93" t="s">
         <v>406</v>
       </c>
-      <c r="E11" s="122" t="str">
+      <c r="E11" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtValorRecargar=By.id("edit-otro-valor");</v>
       </c>
@@ -8923,16 +9139,16 @@
       <c r="A12" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="93" t="s">
         <v>407</v>
       </c>
-      <c r="D12" s="122" t="s">
+      <c r="D12" s="93" t="s">
         <v>408</v>
       </c>
-      <c r="E12" s="122" t="str">
+      <c r="E12" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbErrorValor=By.xpath("//*[@id="other_value"]/div/div/div[1]/p");</v>
       </c>
@@ -8941,16 +9157,16 @@
       <c r="A13" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="93" t="s">
         <v>255</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="122" t="str">
+      <c r="E13" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCorreoElectronico=By.id("edit-email");</v>
       </c>
@@ -8959,70 +9175,70 @@
       <c r="A14" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B14" s="122" t="s">
+      <c r="B14" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="93" t="s">
         <v>409</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="D14" s="93" t="s">
         <v>410</v>
       </c>
-      <c r="E14" s="122" t="str">
+      <c r="E14" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnRecargar=By.id("edit-button-recargar");</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="101" t="s">
         <v>411</v>
       </c>
-      <c r="D15" s="130" t="s">
+      <c r="D15" s="101" t="s">
         <v>412</v>
       </c>
-      <c r="E15" s="130" t="str">
+      <c r="E15" s="101" t="str">
         <f t="shared" si="0"/>
         <v>public By lbResumenTransaccion=By.xpath("//*[@id="title-detail"]");</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="130" t="s">
+      <c r="B16" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="130" t="s">
+      <c r="C16" s="101" t="s">
         <v>413</v>
       </c>
-      <c r="D16" s="130" t="s">
+      <c r="D16" s="101" t="s">
         <v>414</v>
       </c>
-      <c r="E16" s="130" t="str">
+      <c r="E16" s="101" t="str">
         <f t="shared" si="0"/>
         <v>public By lbNumeroDelProducto=By.id("product-number");</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="131" t="s">
+      <c r="A17" s="102" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="132" t="s">
+      <c r="B17" s="103" t="s">
         <v>236</v>
       </c>
-      <c r="C17" s="132" t="s">
+      <c r="C17" s="103" t="s">
         <v>280</v>
       </c>
-      <c r="D17" s="132" t="s">
+      <c r="D17" s="103" t="s">
         <v>415</v>
       </c>
-      <c r="E17" s="132" t="str">
+      <c r="E17" s="103" t="str">
         <f t="shared" si="0"/>
         <v>public By lbValorPagar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]");</v>
       </c>

</xml_diff>

<commit_message>
Se agregan los objetos de la página de Paquetes
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasprilla\Documents\automatizacion_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391733F1-CCED-4BE4-BD82-A9A8811F524B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9968BD8-128A-4624-A156-0C9DBD449D43}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ObjetosPasarela" sheetId="5" r:id="rId5"/>
     <sheet name="ObjetosMiCuenta" sheetId="6" r:id="rId6"/>
     <sheet name="ObjetosRecargas" sheetId="7" r:id="rId7"/>
+    <sheet name="Objetos Paquetes" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ObjetosPasarela!$A$2:$D$77</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="502">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -1197,9 +1198,6 @@
     <t>MsgErrorDocumento</t>
   </si>
   <si>
-    <t>Listado de Objetos en el proceso Recargas y Paquetes</t>
-  </si>
-  <si>
     <t>Recargas</t>
   </si>
   <si>
@@ -1336,6 +1334,213 @@
   </si>
   <si>
     <t>//*[@id='compras-noplan-container']/p</t>
+  </si>
+  <si>
+    <t>Listado de Objetos en el proceso Paquetes</t>
+  </si>
+  <si>
+    <t>Listado de Objetos en el proceso Recargas</t>
+  </si>
+  <si>
+    <t>Paquetes</t>
+  </si>
+  <si>
+    <t>//*[@id="tap_selector"]/div[1]</t>
+  </si>
+  <si>
+    <t>Ofertas</t>
+  </si>
+  <si>
+    <t>Suscripciones</t>
+  </si>
+  <si>
+    <t>//*[@id="ofertas"]</t>
+  </si>
+  <si>
+    <t>//*[@id="suscripciones"]</t>
+  </si>
+  <si>
+    <t>FlechaAtras</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[1]</t>
+  </si>
+  <si>
+    <t>FlechaAdelante</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[2]</t>
+  </si>
+  <si>
+    <t>Comprar600MB</t>
+  </si>
+  <si>
+    <t>Comprar350MB</t>
+  </si>
+  <si>
+    <t>Comprar40MB</t>
+  </si>
+  <si>
+    <t>Comprar100MB</t>
+  </si>
+  <si>
+    <t>Comprar2GB15Dias</t>
+  </si>
+  <si>
+    <t>Comprar2GB30Dias</t>
+  </si>
+  <si>
+    <t>Comprar150MB</t>
+  </si>
+  <si>
+    <t>Comprar120MB</t>
+  </si>
+  <si>
+    <t>Comprar1GB</t>
+  </si>
+  <si>
+    <t>Comprar500MB</t>
+  </si>
+  <si>
+    <t>Comprar50MB</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[1]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[2]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[3]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[4]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[5]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[6]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[7]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[8]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[9]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[10]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[11]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>ComprarSuscripcion1GB</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[1]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>ComprarSuscripcion2GB</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[2]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>IngresaTuLineaTigo</t>
+  </si>
+  <si>
+    <t>numlinsin</t>
+  </si>
+  <si>
+    <t>ContinuarCompraPaquete</t>
+  </si>
+  <si>
+    <t>bt-regsinbal</t>
+  </si>
+  <si>
+    <t>CodigoVerificacion</t>
+  </si>
+  <si>
+    <t>cod_act</t>
+  </si>
+  <si>
+    <t>ErrorCodigoVerificacion</t>
+  </si>
+  <si>
+    <t>//*[@id="mod_regnumber"]/div[3]/div[1]/div/div/div[1]/p</t>
+  </si>
+  <si>
+    <t>ContinuarVerificacion</t>
+  </si>
+  <si>
+    <t>bt-contver</t>
+  </si>
+  <si>
+    <t>ErrorMSISDN</t>
+  </si>
+  <si>
+    <t>//*[@id="wrrp_step1"]/div/p</t>
+  </si>
+  <si>
+    <t>CorreoVerificacion</t>
+  </si>
+  <si>
+    <t>emailpackages</t>
+  </si>
+  <si>
+    <t>EstoySeguro</t>
+  </si>
+  <si>
+    <t>bt-buyconfirmation</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[1]/b</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[3]</t>
+  </si>
+  <si>
+    <t>//*[@id="payment-method-type-label-credit-payu"]/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="payment-method-type-label-debit-payu"]/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>AdelantaSaldo</t>
+  </si>
+  <si>
+    <t>//*[@id="payment-method-type-label-advance-balance"]/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>TeQuedasteSinSaldo</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div/div/h1</t>
+  </si>
+  <si>
+    <t>AdelantarSaldo</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div/div/button</t>
+  </si>
+  <si>
+    <t>CambiarDeLinea</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tieneinformaciondesaldoydeudadelmsisdn"]/div/div[2]/div/div/div/div[2]/div[1]/a</t>
+  </si>
+  <si>
+    <t>VerMisSuscripciones</t>
+  </si>
+  <si>
+    <t>//*[@id="suscriptions_trigger"]/a</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1591,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1492,6 +1697,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1662,7 +1873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2023,6 +2234,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6568,8 +6815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8020,7 +8267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDA504D-8FF2-405F-AE1B-22086E468A89}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
@@ -8679,10 +8926,10 @@
         <v>234</v>
       </c>
       <c r="C37" s="95" t="s">
+        <v>415</v>
+      </c>
+      <c r="D37" s="95" t="s">
         <v>416</v>
-      </c>
-      <c r="D37" s="95" t="s">
-        <v>417</v>
       </c>
       <c r="E37" s="95" t="str">
         <f t="shared" si="7"/>
@@ -8697,10 +8944,10 @@
         <v>234</v>
       </c>
       <c r="C38" s="95" t="s">
+        <v>417</v>
+      </c>
+      <c r="D38" s="95" t="s">
         <v>418</v>
-      </c>
-      <c r="D38" s="95" t="s">
-        <v>419</v>
       </c>
       <c r="E38" s="95" t="str">
         <f t="shared" ref="E38" si="8">CONCATENATE("public By ",B38,C38,"=By.",IF(ISNUMBER(SEARCH("@id=",D38)),"xpath(""","id("""),D38,""");")</f>
@@ -8715,10 +8962,10 @@
         <v>234</v>
       </c>
       <c r="C39" s="95" t="s">
+        <v>419</v>
+      </c>
+      <c r="D39" s="95" t="s">
         <v>420</v>
-      </c>
-      <c r="D39" s="95" t="s">
-        <v>421</v>
       </c>
       <c r="E39" s="95" t="str">
         <f t="shared" si="7"/>
@@ -8769,10 +9016,10 @@
         <v>235</v>
       </c>
       <c r="C42" s="95" t="s">
+        <v>421</v>
+      </c>
+      <c r="D42" s="95" t="s">
         <v>422</v>
-      </c>
-      <c r="D42" s="95" t="s">
-        <v>423</v>
       </c>
       <c r="E42" s="95" t="str">
         <f t="shared" si="9"/>
@@ -8787,10 +9034,10 @@
         <v>235</v>
       </c>
       <c r="C43" s="95" t="s">
+        <v>423</v>
+      </c>
+      <c r="D43" s="95" t="s">
         <v>424</v>
-      </c>
-      <c r="D43" s="95" t="s">
-        <v>425</v>
       </c>
       <c r="E43" s="95" t="str">
         <f t="shared" si="9"/>
@@ -8805,10 +9052,10 @@
         <v>232</v>
       </c>
       <c r="C44" s="95" t="s">
+        <v>425</v>
+      </c>
+      <c r="D44" s="95" t="s">
         <v>426</v>
-      </c>
-      <c r="D44" s="95" t="s">
-        <v>427</v>
       </c>
       <c r="E44" s="95" t="str">
         <f t="shared" si="9"/>
@@ -8823,10 +9070,10 @@
         <v>236</v>
       </c>
       <c r="C45" s="95" t="s">
+        <v>427</v>
+      </c>
+      <c r="D45" s="95" t="s">
         <v>428</v>
-      </c>
-      <c r="D45" s="95" t="s">
-        <v>429</v>
       </c>
       <c r="E45" s="95" t="str">
         <f t="shared" si="9"/>
@@ -8841,10 +9088,10 @@
         <v>236</v>
       </c>
       <c r="C46" s="95" t="s">
+        <v>429</v>
+      </c>
+      <c r="D46" s="95" t="s">
         <v>430</v>
-      </c>
-      <c r="D46" s="95" t="s">
-        <v>431</v>
       </c>
       <c r="E46" s="95" t="str">
         <f t="shared" si="9"/>
@@ -8859,10 +9106,10 @@
         <v>236</v>
       </c>
       <c r="C47" s="95" t="s">
+        <v>431</v>
+      </c>
+      <c r="D47" s="95" t="s">
         <v>432</v>
-      </c>
-      <c r="D47" s="95" t="s">
-        <v>433</v>
       </c>
       <c r="E47" s="95" t="str">
         <f t="shared" si="0"/>
@@ -8934,8 +9181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E972679-EDA2-4ED9-97F5-E044AE9E5203}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="E40" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8949,7 +9196,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="89" t="s">
-        <v>387</v>
+        <v>434</v>
       </c>
       <c r="B1" s="90"/>
       <c r="C1" s="90"/>
@@ -8975,16 +9222,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C3" s="48" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>389</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>390</v>
       </c>
       <c r="E3" s="48" t="str">
         <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
@@ -8993,16 +9240,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>235</v>
       </c>
       <c r="C4" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>391</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>392</v>
       </c>
       <c r="E4" s="48" t="str">
         <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
@@ -9011,16 +9258,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B5" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C5" s="48" t="s">
+        <v>392</v>
+      </c>
+      <c r="D5" s="48" t="s">
         <v>393</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>394</v>
       </c>
       <c r="E5" s="48" t="str">
         <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
@@ -9029,16 +9276,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C6" s="50" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6" s="48" t="s">
         <v>395</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>396</v>
       </c>
       <c r="E6" s="48" t="str">
         <f t="shared" ref="E6:E69" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
@@ -9047,16 +9294,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C7" s="48" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="48" t="s">
         <v>397</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>398</v>
       </c>
       <c r="E7" s="48" t="str">
         <f t="shared" si="0"/>
@@ -9065,16 +9312,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C8" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="D8" s="48" t="s">
         <v>399</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>400</v>
       </c>
       <c r="E8" s="48" t="str">
         <f t="shared" si="0"/>
@@ -9083,16 +9330,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B9" s="91" t="s">
         <v>232</v>
       </c>
       <c r="C9" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="D9" s="91" t="s">
         <v>401</v>
-      </c>
-      <c r="D9" s="91" t="s">
-        <v>402</v>
       </c>
       <c r="E9" s="91" t="str">
         <f t="shared" si="0"/>
@@ -9101,16 +9348,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B10" s="93" t="s">
         <v>232</v>
       </c>
       <c r="C10" s="93" t="s">
+        <v>402</v>
+      </c>
+      <c r="D10" s="93" t="s">
         <v>403</v>
-      </c>
-      <c r="D10" s="93" t="s">
-        <v>404</v>
       </c>
       <c r="E10" s="93" t="str">
         <f t="shared" si="0"/>
@@ -9119,16 +9366,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B11" s="93" t="s">
         <v>235</v>
       </c>
       <c r="C11" s="93" t="s">
+        <v>404</v>
+      </c>
+      <c r="D11" s="93" t="s">
         <v>405</v>
-      </c>
-      <c r="D11" s="93" t="s">
-        <v>406</v>
       </c>
       <c r="E11" s="93" t="str">
         <f t="shared" si="0"/>
@@ -9137,16 +9384,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B12" s="93" t="s">
         <v>236</v>
       </c>
       <c r="C12" s="93" t="s">
+        <v>406</v>
+      </c>
+      <c r="D12" s="93" t="s">
         <v>407</v>
-      </c>
-      <c r="D12" s="93" t="s">
-        <v>408</v>
       </c>
       <c r="E12" s="93" t="str">
         <f t="shared" si="0"/>
@@ -9155,7 +9402,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B13" s="93" t="s">
         <v>235</v>
@@ -9173,16 +9420,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B14" s="93" t="s">
         <v>232</v>
       </c>
       <c r="C14" s="93" t="s">
+        <v>408</v>
+      </c>
+      <c r="D14" s="93" t="s">
         <v>409</v>
-      </c>
-      <c r="D14" s="93" t="s">
-        <v>410</v>
       </c>
       <c r="E14" s="93" t="str">
         <f t="shared" si="0"/>
@@ -9197,10 +9444,10 @@
         <v>236</v>
       </c>
       <c r="C15" s="101" t="s">
+        <v>410</v>
+      </c>
+      <c r="D15" s="101" t="s">
         <v>411</v>
-      </c>
-      <c r="D15" s="101" t="s">
-        <v>412</v>
       </c>
       <c r="E15" s="101" t="str">
         <f t="shared" si="0"/>
@@ -9215,10 +9462,10 @@
         <v>236</v>
       </c>
       <c r="C16" s="101" t="s">
+        <v>412</v>
+      </c>
+      <c r="D16" s="101" t="s">
         <v>413</v>
-      </c>
-      <c r="D16" s="101" t="s">
-        <v>414</v>
       </c>
       <c r="E16" s="101" t="str">
         <f t="shared" si="0"/>
@@ -9236,7 +9483,7 @@
         <v>280</v>
       </c>
       <c r="D17" s="103" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E17" s="103" t="str">
         <f t="shared" si="0"/>
@@ -10235,5 +10482,1279 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079AA414-3B09-4B31-AC8E-D4CF306B3AF3}">
+  <dimension ref="A1:E70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="92" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="131.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>436</v>
+      </c>
+      <c r="E3" s="48" t="str">
+        <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
+        <v>public By btnPaquetes=By.xpath("//*[@id="tap_selector"]/div[1]");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>437</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="E4" s="48" t="str">
+        <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
+        <v>public By btnOfertas=By.xpath("//*[@id="ofertas"]");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>440</v>
+      </c>
+      <c r="E5" s="48" t="str">
+        <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
+        <v>public By btnSuscripciones=By.xpath("//*[@id="suscripciones"]");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>471</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>472</v>
+      </c>
+      <c r="E6" s="48" t="str">
+        <f>CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <v>public By txtIngresaTuLineaTigo=By.id("numlinsin");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>481</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>482</v>
+      </c>
+      <c r="E7" s="48" t="str">
+        <f>CONCATENATE("public By ",B7,C7,"=By.",IF(ISNUMBER(SEARCH("@id=",D7)),"xpath(""","id("""),D7,""");")</f>
+        <v>public By lbErrorMSISDN=By.xpath("//*[@id="wrrp_step1"]/div/p");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>473</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>474</v>
+      </c>
+      <c r="E8" s="48" t="str">
+        <f>CONCATENATE("public By ",B8,C8,"=By.",IF(ISNUMBER(SEARCH("@id=",D8)),"xpath(""","id("""),D8,""");")</f>
+        <v>public By btnContinuarCompraPaquete=By.id("bt-regsinbal");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>475</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>476</v>
+      </c>
+      <c r="E9" s="48" t="str">
+        <f>CONCATENATE("public By ",B9,C9,"=By.",IF(ISNUMBER(SEARCH("@id=",D9)),"xpath(""","id("""),D9,""");")</f>
+        <v>public By txtCodigoVerificacion=By.id("cod_act");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>477</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>478</v>
+      </c>
+      <c r="E10" s="48" t="str">
+        <f>CONCATENATE("public By ",B10,C10,"=By.",IF(ISNUMBER(SEARCH("@id=",D10)),"xpath(""","id("""),D10,""");")</f>
+        <v>public By lbErrorCodigoVerificacion=By.xpath("//*[@id="mod_regnumber"]/div[3]/div[1]/div/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>479</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>480</v>
+      </c>
+      <c r="E11" s="48" t="str">
+        <f>CONCATENATE("public By ",B11,C11,"=By.",IF(ISNUMBER(SEARCH("@id=",D11)),"xpath(""","id("""),D11,""");")</f>
+        <v>public By btnContinuarVerificacion=By.id("bt-contver");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>483</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>484</v>
+      </c>
+      <c r="E12" s="48" t="str">
+        <f>CONCATENATE("public By ",B12,C12,"=By.",IF(ISNUMBER(SEARCH("@id=",D12)),"xpath(""","id("""),D12,""");")</f>
+        <v>public By txtCorreoVerificacion=By.id("emailpackages");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>486</v>
+      </c>
+      <c r="E13" s="48" t="str">
+        <f>CONCATENATE("public By ",B13,C13,"=By.",IF(ISNUMBER(SEARCH("@id=",D13)),"xpath(""","id("""),D13,""");")</f>
+        <v>public By btnEstoySeguro=By.id("bt-buyconfirmation");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>498</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>499</v>
+      </c>
+      <c r="E14" s="48" t="str">
+        <f>CONCATENATE("public By ",B14,C14,"=By.",IF(ISNUMBER(SEARCH("@id=",D14)),"xpath(""","id("""),D14,""");")</f>
+        <v>public By btnCambiarDeLinea=By.xpath("//*[@id="block-tieneinformaciondesaldoydeudadelmsisdn"]/div/div[2]/div/div/div/div[2]/div[1]/a");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>500</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>501</v>
+      </c>
+      <c r="E15" s="48" t="str">
+        <f>CONCATENATE("public By ",B15,C15,"=By.",IF(ISNUMBER(SEARCH("@id=",D15)),"xpath(""","id("""),D15,""");")</f>
+        <v>public By btnVerMisSuscripciones=By.xpath("//*[@id="suscriptions_trigger"]/a");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B16" s="133" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="134" t="s">
+        <v>441</v>
+      </c>
+      <c r="D16" s="133" t="s">
+        <v>442</v>
+      </c>
+      <c r="E16" s="133" t="str">
+        <f t="shared" ref="E16:E24" si="0">CONCATENATE("public By ",B16,C16,"=By.",IF(ISNUMBER(SEARCH("@id=",D16)),"xpath(""","id("""),D16,""");")</f>
+        <v>public By btnFlechaAtras=By.xpath("//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[1]");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B17" s="133" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="133" t="s">
+        <v>443</v>
+      </c>
+      <c r="D17" s="133" t="s">
+        <v>444</v>
+      </c>
+      <c r="E17" s="133" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnFlechaAdelante=By.xpath("//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[2]");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B18" s="133" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" s="133" t="s">
+        <v>445</v>
+      </c>
+      <c r="D18" s="133" t="s">
+        <v>456</v>
+      </c>
+      <c r="E18" s="133" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar600MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[1]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B19" s="135" t="s">
+        <v>232</v>
+      </c>
+      <c r="C19" s="133" t="s">
+        <v>446</v>
+      </c>
+      <c r="D19" s="135" t="s">
+        <v>457</v>
+      </c>
+      <c r="E19" s="135" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar350MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[2]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B20" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" s="95" t="s">
+        <v>450</v>
+      </c>
+      <c r="D20" s="95" t="s">
+        <v>458</v>
+      </c>
+      <c r="E20" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar2GB30Dias=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[3]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B21" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C21" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="D21" s="95" t="s">
+        <v>459</v>
+      </c>
+      <c r="E21" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar40MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[4]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B22" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C22" s="95" t="s">
+        <v>448</v>
+      </c>
+      <c r="D22" s="95" t="s">
+        <v>460</v>
+      </c>
+      <c r="E22" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar100MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[5]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B23" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="95" t="s">
+        <v>449</v>
+      </c>
+      <c r="D23" s="95" t="s">
+        <v>461</v>
+      </c>
+      <c r="E23" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar2GB15Dias=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[6]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B24" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C24" s="95" t="s">
+        <v>451</v>
+      </c>
+      <c r="D24" s="136" t="s">
+        <v>462</v>
+      </c>
+      <c r="E24" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar150MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[7]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B25" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="95" t="s">
+        <v>452</v>
+      </c>
+      <c r="D25" s="136" t="s">
+        <v>463</v>
+      </c>
+      <c r="E25" s="136" t="str">
+        <f t="shared" ref="E25:E26" si="1">CONCATENATE("public By ",B25,C25,"=By.",IF(ISNUMBER(SEARCH("@id=",D25)),"xpath(""","id("""),D25,""");")</f>
+        <v>public By btnComprar120MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[8]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B26" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="95" t="s">
+        <v>453</v>
+      </c>
+      <c r="D26" s="136" t="s">
+        <v>464</v>
+      </c>
+      <c r="E26" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnComprar1GB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[9]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B27" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C27" s="95" t="s">
+        <v>455</v>
+      </c>
+      <c r="D27" s="136" t="s">
+        <v>465</v>
+      </c>
+      <c r="E27" s="136" t="str">
+        <f t="shared" ref="E27" si="2">CONCATENATE("public By ",B27,C27,"=By.",IF(ISNUMBER(SEARCH("@id=",D27)),"xpath(""","id("""),D27,""");")</f>
+        <v>public By btnComprar50MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[10]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="137" t="s">
+        <v>437</v>
+      </c>
+      <c r="B28" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="136" t="s">
+        <v>454</v>
+      </c>
+      <c r="D28" s="136" t="s">
+        <v>466</v>
+      </c>
+      <c r="E28" s="136" t="str">
+        <f t="shared" ref="E28" si="3">CONCATENATE("public By ",B28,C28,"=By.",IF(ISNUMBER(SEARCH("@id=",D28)),"xpath(""","id("""),D28,""");")</f>
+        <v>public By btnComprar500MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[11]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="138" t="s">
+        <v>438</v>
+      </c>
+      <c r="B29" s="139" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" s="139" t="s">
+        <v>467</v>
+      </c>
+      <c r="D29" s="139" t="s">
+        <v>468</v>
+      </c>
+      <c r="E29" s="139" t="str">
+        <f t="shared" ref="E29" si="4">CONCATENATE("public By ",B29,C29,"=By.",IF(ISNUMBER(SEARCH("@id=",D29)),"xpath(""","id("""),D29,""");")</f>
+        <v>public By btnComprarSuscripcion1GB=By.xpath("//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[1]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="138" t="s">
+        <v>438</v>
+      </c>
+      <c r="B30" s="139" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="139" t="s">
+        <v>469</v>
+      </c>
+      <c r="D30" s="139" t="s">
+        <v>470</v>
+      </c>
+      <c r="E30" s="139" t="str">
+        <f t="shared" ref="E30:E70" si="5">CONCATENATE("public By ",B30,C30,"=By.",IF(ISNUMBER(SEARCH("@id=",D30)),"xpath(""","id("""),D30,""");")</f>
+        <v>public By btnComprarSuscripcion2GB=By.xpath("//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[2]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="101" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="101" t="s">
+        <v>410</v>
+      </c>
+      <c r="D31" s="101" t="s">
+        <v>487</v>
+      </c>
+      <c r="E31" s="101" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbResumenTransaccion=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="101" t="s">
+        <v>236</v>
+      </c>
+      <c r="C32" s="101" t="s">
+        <v>412</v>
+      </c>
+      <c r="D32" s="101" t="s">
+        <v>488</v>
+      </c>
+      <c r="E32" s="101" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbNumeroDelProducto=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[1]/b");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="103" t="s">
+        <v>236</v>
+      </c>
+      <c r="C33" s="103" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" s="103" t="s">
+        <v>489</v>
+      </c>
+      <c r="E33" s="103" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbValorPagar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[3]");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>490</v>
+      </c>
+      <c r="E34" s="34" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkTarjetaCredito=By.xpath("//*[@id="payment-method-type-label-credit-payu"]/label/div[1]/div[1]");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>491</v>
+      </c>
+      <c r="E35" s="34" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkDebitoBancarioPSE=By.xpath("//*[@id="payment-method-type-label-debit-payu"]/label/div[1]/div[1]");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="140" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>492</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="E36" s="34" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkAdelantaSaldo=By.xpath("//*[@id="payment-method-type-label-advance-balance"]/label/div[1]/div[1]");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtCVV/CVC=By.id("edit-cvc");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listCuotas=By.id("edit-cardnumber-quota");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNombre=By.id("edit-ccname");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listTipo=By.id("edit-buyer-document-type");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone");</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail");</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E51" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize");</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="E53" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnCancelar=By.id("edit-cancel");</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="D55" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit");</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="142" t="s">
+        <v>234</v>
+      </c>
+      <c r="C56" s="142" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="142" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listBanco=By.id("edit-bank");</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="142" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="142" t="s">
+        <v>244</v>
+      </c>
+      <c r="D57" s="142" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listTipodepersona=By.id("edit-buyer-type-person");</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="142" t="s">
+        <v>235</v>
+      </c>
+      <c r="C58" s="142" t="s">
+        <v>245</v>
+      </c>
+      <c r="D58" s="142" t="s">
+        <v>57</v>
+      </c>
+      <c r="E58" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNombresyapellidos=By.id("edit-buyer-name");</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="142" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" s="142" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="142" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listTipo=By.id("edit-buyer-document-type--2");</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="142" t="s">
+        <v>235</v>
+      </c>
+      <c r="C60" s="142" t="s">
+        <v>246</v>
+      </c>
+      <c r="D60" s="142" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2");</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="142" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" s="142" t="s">
+        <v>264</v>
+      </c>
+      <c r="D61" s="142" t="s">
+        <v>286</v>
+      </c>
+      <c r="E61" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p");</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="142" t="s">
+        <v>235</v>
+      </c>
+      <c r="C62" s="142" t="s">
+        <v>257</v>
+      </c>
+      <c r="D62" s="142" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2");</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="142" t="s">
+        <v>236</v>
+      </c>
+      <c r="C63" s="142" t="s">
+        <v>256</v>
+      </c>
+      <c r="D63" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="E63" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p");</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="142" t="s">
+        <v>233</v>
+      </c>
+      <c r="C64" s="142" t="s">
+        <v>270</v>
+      </c>
+      <c r="D64" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="E64" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a");</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" s="142" t="s">
+        <v>232</v>
+      </c>
+      <c r="C65" s="142" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="142" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnCancelar=By.id("edit-cancel--2");</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="143" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="142" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" s="142" t="s">
+        <v>247</v>
+      </c>
+      <c r="D66" s="142" t="s">
+        <v>65</v>
+      </c>
+      <c r="E66" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2");</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="B67" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>494</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>495</v>
+      </c>
+      <c r="E67" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbTeQuedasteSinSaldo=By.xpath("//*[@id="modal"]/div/div/h1");</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="B68" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>496</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>497</v>
+      </c>
+      <c r="E68" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnAdelantarSaldo=By.xpath("//*[@id="modal"]/div/div/button");</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="B69" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E69" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel");</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="144" t="s">
+        <v>492</v>
+      </c>
+      <c r="B70" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C70" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E70" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnPagar=By.id("tigoune-nequi-button-submit");</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se añaden los objetos de la página de Paquetes
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasprilla\Documents\automatizacion_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B91DB4-8B3F-401D-87B1-5470BFBB51A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9968BD8-128A-4624-A156-0C9DBD449D43}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ObjetosPasarela" sheetId="5" r:id="rId5"/>
     <sheet name="ObjetosMiCuenta" sheetId="6" r:id="rId6"/>
     <sheet name="ObjetosRecargas" sheetId="7" r:id="rId7"/>
+    <sheet name="Objetos Paquetes" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ObjetosPasarela!$A$2:$D$77</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="502">
   <si>
     <t>Listado de Objetos en el proceso de pago de Facturas Móviles</t>
   </si>
@@ -1197,9 +1198,6 @@
     <t>MsgErrorDocumento</t>
   </si>
   <si>
-    <t>Listado de Objetos en el proceso Recargas y Paquetes</t>
-  </si>
-  <si>
     <t>Recargas</t>
   </si>
   <si>
@@ -1282,6 +1280,267 @@
   </si>
   <si>
     <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]</t>
+  </si>
+  <si>
+    <t>LineaPruebasJuanca</t>
+  </si>
+  <si>
+    <t>(((//*[@id='lines'])//a[contains(@href,'')]))[11]</t>
+  </si>
+  <si>
+    <t>LineaHibridoMariana</t>
+  </si>
+  <si>
+    <t>(((((//*[@id='lines'])//a[contains(@href,'')])))//*[contains(text(),'Mariana')])[2]</t>
+  </si>
+  <si>
+    <t>LineaHibridoAna</t>
+  </si>
+  <si>
+    <t>(((//*[@id='lines'])//a[contains(@href,'')]))[9]</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>//*[@id='top_menu_aside']/nav/ul/li/a</t>
+  </si>
+  <si>
+    <t>CerrarSesion</t>
+  </si>
+  <si>
+    <t>//*[@id='top_menu_aside']/nav/ul/li/ul/li[2]/a</t>
+  </si>
+  <si>
+    <t>CambiarCuenta</t>
+  </si>
+  <si>
+    <t>//*[@id='addNew']</t>
+  </si>
+  <si>
+    <t>Planes</t>
+  </si>
+  <si>
+    <t>//*[@id='main-content']/div[2]</t>
+  </si>
+  <si>
+    <t>MejorarPlan</t>
+  </si>
+  <si>
+    <t>//*[@id='compras-noplan-container']/h3</t>
+  </si>
+  <si>
+    <t>DetallePlan</t>
+  </si>
+  <si>
+    <t>//*[@id='compras-noplan-container']/p</t>
+  </si>
+  <si>
+    <t>Listado de Objetos en el proceso Paquetes</t>
+  </si>
+  <si>
+    <t>Listado de Objetos en el proceso Recargas</t>
+  </si>
+  <si>
+    <t>Paquetes</t>
+  </si>
+  <si>
+    <t>//*[@id="tap_selector"]/div[1]</t>
+  </si>
+  <si>
+    <t>Ofertas</t>
+  </si>
+  <si>
+    <t>Suscripciones</t>
+  </si>
+  <si>
+    <t>//*[@id="ofertas"]</t>
+  </si>
+  <si>
+    <t>//*[@id="suscripciones"]</t>
+  </si>
+  <si>
+    <t>FlechaAtras</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[1]</t>
+  </si>
+  <si>
+    <t>FlechaAdelante</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[2]</t>
+  </si>
+  <si>
+    <t>Comprar600MB</t>
+  </si>
+  <si>
+    <t>Comprar350MB</t>
+  </si>
+  <si>
+    <t>Comprar40MB</t>
+  </si>
+  <si>
+    <t>Comprar100MB</t>
+  </si>
+  <si>
+    <t>Comprar2GB15Dias</t>
+  </si>
+  <si>
+    <t>Comprar2GB30Dias</t>
+  </si>
+  <si>
+    <t>Comprar150MB</t>
+  </si>
+  <si>
+    <t>Comprar120MB</t>
+  </si>
+  <si>
+    <t>Comprar1GB</t>
+  </si>
+  <si>
+    <t>Comprar500MB</t>
+  </si>
+  <si>
+    <t>Comprar50MB</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[1]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[2]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[3]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[4]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[5]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[6]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[7]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[8]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[9]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[10]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[11]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>ComprarSuscripcion1GB</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[1]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>ComprarSuscripcion2GB</t>
+  </si>
+  <si>
+    <t>//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[2]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>IngresaTuLineaTigo</t>
+  </si>
+  <si>
+    <t>numlinsin</t>
+  </si>
+  <si>
+    <t>ContinuarCompraPaquete</t>
+  </si>
+  <si>
+    <t>bt-regsinbal</t>
+  </si>
+  <si>
+    <t>CodigoVerificacion</t>
+  </si>
+  <si>
+    <t>cod_act</t>
+  </si>
+  <si>
+    <t>ErrorCodigoVerificacion</t>
+  </si>
+  <si>
+    <t>//*[@id="mod_regnumber"]/div[3]/div[1]/div/div/div[1]/p</t>
+  </si>
+  <si>
+    <t>ContinuarVerificacion</t>
+  </si>
+  <si>
+    <t>bt-contver</t>
+  </si>
+  <si>
+    <t>ErrorMSISDN</t>
+  </si>
+  <si>
+    <t>//*[@id="wrrp_step1"]/div/p</t>
+  </si>
+  <si>
+    <t>CorreoVerificacion</t>
+  </si>
+  <si>
+    <t>emailpackages</t>
+  </si>
+  <si>
+    <t>EstoySeguro</t>
+  </si>
+  <si>
+    <t>bt-buyconfirmation</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[1]/b</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[3]</t>
+  </si>
+  <si>
+    <t>//*[@id="payment-method-type-label-credit-payu"]/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="payment-method-type-label-debit-payu"]/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>AdelantaSaldo</t>
+  </si>
+  <si>
+    <t>//*[@id="payment-method-type-label-advance-balance"]/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>TeQuedasteSinSaldo</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div/div/h1</t>
+  </si>
+  <si>
+    <t>AdelantarSaldo</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div/div/button</t>
+  </si>
+  <si>
+    <t>CambiarDeLinea</t>
+  </si>
+  <si>
+    <t>//*[@id="block-tieneinformaciondesaldoydeudadelmsisdn"]/div/div[2]/div/div/div/div[2]/div[1]/a</t>
+  </si>
+  <si>
+    <t>VerMisSuscripciones</t>
+  </si>
+  <si>
+    <t>//*[@id="suscriptions_trigger"]/a</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1591,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1438,6 +1697,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1608,7 +1873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1850,6 +2115,39 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1937,38 +2235,41 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2596,78 +2897,78 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="104" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="93"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="93"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="93"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="93"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="93"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="93"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
+      <c r="A20" s="104"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="93"/>
-      <c r="B21" s="93"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2700,17 +3001,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -4985,14 +5286,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5015,7 +5316,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="118" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -5035,7 +5336,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="108"/>
+      <c r="A4" s="119"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -5053,7 +5354,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="108"/>
+      <c r="A5" s="119"/>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -5071,7 +5372,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
+      <c r="A6" s="119"/>
       <c r="B6" s="3" t="s">
         <v>101</v>
       </c>
@@ -5089,7 +5390,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="108"/>
+      <c r="A7" s="119"/>
       <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
@@ -5110,7 +5411,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="108"/>
+      <c r="A8" s="119"/>
       <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
@@ -5131,7 +5432,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="109"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="3" t="s">
         <v>229</v>
       </c>
@@ -5149,7 +5450,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="127" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -5169,7 +5470,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="117"/>
+      <c r="A11" s="128"/>
       <c r="B11" s="7" t="s">
         <v>124</v>
       </c>
@@ -5190,7 +5491,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="117"/>
+      <c r="A12" s="128"/>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -5208,7 +5509,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="117"/>
+      <c r="A13" s="128"/>
       <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
@@ -5229,7 +5530,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
+      <c r="A14" s="128"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -5247,7 +5548,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+      <c r="A15" s="128"/>
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -5265,7 +5566,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="117"/>
+      <c r="A16" s="128"/>
       <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
@@ -5283,7 +5584,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="117"/>
+      <c r="A17" s="128"/>
       <c r="B17" s="7" t="s">
         <v>101</v>
       </c>
@@ -5301,7 +5602,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="117"/>
+      <c r="A18" s="128"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -5319,7 +5620,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
+      <c r="A19" s="129"/>
       <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
@@ -5337,7 +5638,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="101" t="s">
+      <c r="A20" s="112" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -5357,7 +5658,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="102"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="4" t="s">
         <v>81</v>
       </c>
@@ -5382,7 +5683,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="102"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
@@ -5400,7 +5701,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="102"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="4" t="s">
         <v>82</v>
       </c>
@@ -5418,7 +5719,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
+      <c r="A24" s="114"/>
       <c r="B24" s="4" t="s">
         <v>83</v>
       </c>
@@ -5443,7 +5744,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="104" t="s">
+      <c r="A25" s="115" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -5463,7 +5764,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="105"/>
+      <c r="A26" s="116"/>
       <c r="B26" s="13" t="s">
         <v>27</v>
       </c>
@@ -5481,7 +5782,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="106"/>
+      <c r="A27" s="117"/>
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -5499,7 +5800,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="130" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5519,7 +5820,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="120"/>
+      <c r="A29" s="131"/>
       <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
@@ -5540,7 +5841,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="120"/>
+      <c r="A30" s="131"/>
       <c r="B30" s="15" t="s">
         <v>118</v>
       </c>
@@ -5561,7 +5862,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="120"/>
+      <c r="A31" s="131"/>
       <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
@@ -5579,7 +5880,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="120"/>
+      <c r="A32" s="131"/>
       <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
@@ -5597,7 +5898,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="120"/>
+      <c r="A33" s="131"/>
       <c r="B33" s="15" t="s">
         <v>35</v>
       </c>
@@ -5615,7 +5916,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="120"/>
+      <c r="A34" s="131"/>
       <c r="B34" s="15" t="s">
         <v>36</v>
       </c>
@@ -5633,7 +5934,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="120"/>
+      <c r="A35" s="131"/>
       <c r="B35" s="15" t="s">
         <v>39</v>
       </c>
@@ -5651,7 +5952,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="120"/>
+      <c r="A36" s="131"/>
       <c r="B36" s="15" t="s">
         <v>3</v>
       </c>
@@ -5669,7 +5970,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="120"/>
+      <c r="A37" s="131"/>
       <c r="B37" s="15" t="s">
         <v>42</v>
       </c>
@@ -5687,7 +5988,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="120"/>
+      <c r="A38" s="131"/>
       <c r="B38" s="15" t="s">
         <v>122</v>
       </c>
@@ -5708,7 +6009,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="120"/>
+      <c r="A39" s="131"/>
       <c r="B39" s="15" t="s">
         <v>44</v>
       </c>
@@ -5726,7 +6027,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="120"/>
+      <c r="A40" s="131"/>
       <c r="B40" s="15" t="s">
         <v>130</v>
       </c>
@@ -5747,7 +6048,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="120"/>
+      <c r="A41" s="131"/>
       <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
@@ -5765,7 +6066,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="120"/>
+      <c r="A42" s="131"/>
       <c r="B42" s="15" t="s">
         <v>110</v>
       </c>
@@ -5786,7 +6087,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="120"/>
+      <c r="A43" s="131"/>
       <c r="B43" s="15" t="s">
         <v>47</v>
       </c>
@@ -5802,7 +6103,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="120"/>
+      <c r="A44" s="131"/>
       <c r="B44" s="15" t="s">
         <v>101</v>
       </c>
@@ -5818,7 +6119,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="120"/>
+      <c r="A45" s="131"/>
       <c r="B45" s="15" t="s">
         <v>22</v>
       </c>
@@ -5836,7 +6137,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="121"/>
+      <c r="A46" s="132"/>
       <c r="B46" s="15" t="s">
         <v>51</v>
       </c>
@@ -5854,7 +6155,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="110" t="s">
+      <c r="A47" s="121" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -5874,7 +6175,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="111"/>
+      <c r="A48" s="122"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -5892,7 +6193,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="111"/>
+      <c r="A49" s="122"/>
       <c r="B49" s="5" t="s">
         <v>56</v>
       </c>
@@ -5910,7 +6211,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="111"/>
+      <c r="A50" s="122"/>
       <c r="B50" s="5" t="s">
         <v>3</v>
       </c>
@@ -5928,7 +6229,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="111"/>
+      <c r="A51" s="122"/>
       <c r="B51" s="5" t="s">
         <v>60</v>
       </c>
@@ -5946,7 +6247,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="111"/>
+      <c r="A52" s="122"/>
       <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
@@ -5964,7 +6265,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="111"/>
+      <c r="A53" s="122"/>
       <c r="B53" s="5" t="s">
         <v>101</v>
       </c>
@@ -5980,7 +6281,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="111"/>
+      <c r="A54" s="122"/>
       <c r="B54" s="5" t="s">
         <v>22</v>
       </c>
@@ -5998,7 +6299,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="112"/>
+      <c r="A55" s="123"/>
       <c r="B55" s="5" t="s">
         <v>64</v>
       </c>
@@ -6016,7 +6317,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="113" t="s">
+      <c r="A56" s="124" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -6036,7 +6337,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="114"/>
+      <c r="A57" s="125"/>
       <c r="B57" s="1" t="s">
         <v>101</v>
       </c>
@@ -6052,7 +6353,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="114"/>
+      <c r="A58" s="125"/>
       <c r="B58" s="1" t="s">
         <v>22</v>
       </c>
@@ -6070,7 +6371,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="115"/>
+      <c r="A59" s="126"/>
       <c r="B59" s="1" t="s">
         <v>48</v>
       </c>
@@ -6088,7 +6389,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="96" t="s">
+      <c r="A60" s="107" t="s">
         <v>136</v>
       </c>
       <c r="B60" s="23" t="s">
@@ -6111,7 +6412,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="97"/>
+      <c r="A61" s="108"/>
       <c r="B61" s="23" t="s">
         <v>137</v>
       </c>
@@ -6129,7 +6430,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="97"/>
+      <c r="A62" s="108"/>
       <c r="B62" s="23" t="s">
         <v>138</v>
       </c>
@@ -6147,7 +6448,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="97"/>
+      <c r="A63" s="108"/>
       <c r="B63" s="23" t="s">
         <v>139</v>
       </c>
@@ -6165,7 +6466,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="97"/>
+      <c r="A64" s="108"/>
       <c r="B64" s="23" t="s">
         <v>140</v>
       </c>
@@ -6183,7 +6484,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="97"/>
+      <c r="A65" s="108"/>
       <c r="B65" s="23" t="s">
         <v>141</v>
       </c>
@@ -6201,7 +6502,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="97"/>
+      <c r="A66" s="108"/>
       <c r="B66" s="23" t="s">
         <v>142</v>
       </c>
@@ -6219,7 +6520,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="97"/>
+      <c r="A67" s="108"/>
       <c r="B67" s="23" t="s">
         <v>143</v>
       </c>
@@ -6237,7 +6538,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="97"/>
+      <c r="A68" s="108"/>
       <c r="B68" s="23" t="s">
         <v>144</v>
       </c>
@@ -6255,7 +6556,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="97"/>
+      <c r="A69" s="108"/>
       <c r="B69" s="23" t="s">
         <v>145</v>
       </c>
@@ -6273,7 +6574,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="97"/>
+      <c r="A70" s="108"/>
       <c r="B70" s="23" t="s">
         <v>146</v>
       </c>
@@ -6291,7 +6592,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="97"/>
+      <c r="A71" s="108"/>
       <c r="B71" s="23" t="s">
         <v>147</v>
       </c>
@@ -6309,7 +6610,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="97"/>
+      <c r="A72" s="108"/>
       <c r="B72" s="23" t="s">
         <v>148</v>
       </c>
@@ -6327,7 +6628,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="97"/>
+      <c r="A73" s="108"/>
       <c r="B73" s="23" t="s">
         <v>149</v>
       </c>
@@ -6345,7 +6646,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="98"/>
+      <c r="A74" s="109"/>
       <c r="B74" s="23" t="s">
         <v>150</v>
       </c>
@@ -6514,8 +6815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7964,10 +8265,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDA504D-8FF2-405F-AE1B-22086E468A89}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7976,7 +8277,7 @@
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="75.42578125" customWidth="1"/>
-    <col min="5" max="5" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="114.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8073,7 +8374,7 @@
         <v>316</v>
       </c>
       <c r="E6" s="48" t="str">
-        <f t="shared" ref="E6:E41" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <f t="shared" ref="E6:E50" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
         <v>public By btnIngresar=By.xpath("//*[@id="main-content"]/div[2]/div[2]/div/div/div/section/div[3]/a[2]");</v>
       </c>
     </row>
@@ -8135,16 +8436,16 @@
       <c r="A10" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="93" t="s">
         <v>323</v>
       </c>
-      <c r="D10" s="122" t="s">
+      <c r="D10" s="93" t="s">
         <v>324</v>
       </c>
-      <c r="E10" s="122" t="str">
+      <c r="E10" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnReponeTuSim=By.xpath("//*[@id="main-content"]/div[2]/div[6]/div/div/div/div/a");</v>
       </c>
@@ -8153,16 +8454,16 @@
       <c r="A11" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="93" t="s">
         <v>325</v>
       </c>
-      <c r="D11" s="122" t="s">
+      <c r="D11" s="93" t="s">
         <v>326</v>
       </c>
-      <c r="E11" s="122" t="str">
+      <c r="E11" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCambiarMiClave=By.xpath("//*[@id="main-content"]/div[2]/div[7]/div/div/div/div/div[2]/a");</v>
       </c>
@@ -8171,16 +8472,16 @@
       <c r="A12" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="93" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="122" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="122" t="s">
+      <c r="C12" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="93" t="s">
         <v>327</v>
       </c>
-      <c r="E12" s="122" t="str">
+      <c r="E12" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By listTipo=By.xpath("//*[@id="t_document"]/div/div/input");</v>
       </c>
@@ -8189,16 +8490,16 @@
       <c r="A13" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="93" t="s">
         <v>276</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="93" t="s">
         <v>328</v>
       </c>
-      <c r="E13" s="122" t="str">
+      <c r="E13" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtNumeroDocumento=By.xpath("//*[@id="document"]");</v>
       </c>
@@ -8207,16 +8508,16 @@
       <c r="A14" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B14" s="122" t="s">
+      <c r="B14" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="93" t="s">
         <v>386</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="D14" s="93" t="s">
         <v>329</v>
       </c>
-      <c r="E14" s="122" t="str">
+      <c r="E14" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbMsgErrorDocumento=By.xpath("//*[@id="query-container"]/section/div[1]/span[2]");</v>
       </c>
@@ -8225,16 +8526,16 @@
       <c r="A15" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C15" s="122" t="s">
+      <c r="C15" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="122" t="s">
+      <c r="D15" s="93" t="s">
         <v>330</v>
       </c>
-      <c r="E15" s="122" t="str">
+      <c r="E15" s="93" t="str">
         <f t="shared" ref="E15" si="1">CONCATENATE("public By ",B15,C15,"=By.",IF(ISNUMBER(SEARCH("@id=",D15)),"xpath(""","id("""),D15,""");")</f>
         <v>public By btnConsultar=By.xpath("//*[@id="findagenda"]/div[2]/div[2]");</v>
       </c>
@@ -8243,16 +8544,16 @@
       <c r="A16" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B16" s="122" t="s">
+      <c r="B16" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="122" t="s">
+      <c r="C16" s="93" t="s">
         <v>384</v>
       </c>
-      <c r="D16" s="122" t="s">
+      <c r="D16" s="93" t="s">
         <v>385</v>
       </c>
-      <c r="E16" s="122" t="str">
+      <c r="E16" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbVisitasPendientes=By.xpath("//*[@id=\'schedule-visits-container\']/div[2]/div[1]/div/p");</v>
       </c>
@@ -8261,16 +8562,16 @@
       <c r="A17" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B17" s="122" t="s">
+      <c r="B17" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C17" s="122" t="s">
+      <c r="C17" s="93" t="s">
         <v>331</v>
       </c>
-      <c r="D17" s="122" t="s">
+      <c r="D17" s="93" t="s">
         <v>332</v>
       </c>
-      <c r="E17" s="122" t="str">
+      <c r="E17" s="93" t="str">
         <f t="shared" ref="E17" si="2">CONCATENATE("public By ",B17,C17,"=By.",IF(ISNUMBER(SEARCH("@id=",D17)),"xpath(""","id("""),D17,""");")</f>
         <v>public By txtConsultaPQRUne=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[1]/p/a");</v>
       </c>
@@ -8279,16 +8580,16 @@
       <c r="A18" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="93" t="s">
         <v>374</v>
       </c>
-      <c r="D18" s="122" t="s">
+      <c r="D18" s="93" t="s">
         <v>375</v>
       </c>
-      <c r="E18" s="122" t="str">
+      <c r="E18" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbPQRUne=By.id("/html/body/div[4]/div/div/div/div[1]/h3");</v>
       </c>
@@ -8297,16 +8598,16 @@
       <c r="A19" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="93" t="s">
         <v>333</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="93" t="s">
         <v>334</v>
       </c>
-      <c r="E19" s="122" t="str">
+      <c r="E19" s="93" t="str">
         <f t="shared" ref="E19" si="3">CONCATENATE("public By ",B19,C19,"=By.",IF(ISNUMBER(SEARCH("@id=",D19)),"xpath(""","id("""),D19,""");")</f>
         <v>public By txtConsultaPQRTigo=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[2]/p/a");</v>
       </c>
@@ -8315,16 +8616,16 @@
       <c r="A20" s="26" t="s">
         <v>380</v>
       </c>
-      <c r="B20" s="122" t="s">
+      <c r="B20" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C20" s="122" t="s">
+      <c r="C20" s="93" t="s">
         <v>376</v>
       </c>
-      <c r="D20" s="122" t="s">
+      <c r="D20" s="93" t="s">
         <v>377</v>
       </c>
-      <c r="E20" s="122" t="str">
+      <c r="E20" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbPQRTigo=By.xpath("//*[@id='formInicioPqr:panelBotonesInicio']/thead/tr/th/span");</v>
       </c>
@@ -8333,16 +8634,16 @@
       <c r="A21" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="122" t="s">
+      <c r="C21" s="93" t="s">
         <v>335</v>
       </c>
-      <c r="D21" s="122" t="s">
+      <c r="D21" s="93" t="s">
         <v>336</v>
       </c>
-      <c r="E21" s="122" t="str">
+      <c r="E21" s="93" t="str">
         <f t="shared" ref="E21" si="4">CONCATENATE("public By ",B21,C21,"=By.",IF(ISNUMBER(SEARCH("@id=",D21)),"xpath(""","id("""),D21,""");")</f>
         <v>public By txtConsultaSic=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[3]/p/a");</v>
       </c>
@@ -8351,16 +8652,16 @@
       <c r="A22" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="B22" s="122" t="s">
+      <c r="B22" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="93" t="s">
         <v>378</v>
       </c>
-      <c r="D22" s="122" t="s">
+      <c r="D22" s="93" t="s">
         <v>379</v>
       </c>
-      <c r="E22" s="122" t="str">
+      <c r="E22" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbSic=By.xpath("//*[@id=\'contenido_medio\']/div[1]/h1");</v>
       </c>
@@ -8369,16 +8670,16 @@
       <c r="A23" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B23" s="122" t="s">
+      <c r="B23" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C23" s="122" t="s">
+      <c r="C23" s="93" t="s">
         <v>337</v>
       </c>
-      <c r="D23" s="122" t="s">
+      <c r="D23" s="93" t="s">
         <v>338</v>
       </c>
-      <c r="E23" s="122" t="str">
+      <c r="E23" s="93" t="str">
         <f t="shared" ref="E23" si="5">CONCATENATE("public By ",B23,C23,"=By.",IF(ISNUMBER(SEARCH("@id=",D23)),"xpath(""","id("""),D23,""");")</f>
         <v>public By txtConoceNuestrasTiendas=By.xpath("//*[@id="main-content"]/div[2]/div[9]/div/div/div/div/div/div/div/div[4]/p/a");</v>
       </c>
@@ -8387,16 +8688,16 @@
       <c r="A24" s="26" t="s">
         <v>382</v>
       </c>
-      <c r="B24" s="122" t="s">
+      <c r="B24" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C24" s="122" t="s">
+      <c r="C24" s="93" t="s">
         <v>382</v>
       </c>
-      <c r="D24" s="122" t="s">
+      <c r="D24" s="93" t="s">
         <v>383</v>
       </c>
-      <c r="E24" s="122" t="str">
+      <c r="E24" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbTiendas=By.id("/html/body/content/div[2]/div/section[1]/div/div/h3");</v>
       </c>
@@ -8405,16 +8706,16 @@
       <c r="A25" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B25" s="122" t="s">
+      <c r="B25" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C25" s="122" t="s">
+      <c r="C25" s="93" t="s">
         <v>339</v>
       </c>
-      <c r="D25" s="122" t="s">
+      <c r="D25" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="E25" s="122" t="str">
+      <c r="E25" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnChatYAyuda=By.xpath("//*[@id="Embed"]/button/span[2]");</v>
       </c>
@@ -8423,16 +8724,16 @@
       <c r="A26" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B26" s="122" t="s">
+      <c r="B26" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C26" s="122" t="s">
+      <c r="C26" s="93" t="s">
         <v>341</v>
       </c>
-      <c r="D26" s="122" t="s">
+      <c r="D26" s="93" t="s">
         <v>342</v>
       </c>
-      <c r="E26" s="122" t="str">
+      <c r="E26" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtPersonas=By.xpath("//*[@id="top_menu"]/nav/ul/li[1]/a");</v>
       </c>
@@ -8441,16 +8742,16 @@
       <c r="A27" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B27" s="122" t="s">
+      <c r="B27" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C27" s="122" t="s">
+      <c r="C27" s="93" t="s">
         <v>343</v>
       </c>
-      <c r="D27" s="122" t="s">
+      <c r="D27" s="93" t="s">
         <v>344</v>
       </c>
-      <c r="E27" s="122" t="str">
+      <c r="E27" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtEmpresas=By.xpath("//*[@id="top_menu"]/nav/ul/li[2]/a");</v>
       </c>
@@ -8459,255 +8760,417 @@
       <c r="A28" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="122" t="s">
+      <c r="C28" s="93" t="s">
         <v>345</v>
       </c>
-      <c r="D28" s="122" t="s">
+      <c r="D28" s="93" t="s">
         <v>346</v>
       </c>
-      <c r="E28" s="122" t="str">
+      <c r="E28" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnDescubreloYa=By.xpath("//*[@id="main-content"]/div[2]/div[1]/div/div/div/section/div/div/a");</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B29" s="124" t="s">
+      <c r="B29" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C29" s="124" t="s">
+      <c r="C29" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="D29" s="124" t="s">
+      <c r="D29" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="E29" s="124" t="str">
+      <c r="E29" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCorreoElectronico=By.id("idEmail");</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="123" t="s">
+      <c r="A30" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B30" s="124" t="s">
+      <c r="B30" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="C30" s="124" t="s">
+      <c r="C30" s="95" t="s">
         <v>349</v>
       </c>
-      <c r="D30" s="124" t="s">
+      <c r="D30" s="95" t="s">
         <v>350</v>
       </c>
-      <c r="E30" s="124" t="str">
+      <c r="E30" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By btnValidarCorreo=By.id("continueBtn");</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="123" t="s">
+      <c r="A31" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="95" t="s">
         <v>236</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="95" t="s">
         <v>371</v>
       </c>
-      <c r="D31" s="124" t="s">
+      <c r="D31" s="95" t="s">
         <v>372</v>
       </c>
-      <c r="E31" s="124" t="str">
+      <c r="E31" s="95" t="str">
         <f t="shared" ref="E31" si="6">CONCATENATE("public By ",B31,C31,"=By.",IF(ISNUMBER(SEARCH("@id=",D31)),"xpath(""","id("""),D31,""");")</f>
         <v>public By lbIngresaAMiCuenta=By.id("/html/body/div[2]/div/div[1]/h5");</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="123" t="s">
+      <c r="A32" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B32" s="124" t="s">
+      <c r="B32" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C32" s="124" t="s">
+      <c r="C32" s="95" t="s">
         <v>351</v>
       </c>
-      <c r="D32" s="124" t="s">
+      <c r="D32" s="95" t="s">
         <v>352</v>
       </c>
-      <c r="E32" s="124" t="str">
+      <c r="E32" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCrearTuCuenta=By.id("/html/body/div[2]/div/div[3]/div/p[2]/a");</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="123" t="s">
+      <c r="A33" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B33" s="124" t="s">
+      <c r="B33" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C33" s="124" t="s">
+      <c r="C33" s="95" t="s">
         <v>353</v>
       </c>
-      <c r="D33" s="124" t="s">
+      <c r="D33" s="95" t="s">
         <v>354</v>
       </c>
-      <c r="E33" s="124" t="str">
+      <c r="E33" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtContraseña=By.id("password");</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="123" t="s">
+      <c r="A34" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B34" s="124" t="s">
+      <c r="B34" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="C34" s="124" t="s">
+      <c r="C34" s="95" t="s">
         <v>355</v>
       </c>
-      <c r="D34" s="124" t="s">
+      <c r="D34" s="95" t="s">
         <v>356</v>
       </c>
-      <c r="E34" s="124" t="str">
+      <c r="E34" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By btnContinuar=By.id("/html/body/div[2]/div/form/div[3]/button");</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="123" t="s">
+      <c r="A35" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B35" s="124" t="s">
+      <c r="B35" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C35" s="124" t="s">
+      <c r="C35" s="95" t="s">
         <v>373</v>
       </c>
-      <c r="D35" s="124" t="s">
+      <c r="D35" s="95" t="s">
         <v>357</v>
       </c>
-      <c r="E35" s="124" t="str">
+      <c r="E35" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtOlvidasteContrasena =By.id("/html/body/div[2]/div/form/div[4]/a");</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="123" t="s">
+      <c r="A36" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B36" s="124" t="s">
+      <c r="B36" s="95" t="s">
         <v>234</v>
       </c>
-      <c r="C36" s="124" t="s">
+      <c r="C36" s="95" t="s">
         <v>358</v>
       </c>
-      <c r="D36" s="124" t="s">
+      <c r="D36" s="95" t="s">
         <v>359</v>
       </c>
-      <c r="E36" s="124" t="str">
-        <f t="shared" si="0"/>
+      <c r="E36" s="95" t="str">
+        <f t="shared" ref="E36:E39" si="7">CONCATENATE("public By ",B36,C36,"=By.",IF(ISNUMBER(SEARCH("@id=",D36)),"xpath(""","id("""),D36,""");")</f>
         <v>public By listNumeroPlan=By.xpath("//*[@id="block-accountsblock-2"]/div/div/div/div/div/span");</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="123" t="s">
+      <c r="A37" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B37" s="124" t="s">
+      <c r="B37" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="95" t="s">
+        <v>415</v>
+      </c>
+      <c r="D37" s="95" t="s">
+        <v>416</v>
+      </c>
+      <c r="E37" s="95" t="str">
+        <f t="shared" si="7"/>
+        <v>public By listLineaPruebasJuanca=By.xpath("(((//*[@id='lines'])//a[contains(@href,'')]))[11]");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B38" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C38" s="95" t="s">
+        <v>417</v>
+      </c>
+      <c r="D38" s="95" t="s">
+        <v>418</v>
+      </c>
+      <c r="E38" s="95" t="str">
+        <f t="shared" ref="E38" si="8">CONCATENATE("public By ",B38,C38,"=By.",IF(ISNUMBER(SEARCH("@id=",D38)),"xpath(""","id("""),D38,""");")</f>
+        <v>public By listLineaHibridoMariana=By.xpath("(((((//*[@id='lines'])//a[contains(@href,'')])))//*[contains(text(),'Mariana')])[2]");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B39" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" s="95" t="s">
+        <v>419</v>
+      </c>
+      <c r="D39" s="95" t="s">
+        <v>420</v>
+      </c>
+      <c r="E39" s="95" t="str">
+        <f t="shared" si="7"/>
+        <v>public By listLineaHibridoAna=By.xpath("(((//*[@id='lines'])//a[contains(@href,'')]))[9]");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B40" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C37" s="124" t="s">
+      <c r="C40" s="95" t="s">
         <v>360</v>
       </c>
-      <c r="D37" s="124" t="s">
+      <c r="D40" s="95" t="s">
         <v>361</v>
       </c>
-      <c r="E37" s="124" t="str">
+      <c r="E40" s="95" t="str">
         <f t="shared" si="0"/>
         <v>public By txtResumen=By.id("/html/body/div[3]/div[2]/div/div/nav/div/div/ul/li[1]/a");</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="123" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="B38" s="124" t="s">
+      <c r="B41" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C38" s="124" t="s">
+      <c r="C41" s="95" t="s">
         <v>362</v>
       </c>
-      <c r="D38" s="124" t="s">
+      <c r="D41" s="95" t="s">
         <v>363</v>
       </c>
-      <c r="E38" s="124" t="str">
-        <f t="shared" si="0"/>
+      <c r="E41" s="95" t="str">
+        <f t="shared" ref="E41:E46" si="9">CONCATENATE("public By ",B41,C41,"=By.",IF(ISNUMBER(SEARCH("@id=",D41)),"xpath(""","id("""),D41,""");")</f>
         <v>public By txtCambiateYa=By.xpath("//*[@id="action_Cámbiate ya"]");</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="125" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B42" s="95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="95" t="s">
+        <v>421</v>
+      </c>
+      <c r="D42" s="95" t="s">
+        <v>422</v>
+      </c>
+      <c r="E42" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By txtUsuario=By.xpath("//*[@id='top_menu_aside']/nav/ul/li/a");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B43" s="95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="95" t="s">
+        <v>423</v>
+      </c>
+      <c r="D43" s="95" t="s">
+        <v>424</v>
+      </c>
+      <c r="E43" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By txtCerrarSesion=By.xpath("//*[@id='top_menu_aside']/nav/ul/li/ul/li[2]/a");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B44" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C44" s="95" t="s">
+        <v>425</v>
+      </c>
+      <c r="D44" s="95" t="s">
+        <v>426</v>
+      </c>
+      <c r="E44" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By btnCambiarCuenta=By.xpath("//*[@id='addNew']");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B45" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C45" s="95" t="s">
+        <v>427</v>
+      </c>
+      <c r="D45" s="95" t="s">
+        <v>428</v>
+      </c>
+      <c r="E45" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By lbPlanes=By.xpath("//*[@id='main-content']/div[2]");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B46" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C46" s="95" t="s">
+        <v>429</v>
+      </c>
+      <c r="D46" s="95" t="s">
+        <v>430</v>
+      </c>
+      <c r="E46" s="95" t="str">
+        <f t="shared" si="9"/>
+        <v>public By lbMejorarPlan=By.xpath("//*[@id='compras-noplan-container']/h3");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B47" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C47" s="95" t="s">
+        <v>431</v>
+      </c>
+      <c r="D47" s="95" t="s">
+        <v>432</v>
+      </c>
+      <c r="E47" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbDetallePlan=By.xpath("//*[@id='compras-noplan-container']/p");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="B39" s="126" t="s">
+      <c r="B48" s="97" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="126" t="s">
+      <c r="C48" s="97" t="s">
         <v>365</v>
       </c>
-      <c r="D39" s="126" t="s">
+      <c r="D48" s="97" t="s">
         <v>366</v>
       </c>
-      <c r="E39" s="126" t="str">
+      <c r="E48" s="97" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConMiCorreo=By.xpath("//*[@id="addNew"]");</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="125" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="B40" s="126" t="s">
+      <c r="B49" s="97" t="s">
         <v>232</v>
       </c>
-      <c r="C40" s="126" t="s">
+      <c r="C49" s="97" t="s">
         <v>367</v>
       </c>
-      <c r="D40" s="126" t="s">
+      <c r="D49" s="97" t="s">
         <v>368</v>
       </c>
-      <c r="E40" s="126" t="str">
+      <c r="E49" s="97" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConFacebook=By.xpath("//*[@id="SLFacebook"]");</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="127" t="s">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="98" t="s">
         <v>364</v>
       </c>
-      <c r="B41" s="128" t="s">
+      <c r="B50" s="99" t="s">
         <v>232</v>
       </c>
-      <c r="C41" s="128" t="s">
+      <c r="C50" s="99" t="s">
         <v>369</v>
       </c>
-      <c r="D41" s="128" t="s">
+      <c r="D50" s="99" t="s">
         <v>370</v>
       </c>
-      <c r="E41" s="128" t="str">
+      <c r="E50" s="99" t="str">
         <f t="shared" si="0"/>
         <v>public By btnConGoogle=By.xpath("//*[@id="SLGoogle"]");</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8718,8 +9181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E972679-EDA2-4ED9-97F5-E044AE9E5203}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="E40" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8733,7 +9196,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="89" t="s">
-        <v>387</v>
+        <v>434</v>
       </c>
       <c r="B1" s="90"/>
       <c r="C1" s="90"/>
@@ -8759,16 +9222,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C3" s="48" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>389</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>390</v>
       </c>
       <c r="E3" s="48" t="str">
         <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
@@ -8777,16 +9240,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>235</v>
       </c>
       <c r="C4" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>391</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>392</v>
       </c>
       <c r="E4" s="48" t="str">
         <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
@@ -8795,16 +9258,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B5" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C5" s="48" t="s">
+        <v>392</v>
+      </c>
+      <c r="D5" s="48" t="s">
         <v>393</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>394</v>
       </c>
       <c r="E5" s="48" t="str">
         <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
@@ -8813,16 +9276,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C6" s="50" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6" s="48" t="s">
         <v>395</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>396</v>
       </c>
       <c r="E6" s="48" t="str">
         <f t="shared" ref="E6:E69" si="0">CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
@@ -8831,16 +9294,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C7" s="48" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="48" t="s">
         <v>397</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>398</v>
       </c>
       <c r="E7" s="48" t="str">
         <f t="shared" si="0"/>
@@ -8849,16 +9312,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>232</v>
       </c>
       <c r="C8" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="D8" s="48" t="s">
         <v>399</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>400</v>
       </c>
       <c r="E8" s="48" t="str">
         <f t="shared" si="0"/>
@@ -8867,16 +9330,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B9" s="91" t="s">
         <v>232</v>
       </c>
       <c r="C9" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="D9" s="91" t="s">
         <v>401</v>
-      </c>
-      <c r="D9" s="91" t="s">
-        <v>402</v>
       </c>
       <c r="E9" s="91" t="str">
         <f t="shared" si="0"/>
@@ -8885,144 +9348,144 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="B10" s="122" t="s">
+        <v>387</v>
+      </c>
+      <c r="B10" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="93" t="s">
+        <v>402</v>
+      </c>
+      <c r="D10" s="93" t="s">
         <v>403</v>
       </c>
-      <c r="D10" s="122" t="s">
-        <v>404</v>
-      </c>
-      <c r="E10" s="122" t="str">
+      <c r="E10" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By btnOtroValor=By.xpath("//*[@id="container_recharge"]/div/div[1]/div/ul/div/li[6]");</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="B11" s="122" t="s">
+        <v>387</v>
+      </c>
+      <c r="B11" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="93" t="s">
+        <v>404</v>
+      </c>
+      <c r="D11" s="93" t="s">
         <v>405</v>
       </c>
-      <c r="D11" s="122" t="s">
-        <v>406</v>
-      </c>
-      <c r="E11" s="122" t="str">
+      <c r="E11" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtValorRecargar=By.id("edit-otro-valor");</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="B12" s="122" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="93" t="s">
+        <v>406</v>
+      </c>
+      <c r="D12" s="93" t="s">
         <v>407</v>
       </c>
-      <c r="D12" s="122" t="s">
-        <v>408</v>
-      </c>
-      <c r="E12" s="122" t="str">
+      <c r="E12" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By lbErrorValor=By.xpath("//*[@id="other_value"]/div/div/div[1]/p");</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="B13" s="122" t="s">
+        <v>387</v>
+      </c>
+      <c r="B13" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="93" t="s">
         <v>255</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="122" t="str">
+      <c r="E13" s="93" t="str">
         <f t="shared" si="0"/>
         <v>public By txtCorreoElectronico=By.id("edit-email");</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="B14" s="122" t="s">
+        <v>387</v>
+      </c>
+      <c r="B14" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="93" t="s">
+        <v>408</v>
+      </c>
+      <c r="D14" s="93" t="s">
         <v>409</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="E14" s="93" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnRecargar=By.id("edit-button-recargar");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="101" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="101" t="s">
         <v>410</v>
       </c>
-      <c r="E14" s="122" t="str">
-        <f t="shared" si="0"/>
-        <v>public By btnRecargar=By.id("edit-button-recargar");</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="129" t="s">
+      <c r="D15" s="101" t="s">
+        <v>411</v>
+      </c>
+      <c r="E15" s="101" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbResumenTransaccion=By.xpath("//*[@id="title-detail"]");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B16" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="C15" s="130" t="s">
-        <v>411</v>
-      </c>
-      <c r="D15" s="130" t="s">
+      <c r="C16" s="101" t="s">
         <v>412</v>
       </c>
-      <c r="E15" s="130" t="str">
-        <f t="shared" si="0"/>
-        <v>public By lbResumenTransaccion=By.xpath("//*[@id="title-detail"]");</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="129" t="s">
+      <c r="D16" s="101" t="s">
+        <v>413</v>
+      </c>
+      <c r="E16" s="101" t="str">
+        <f t="shared" si="0"/>
+        <v>public By lbNumeroDelProducto=By.id("product-number");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="102" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="130" t="s">
+      <c r="B17" s="103" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="130" t="s">
-        <v>413</v>
-      </c>
-      <c r="D16" s="130" t="s">
+      <c r="C17" s="103" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="103" t="s">
         <v>414</v>
       </c>
-      <c r="E16" s="130" t="str">
-        <f t="shared" si="0"/>
-        <v>public By lbNumeroDelProducto=By.id("product-number");</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="131" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="132" t="s">
-        <v>236</v>
-      </c>
-      <c r="C17" s="132" t="s">
-        <v>280</v>
-      </c>
-      <c r="D17" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="E17" s="132" t="str">
+      <c r="E17" s="103" t="str">
         <f t="shared" si="0"/>
         <v>public By lbValorPagar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div[2]/div[3]/div[2]");</v>
       </c>
@@ -10019,5 +10482,1279 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079AA414-3B09-4B31-AC8E-D4CF306B3AF3}">
+  <dimension ref="A1:E70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="92" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="131.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>436</v>
+      </c>
+      <c r="E3" s="48" t="str">
+        <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
+        <v>public By btnPaquetes=By.xpath("//*[@id="tap_selector"]/div[1]");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>437</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="E4" s="48" t="str">
+        <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
+        <v>public By btnOfertas=By.xpath("//*[@id="ofertas"]");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>440</v>
+      </c>
+      <c r="E5" s="48" t="str">
+        <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
+        <v>public By btnSuscripciones=By.xpath("//*[@id="suscripciones"]");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>471</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>472</v>
+      </c>
+      <c r="E6" s="48" t="str">
+        <f>CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
+        <v>public By txtIngresaTuLineaTigo=By.id("numlinsin");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>481</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>482</v>
+      </c>
+      <c r="E7" s="48" t="str">
+        <f>CONCATENATE("public By ",B7,C7,"=By.",IF(ISNUMBER(SEARCH("@id=",D7)),"xpath(""","id("""),D7,""");")</f>
+        <v>public By lbErrorMSISDN=By.xpath("//*[@id="wrrp_step1"]/div/p");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>473</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>474</v>
+      </c>
+      <c r="E8" s="48" t="str">
+        <f>CONCATENATE("public By ",B8,C8,"=By.",IF(ISNUMBER(SEARCH("@id=",D8)),"xpath(""","id("""),D8,""");")</f>
+        <v>public By btnContinuarCompraPaquete=By.id("bt-regsinbal");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>475</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>476</v>
+      </c>
+      <c r="E9" s="48" t="str">
+        <f>CONCATENATE("public By ",B9,C9,"=By.",IF(ISNUMBER(SEARCH("@id=",D9)),"xpath(""","id("""),D9,""");")</f>
+        <v>public By txtCodigoVerificacion=By.id("cod_act");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>477</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>478</v>
+      </c>
+      <c r="E10" s="48" t="str">
+        <f>CONCATENATE("public By ",B10,C10,"=By.",IF(ISNUMBER(SEARCH("@id=",D10)),"xpath(""","id("""),D10,""");")</f>
+        <v>public By lbErrorCodigoVerificacion=By.xpath("//*[@id="mod_regnumber"]/div[3]/div[1]/div/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>479</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>480</v>
+      </c>
+      <c r="E11" s="48" t="str">
+        <f>CONCATENATE("public By ",B11,C11,"=By.",IF(ISNUMBER(SEARCH("@id=",D11)),"xpath(""","id("""),D11,""");")</f>
+        <v>public By btnContinuarVerificacion=By.id("bt-contver");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>483</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>484</v>
+      </c>
+      <c r="E12" s="48" t="str">
+        <f>CONCATENATE("public By ",B12,C12,"=By.",IF(ISNUMBER(SEARCH("@id=",D12)),"xpath(""","id("""),D12,""");")</f>
+        <v>public By txtCorreoVerificacion=By.id("emailpackages");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>486</v>
+      </c>
+      <c r="E13" s="48" t="str">
+        <f>CONCATENATE("public By ",B13,C13,"=By.",IF(ISNUMBER(SEARCH("@id=",D13)),"xpath(""","id("""),D13,""");")</f>
+        <v>public By btnEstoySeguro=By.id("bt-buyconfirmation");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>498</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>499</v>
+      </c>
+      <c r="E14" s="48" t="str">
+        <f>CONCATENATE("public By ",B14,C14,"=By.",IF(ISNUMBER(SEARCH("@id=",D14)),"xpath(""","id("""),D14,""");")</f>
+        <v>public By btnCambiarDeLinea=By.xpath("//*[@id="block-tieneinformaciondesaldoydeudadelmsisdn"]/div/div[2]/div/div/div/div[2]/div[1]/a");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>500</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>501</v>
+      </c>
+      <c r="E15" s="48" t="str">
+        <f>CONCATENATE("public By ",B15,C15,"=By.",IF(ISNUMBER(SEARCH("@id=",D15)),"xpath(""","id("""),D15,""");")</f>
+        <v>public By btnVerMisSuscripciones=By.xpath("//*[@id="suscriptions_trigger"]/a");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B16" s="133" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="134" t="s">
+        <v>441</v>
+      </c>
+      <c r="D16" s="133" t="s">
+        <v>442</v>
+      </c>
+      <c r="E16" s="133" t="str">
+        <f t="shared" ref="E16:E24" si="0">CONCATENATE("public By ",B16,C16,"=By.",IF(ISNUMBER(SEARCH("@id=",D16)),"xpath(""","id("""),D16,""");")</f>
+        <v>public By btnFlechaAtras=By.xpath("//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[1]");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B17" s="133" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="133" t="s">
+        <v>443</v>
+      </c>
+      <c r="D17" s="133" t="s">
+        <v>444</v>
+      </c>
+      <c r="E17" s="133" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnFlechaAdelante=By.xpath("//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[2]");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B18" s="133" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" s="133" t="s">
+        <v>445</v>
+      </c>
+      <c r="D18" s="133" t="s">
+        <v>456</v>
+      </c>
+      <c r="E18" s="133" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar600MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[1]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B19" s="135" t="s">
+        <v>232</v>
+      </c>
+      <c r="C19" s="133" t="s">
+        <v>446</v>
+      </c>
+      <c r="D19" s="135" t="s">
+        <v>457</v>
+      </c>
+      <c r="E19" s="135" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar350MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[2]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B20" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" s="95" t="s">
+        <v>450</v>
+      </c>
+      <c r="D20" s="95" t="s">
+        <v>458</v>
+      </c>
+      <c r="E20" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar2GB30Dias=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[3]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B21" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C21" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="D21" s="95" t="s">
+        <v>459</v>
+      </c>
+      <c r="E21" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar40MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[4]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B22" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C22" s="95" t="s">
+        <v>448</v>
+      </c>
+      <c r="D22" s="95" t="s">
+        <v>460</v>
+      </c>
+      <c r="E22" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar100MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[5]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B23" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="95" t="s">
+        <v>449</v>
+      </c>
+      <c r="D23" s="95" t="s">
+        <v>461</v>
+      </c>
+      <c r="E23" s="95" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar2GB15Dias=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[6]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B24" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C24" s="95" t="s">
+        <v>451</v>
+      </c>
+      <c r="D24" s="136" t="s">
+        <v>462</v>
+      </c>
+      <c r="E24" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v>public By btnComprar150MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[7]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B25" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="95" t="s">
+        <v>452</v>
+      </c>
+      <c r="D25" s="136" t="s">
+        <v>463</v>
+      </c>
+      <c r="E25" s="136" t="str">
+        <f t="shared" ref="E25:E26" si="1">CONCATENATE("public By ",B25,C25,"=By.",IF(ISNUMBER(SEARCH("@id=",D25)),"xpath(""","id("""),D25,""");")</f>
+        <v>public By btnComprar120MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[8]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B26" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="95" t="s">
+        <v>453</v>
+      </c>
+      <c r="D26" s="136" t="s">
+        <v>464</v>
+      </c>
+      <c r="E26" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v>public By btnComprar1GB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[9]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="94" t="s">
+        <v>437</v>
+      </c>
+      <c r="B27" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C27" s="95" t="s">
+        <v>455</v>
+      </c>
+      <c r="D27" s="136" t="s">
+        <v>465</v>
+      </c>
+      <c r="E27" s="136" t="str">
+        <f t="shared" ref="E27" si="2">CONCATENATE("public By ",B27,C27,"=By.",IF(ISNUMBER(SEARCH("@id=",D27)),"xpath(""","id("""),D27,""");")</f>
+        <v>public By btnComprar50MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[10]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="137" t="s">
+        <v>437</v>
+      </c>
+      <c r="B28" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="136" t="s">
+        <v>454</v>
+      </c>
+      <c r="D28" s="136" t="s">
+        <v>466</v>
+      </c>
+      <c r="E28" s="136" t="str">
+        <f t="shared" ref="E28" si="3">CONCATENATE("public By ",B28,C28,"=By.",IF(ISNUMBER(SEARCH("@id=",D28)),"xpath(""","id("""),D28,""");")</f>
+        <v>public By btnComprar500MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[11]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="138" t="s">
+        <v>438</v>
+      </c>
+      <c r="B29" s="139" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" s="139" t="s">
+        <v>467</v>
+      </c>
+      <c r="D29" s="139" t="s">
+        <v>468</v>
+      </c>
+      <c r="E29" s="139" t="str">
+        <f t="shared" ref="E29" si="4">CONCATENATE("public By ",B29,C29,"=By.",IF(ISNUMBER(SEARCH("@id=",D29)),"xpath(""","id("""),D29,""");")</f>
+        <v>public By btnComprarSuscripcion1GB=By.xpath("//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[1]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="138" t="s">
+        <v>438</v>
+      </c>
+      <c r="B30" s="139" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="139" t="s">
+        <v>469</v>
+      </c>
+      <c r="D30" s="139" t="s">
+        <v>470</v>
+      </c>
+      <c r="E30" s="139" t="str">
+        <f t="shared" ref="E30:E70" si="5">CONCATENATE("public By ",B30,C30,"=By.",IF(ISNUMBER(SEARCH("@id=",D30)),"xpath(""","id("""),D30,""");")</f>
+        <v>public By btnComprarSuscripcion2GB=By.xpath("//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[2]/div/div[2]/div/a");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="101" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="101" t="s">
+        <v>410</v>
+      </c>
+      <c r="D31" s="101" t="s">
+        <v>487</v>
+      </c>
+      <c r="E31" s="101" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbResumenTransaccion=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="101" t="s">
+        <v>236</v>
+      </c>
+      <c r="C32" s="101" t="s">
+        <v>412</v>
+      </c>
+      <c r="D32" s="101" t="s">
+        <v>488</v>
+      </c>
+      <c r="E32" s="101" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbNumeroDelProducto=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[1]/b");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="103" t="s">
+        <v>236</v>
+      </c>
+      <c r="C33" s="103" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" s="103" t="s">
+        <v>489</v>
+      </c>
+      <c r="E33" s="103" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbValorPagar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[3]");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>490</v>
+      </c>
+      <c r="E34" s="34" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkTarjetaCredito=By.xpath("//*[@id="payment-method-type-label-credit-payu"]/label/div[1]/div[1]");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>491</v>
+      </c>
+      <c r="E35" s="34" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkDebitoBancarioPSE=By.xpath("//*[@id="payment-method-type-label-debit-payu"]/label/div[1]/div[1]");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="140" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>492</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="E36" s="34" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkAdelantaSaldo=By.xpath("//*[@id="payment-method-type-label-advance-balance"]/label/div[1]/div[1]");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtCVV/CVC=By.id("edit-cvc");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listCuotas=By.id("edit-cardnumber-quota");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNombre=By.id("edit-ccname");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listTipo=By.id("edit-buyer-document-type");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone");</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail");</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E51" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize");</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="E53" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnCancelar=By.id("edit-cancel");</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="D55" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit");</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="142" t="s">
+        <v>234</v>
+      </c>
+      <c r="C56" s="142" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="142" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listBanco=By.id("edit-bank");</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="142" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="142" t="s">
+        <v>244</v>
+      </c>
+      <c r="D57" s="142" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listTipodepersona=By.id("edit-buyer-type-person");</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="142" t="s">
+        <v>235</v>
+      </c>
+      <c r="C58" s="142" t="s">
+        <v>245</v>
+      </c>
+      <c r="D58" s="142" t="s">
+        <v>57</v>
+      </c>
+      <c r="E58" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNombresyapellidos=By.id("edit-buyer-name");</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="142" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" s="142" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="142" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By listTipo=By.id("edit-buyer-document-type--2");</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="142" t="s">
+        <v>235</v>
+      </c>
+      <c r="C60" s="142" t="s">
+        <v>246</v>
+      </c>
+      <c r="D60" s="142" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2");</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="142" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" s="142" t="s">
+        <v>264</v>
+      </c>
+      <c r="D61" s="142" t="s">
+        <v>286</v>
+      </c>
+      <c r="E61" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p");</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="142" t="s">
+        <v>235</v>
+      </c>
+      <c r="C62" s="142" t="s">
+        <v>257</v>
+      </c>
+      <c r="D62" s="142" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2");</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="142" t="s">
+        <v>236</v>
+      </c>
+      <c r="C63" s="142" t="s">
+        <v>256</v>
+      </c>
+      <c r="D63" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="E63" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p");</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="142" t="s">
+        <v>233</v>
+      </c>
+      <c r="C64" s="142" t="s">
+        <v>270</v>
+      </c>
+      <c r="D64" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="E64" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a");</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" s="142" t="s">
+        <v>232</v>
+      </c>
+      <c r="C65" s="142" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="142" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnCancelar=By.id("edit-cancel--2");</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="143" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="142" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" s="142" t="s">
+        <v>247</v>
+      </c>
+      <c r="D66" s="142" t="s">
+        <v>65</v>
+      </c>
+      <c r="E66" s="142" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2");</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="B67" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>494</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>495</v>
+      </c>
+      <c r="E67" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>public By lbTeQuedasteSinSaldo=By.xpath("//*[@id="modal"]/div/div/h1");</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="B68" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>496</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>497</v>
+      </c>
+      <c r="E68" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnAdelantarSaldo=By.xpath("//*[@id="modal"]/div/div/button");</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="B69" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E69" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel");</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="144" t="s">
+        <v>492</v>
+      </c>
+      <c r="B70" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C70" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E70" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>public By btnPagar=By.id("tigoune-nequi-button-submit");</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización creación de objetos
</commit_message>
<xml_diff>
--- a/Adherencia Pasarela de pagos.xlsx
+++ b/Adherencia Pasarela de pagos.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasprilla\Documents\automatizacion_base\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9968BD8-128A-4624-A156-0C9DBD449D43}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -26,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ObjetosPasarela!$A$2:$D$77</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Unificado!$A$2:$I$75</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1345,33 +1339,18 @@
     <t>Paquetes</t>
   </si>
   <si>
-    <t>//*[@id="tap_selector"]/div[1]</t>
-  </si>
-  <si>
     <t>Ofertas</t>
   </si>
   <si>
     <t>Suscripciones</t>
   </si>
   <si>
-    <t>//*[@id="ofertas"]</t>
-  </si>
-  <si>
-    <t>//*[@id="suscripciones"]</t>
-  </si>
-  <si>
     <t>FlechaAtras</t>
   </si>
   <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[1]</t>
-  </si>
-  <si>
     <t>FlechaAdelante</t>
   </si>
   <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[2]</t>
-  </si>
-  <si>
     <t>Comprar600MB</t>
   </si>
   <si>
@@ -1405,51 +1384,12 @@
     <t>Comprar50MB</t>
   </si>
   <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[1]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[2]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[3]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[4]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[5]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[6]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[7]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[8]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[9]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[10]/div/div[2]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[11]/div/div[2]/div/a</t>
-  </si>
-  <si>
     <t>ComprarSuscripcion1GB</t>
   </si>
   <si>
-    <t>//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[1]/div/div[2]/div/a</t>
-  </si>
-  <si>
     <t>ComprarSuscripcion2GB</t>
   </si>
   <si>
-    <t>//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[2]/div/div[2]/div/a</t>
-  </si>
-  <si>
     <t>IngresaTuLineaTigo</t>
   </si>
   <si>
@@ -1471,9 +1411,6 @@
     <t>ErrorCodigoVerificacion</t>
   </si>
   <si>
-    <t>//*[@id="mod_regnumber"]/div[3]/div[1]/div/div/div[1]/p</t>
-  </si>
-  <si>
     <t>ContinuarVerificacion</t>
   </si>
   <si>
@@ -1483,9 +1420,6 @@
     <t>ErrorMSISDN</t>
   </si>
   <si>
-    <t>//*[@id="wrrp_step1"]/div/p</t>
-  </si>
-  <si>
     <t>CorreoVerificacion</t>
   </si>
   <si>
@@ -1498,55 +1432,115 @@
     <t>bt-buyconfirmation</t>
   </si>
   <si>
-    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div</t>
-  </si>
-  <si>
-    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[1]/b</t>
-  </si>
-  <si>
-    <t>//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[3]</t>
-  </si>
-  <si>
-    <t>//*[@id="payment-method-type-label-credit-payu"]/label/div[1]/div[1]</t>
-  </si>
-  <si>
-    <t>//*[@id="payment-method-type-label-debit-payu"]/label/div[1]/div[1]</t>
-  </si>
-  <si>
     <t>AdelantaSaldo</t>
   </si>
   <si>
-    <t>//*[@id="payment-method-type-label-advance-balance"]/label/div[1]/div[1]</t>
-  </si>
-  <si>
     <t>TeQuedasteSinSaldo</t>
   </si>
   <si>
-    <t>//*[@id="modal"]/div/div/h1</t>
-  </si>
-  <si>
     <t>AdelantarSaldo</t>
   </si>
   <si>
-    <t>//*[@id="modal"]/div/div/button</t>
-  </si>
-  <si>
     <t>CambiarDeLinea</t>
   </si>
   <si>
-    <t>//*[@id="block-tieneinformaciondesaldoydeudadelmsisdn"]/div/div[2]/div/div/div/div[2]/div[1]/a</t>
-  </si>
-  <si>
     <t>VerMisSuscripciones</t>
   </si>
   <si>
-    <t>//*[@id="suscriptions_trigger"]/a</t>
+    <t>//*[@id='tap_selector']/div[1]</t>
+  </si>
+  <si>
+    <t>//*[@id='ofertas']</t>
+  </si>
+  <si>
+    <t>//*[@id='suscripciones']</t>
+  </si>
+  <si>
+    <t>//*[@id='wrrp_step1']/div/p</t>
+  </si>
+  <si>
+    <t>//*[@id='mod_regnumber']/div[3]/div[1]/div/div/div[1]/p</t>
+  </si>
+  <si>
+    <t>//*[@id='block-tieneinformaciondesaldoydeudadelmsisdn']/div/div[2]/div/div/div/div[2]/div[1]/a</t>
+  </si>
+  <si>
+    <t>//*[@id='suscriptions_trigger']/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[2]/div[2]/a[1]</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[2]/div[2]/a[2]</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[1]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[2]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[3]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[4]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[5]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[6]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[7]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[8]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[9]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[10]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[1]/div[1]/ul/li[11]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[2]/div[1]/ul/li[1]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='tab_navegar']/div[2]/div[1]/ul/li[2]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='block-tigo-theme-content']/div/div[2]/div/div/div</t>
+  </si>
+  <si>
+    <t>//*[@id='block-tigo-theme-content']/div/div[2]/div/div/div/div[1]/p[1]/b</t>
+  </si>
+  <si>
+    <t>//*[@id='block-tigo-theme-content']/div/div[2]/div/div/div/div[1]/p[3]</t>
+  </si>
+  <si>
+    <t>//*[@id='payment-method-type-label-credit-payu']/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>//*[@id='payment-method-type-label-debit-payu']/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>//*[@id='payment-method-type-label-advance-balance']/label/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>//*[@id='modal']/div/div/h1</t>
+  </si>
+  <si>
+    <t>//*[@id='modal']/div/div/button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -2148,6 +2142,42 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2234,47 +2264,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2290,7 +2284,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2332,7 +2326,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2365,26 +2359,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2417,23 +2394,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2609,14 +2569,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -2671,7 +2631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>194</v>
       </c>
@@ -2897,78 +2857,78 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="104" t="s">
+      <c r="A14" s="116" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="104"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
-      <c r="B15" s="104"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="104"/>
+      <c r="A15" s="116"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="104"/>
-      <c r="B16" s="104"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="104"/>
-      <c r="E16" s="104"/>
-      <c r="F16" s="104"/>
+      <c r="A16" s="116"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="104"/>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
+      <c r="A17" s="116"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="104"/>
-      <c r="B18" s="104"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
+      <c r="A18" s="116"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="104"/>
-      <c r="B19" s="104"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="104"/>
+      <c r="A19" s="116"/>
+      <c r="B19" s="116"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="116"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="104"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104"/>
+      <c r="A20" s="116"/>
+      <c r="B20" s="116"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="116"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="104"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
+      <c r="A21" s="116"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="116"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="104"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="104"/>
+      <c r="A22" s="116"/>
+      <c r="B22" s="116"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2979,14 +2939,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" style="39" customWidth="1"/>
     <col min="2" max="2" width="45" style="39" bestFit="1" customWidth="1"/>
@@ -3001,17 +2961,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -4152,7 +4112,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>26</v>
       </c>
@@ -5258,7 +5218,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I75" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A2:I75"/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
@@ -5267,14 +5227,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F10" sqref="F10:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
@@ -5286,14 +5246,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5316,7 +5276,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="130" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -5336,7 +5296,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
+      <c r="A4" s="131"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -5354,7 +5314,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="119"/>
+      <c r="A5" s="131"/>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -5372,7 +5332,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="119"/>
+      <c r="A6" s="131"/>
       <c r="B6" s="3" t="s">
         <v>101</v>
       </c>
@@ -5390,7 +5350,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="119"/>
+      <c r="A7" s="131"/>
       <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
@@ -5411,7 +5371,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="119"/>
+      <c r="A8" s="131"/>
       <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
@@ -5432,7 +5392,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="120"/>
+      <c r="A9" s="132"/>
       <c r="B9" s="3" t="s">
         <v>229</v>
       </c>
@@ -5450,7 +5410,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="139" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -5470,7 +5430,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="128"/>
+      <c r="A11" s="140"/>
       <c r="B11" s="7" t="s">
         <v>124</v>
       </c>
@@ -5491,7 +5451,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="128"/>
+      <c r="A12" s="140"/>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -5509,7 +5469,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="128"/>
+      <c r="A13" s="140"/>
       <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
@@ -5530,7 +5490,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="128"/>
+      <c r="A14" s="140"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -5548,7 +5508,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="128"/>
+      <c r="A15" s="140"/>
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -5566,7 +5526,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="128"/>
+      <c r="A16" s="140"/>
       <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
@@ -5584,7 +5544,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="128"/>
+      <c r="A17" s="140"/>
       <c r="B17" s="7" t="s">
         <v>101</v>
       </c>
@@ -5602,7 +5562,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="128"/>
+      <c r="A18" s="140"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -5620,7 +5580,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="129"/>
+      <c r="A19" s="141"/>
       <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
@@ -5638,7 +5598,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="112" t="s">
+      <c r="A20" s="124" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -5658,7 +5618,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="113"/>
+      <c r="A21" s="125"/>
       <c r="B21" s="4" t="s">
         <v>81</v>
       </c>
@@ -5683,7 +5643,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="113"/>
+      <c r="A22" s="125"/>
       <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
@@ -5701,7 +5661,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="113"/>
+      <c r="A23" s="125"/>
       <c r="B23" s="4" t="s">
         <v>82</v>
       </c>
@@ -5719,7 +5679,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="114"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="4" t="s">
         <v>83</v>
       </c>
@@ -5744,7 +5704,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="115" t="s">
+      <c r="A25" s="127" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -5764,7 +5724,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="116"/>
+      <c r="A26" s="128"/>
       <c r="B26" s="13" t="s">
         <v>27</v>
       </c>
@@ -5782,7 +5742,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="117"/>
+      <c r="A27" s="129"/>
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -5800,7 +5760,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="130" t="s">
+      <c r="A28" s="142" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5820,7 +5780,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="131"/>
+      <c r="A29" s="143"/>
       <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
@@ -5841,7 +5801,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="131"/>
+      <c r="A30" s="143"/>
       <c r="B30" s="15" t="s">
         <v>118</v>
       </c>
@@ -5862,7 +5822,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="131"/>
+      <c r="A31" s="143"/>
       <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
@@ -5880,7 +5840,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="131"/>
+      <c r="A32" s="143"/>
       <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
@@ -5898,7 +5858,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="131"/>
+      <c r="A33" s="143"/>
       <c r="B33" s="15" t="s">
         <v>35</v>
       </c>
@@ -5916,7 +5876,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="131"/>
+      <c r="A34" s="143"/>
       <c r="B34" s="15" t="s">
         <v>36</v>
       </c>
@@ -5934,7 +5894,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="131"/>
+      <c r="A35" s="143"/>
       <c r="B35" s="15" t="s">
         <v>39</v>
       </c>
@@ -5952,7 +5912,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="131"/>
+      <c r="A36" s="143"/>
       <c r="B36" s="15" t="s">
         <v>3</v>
       </c>
@@ -5970,7 +5930,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="131"/>
+      <c r="A37" s="143"/>
       <c r="B37" s="15" t="s">
         <v>42</v>
       </c>
@@ -5988,7 +5948,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="131"/>
+      <c r="A38" s="143"/>
       <c r="B38" s="15" t="s">
         <v>122</v>
       </c>
@@ -6009,7 +5969,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="131"/>
+      <c r="A39" s="143"/>
       <c r="B39" s="15" t="s">
         <v>44</v>
       </c>
@@ -6027,7 +5987,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="131"/>
+      <c r="A40" s="143"/>
       <c r="B40" s="15" t="s">
         <v>130</v>
       </c>
@@ -6048,7 +6008,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="131"/>
+      <c r="A41" s="143"/>
       <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
@@ -6066,7 +6026,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="131"/>
+      <c r="A42" s="143"/>
       <c r="B42" s="15" t="s">
         <v>110</v>
       </c>
@@ -6087,7 +6047,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="131"/>
+      <c r="A43" s="143"/>
       <c r="B43" s="15" t="s">
         <v>47</v>
       </c>
@@ -6103,7 +6063,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="131"/>
+      <c r="A44" s="143"/>
       <c r="B44" s="15" t="s">
         <v>101</v>
       </c>
@@ -6119,7 +6079,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="131"/>
+      <c r="A45" s="143"/>
       <c r="B45" s="15" t="s">
         <v>22</v>
       </c>
@@ -6137,7 +6097,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="132"/>
+      <c r="A46" s="144"/>
       <c r="B46" s="15" t="s">
         <v>51</v>
       </c>
@@ -6155,7 +6115,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="121" t="s">
+      <c r="A47" s="133" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -6175,7 +6135,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="122"/>
+      <c r="A48" s="134"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -6193,7 +6153,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="122"/>
+      <c r="A49" s="134"/>
       <c r="B49" s="5" t="s">
         <v>56</v>
       </c>
@@ -6211,7 +6171,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="122"/>
+      <c r="A50" s="134"/>
       <c r="B50" s="5" t="s">
         <v>3</v>
       </c>
@@ -6229,7 +6189,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="122"/>
+      <c r="A51" s="134"/>
       <c r="B51" s="5" t="s">
         <v>60</v>
       </c>
@@ -6247,7 +6207,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="122"/>
+      <c r="A52" s="134"/>
       <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
@@ -6265,7 +6225,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="122"/>
+      <c r="A53" s="134"/>
       <c r="B53" s="5" t="s">
         <v>101</v>
       </c>
@@ -6281,7 +6241,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="122"/>
+      <c r="A54" s="134"/>
       <c r="B54" s="5" t="s">
         <v>22</v>
       </c>
@@ -6299,7 +6259,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="123"/>
+      <c r="A55" s="135"/>
       <c r="B55" s="5" t="s">
         <v>64</v>
       </c>
@@ -6317,7 +6277,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="124" t="s">
+      <c r="A56" s="136" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -6337,7 +6297,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="125"/>
+      <c r="A57" s="137"/>
       <c r="B57" s="1" t="s">
         <v>101</v>
       </c>
@@ -6353,7 +6313,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="125"/>
+      <c r="A58" s="137"/>
       <c r="B58" s="1" t="s">
         <v>22</v>
       </c>
@@ -6371,7 +6331,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="126"/>
+      <c r="A59" s="138"/>
       <c r="B59" s="1" t="s">
         <v>48</v>
       </c>
@@ -6389,7 +6349,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="107" t="s">
+      <c r="A60" s="119" t="s">
         <v>136</v>
       </c>
       <c r="B60" s="23" t="s">
@@ -6412,7 +6372,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="108"/>
+      <c r="A61" s="120"/>
       <c r="B61" s="23" t="s">
         <v>137</v>
       </c>
@@ -6430,7 +6390,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="108"/>
+      <c r="A62" s="120"/>
       <c r="B62" s="23" t="s">
         <v>138</v>
       </c>
@@ -6448,7 +6408,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="108"/>
+      <c r="A63" s="120"/>
       <c r="B63" s="23" t="s">
         <v>139</v>
       </c>
@@ -6466,7 +6426,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="108"/>
+      <c r="A64" s="120"/>
       <c r="B64" s="23" t="s">
         <v>140</v>
       </c>
@@ -6484,7 +6444,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="108"/>
+      <c r="A65" s="120"/>
       <c r="B65" s="23" t="s">
         <v>141</v>
       </c>
@@ -6502,7 +6462,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="108"/>
+      <c r="A66" s="120"/>
       <c r="B66" s="23" t="s">
         <v>142</v>
       </c>
@@ -6520,7 +6480,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="108"/>
+      <c r="A67" s="120"/>
       <c r="B67" s="23" t="s">
         <v>143</v>
       </c>
@@ -6538,7 +6498,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="108"/>
+      <c r="A68" s="120"/>
       <c r="B68" s="23" t="s">
         <v>144</v>
       </c>
@@ -6556,7 +6516,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="108"/>
+      <c r="A69" s="120"/>
       <c r="B69" s="23" t="s">
         <v>145</v>
       </c>
@@ -6574,7 +6534,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="108"/>
+      <c r="A70" s="120"/>
       <c r="B70" s="23" t="s">
         <v>146</v>
       </c>
@@ -6592,7 +6552,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="108"/>
+      <c r="A71" s="120"/>
       <c r="B71" s="23" t="s">
         <v>147</v>
       </c>
@@ -6610,7 +6570,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="108"/>
+      <c r="A72" s="120"/>
       <c r="B72" s="23" t="s">
         <v>148</v>
       </c>
@@ -6628,7 +6588,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="108"/>
+      <c r="A73" s="120"/>
       <c r="B73" s="23" t="s">
         <v>149</v>
       </c>
@@ -6646,7 +6606,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="109"/>
+      <c r="A74" s="121"/>
       <c r="B74" s="23" t="s">
         <v>150</v>
       </c>
@@ -6681,14 +6641,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" hidden="1" customWidth="1"/>
@@ -6812,14 +6772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" style="39" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
@@ -8257,21 +8217,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D77" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A2:D77"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDA504D-8FF2-405F-AE1B-22086E468A89}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
@@ -9178,14 +9138,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E972679-EDA2-4ED9-97F5-E044AE9E5203}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView topLeftCell="E40" workbookViewId="0">
       <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
@@ -10487,14 +10447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079AA414-3B09-4B31-AC8E-D4CF306B3AF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
@@ -10540,11 +10500,11 @@
         <v>435</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>436</v>
+        <v>472</v>
       </c>
       <c r="E3" s="48" t="str">
-        <f>CONCATENATE("public By ",B3,C3,"=By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,""");")</f>
-        <v>public By btnPaquetes=By.xpath("//*[@id="tap_selector"]/div[1]");</v>
+        <f>CONCATENATE("ActionsUtil.objetosPut(""",B3,C3,""",By.",IF(ISNUMBER(SEARCH("@id=",D3)),"xpath(""","id("""),D3,"""));")</f>
+        <v>ActionsUtil.objetosPut("btnPaquetes",By.xpath("//*[@id='tap_selector']/div[1]"));</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -10555,14 +10515,14 @@
         <v>232</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>439</v>
+        <v>473</v>
       </c>
       <c r="E4" s="48" t="str">
-        <f>CONCATENATE("public By ",B4,C4,"=By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,""");")</f>
-        <v>public By btnOfertas=By.xpath("//*[@id="ofertas"]");</v>
+        <f t="shared" ref="E4:E67" si="0">CONCATENATE("ActionsUtil.objetosPut(""",B4,C4,""",By.",IF(ISNUMBER(SEARCH("@id=",D4)),"xpath(""","id("""),D4,"""));")</f>
+        <v>ActionsUtil.objetosPut("btnOfertas",By.xpath("//*[@id='ofertas']"));</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -10573,14 +10533,14 @@
         <v>232</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>440</v>
+        <v>474</v>
       </c>
       <c r="E5" s="48" t="str">
-        <f>CONCATENATE("public By ",B5,C5,"=By.",IF(ISNUMBER(SEARCH("@id=",D5)),"xpath(""","id("""),D5,""");")</f>
-        <v>public By btnSuscripciones=By.xpath("//*[@id="suscripciones"]");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnSuscripciones",By.xpath("//*[@id='suscripciones']"));</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -10591,14 +10551,14 @@
         <v>235</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="E6" s="48" t="str">
-        <f>CONCATENATE("public By ",B6,C6,"=By.",IF(ISNUMBER(SEARCH("@id=",D6)),"xpath(""","id("""),D6,""");")</f>
-        <v>public By txtIngresaTuLineaTigo=By.id("numlinsin");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtIngresaTuLineaTigo",By.id("numlinsin"));</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -10609,14 +10569,14 @@
         <v>236</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="E7" s="48" t="str">
-        <f>CONCATENATE("public By ",B7,C7,"=By.",IF(ISNUMBER(SEARCH("@id=",D7)),"xpath(""","id("""),D7,""");")</f>
-        <v>public By lbErrorMSISDN=By.xpath("//*[@id="wrrp_step1"]/div/p");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbErrorMSISDN",By.xpath("//*[@id='wrrp_step1']/div/p"));</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -10627,14 +10587,14 @@
         <v>232</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="E8" s="48" t="str">
-        <f>CONCATENATE("public By ",B8,C8,"=By.",IF(ISNUMBER(SEARCH("@id=",D8)),"xpath(""","id("""),D8,""");")</f>
-        <v>public By btnContinuarCompraPaquete=By.id("bt-regsinbal");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnContinuarCompraPaquete",By.id("bt-regsinbal"));</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -10645,14 +10605,14 @@
         <v>235</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="E9" s="48" t="str">
-        <f>CONCATENATE("public By ",B9,C9,"=By.",IF(ISNUMBER(SEARCH("@id=",D9)),"xpath(""","id("""),D9,""");")</f>
-        <v>public By txtCodigoVerificacion=By.id("cod_act");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtCodigoVerificacion",By.id("cod_act"));</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -10663,14 +10623,14 @@
         <v>236</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E10" s="48" t="str">
-        <f>CONCATENATE("public By ",B10,C10,"=By.",IF(ISNUMBER(SEARCH("@id=",D10)),"xpath(""","id("""),D10,""");")</f>
-        <v>public By lbErrorCodigoVerificacion=By.xpath("//*[@id="mod_regnumber"]/div[3]/div[1]/div/div/div[1]/p");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbErrorCodigoVerificacion",By.xpath("//*[@id='mod_regnumber']/div[3]/div[1]/div/div/div[1]/p"));</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -10681,14 +10641,14 @@
         <v>232</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
       <c r="E11" s="48" t="str">
-        <f>CONCATENATE("public By ",B11,C11,"=By.",IF(ISNUMBER(SEARCH("@id=",D11)),"xpath(""","id("""),D11,""");")</f>
-        <v>public By btnContinuarVerificacion=By.id("bt-contver");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnContinuarVerificacion",By.id("bt-contver"));</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -10699,14 +10659,14 @@
         <v>235</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
       <c r="E12" s="48" t="str">
-        <f>CONCATENATE("public By ",B12,C12,"=By.",IF(ISNUMBER(SEARCH("@id=",D12)),"xpath(""","id("""),D12,""");")</f>
-        <v>public By txtCorreoVerificacion=By.id("emailpackages");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtCorreoVerificacion",By.id("emailpackages"));</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -10717,14 +10677,14 @@
         <v>232</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
       <c r="E13" s="48" t="str">
-        <f>CONCATENATE("public By ",B13,C13,"=By.",IF(ISNUMBER(SEARCH("@id=",D13)),"xpath(""","id("""),D13,""");")</f>
-        <v>public By btnEstoySeguro=By.id("bt-buyconfirmation");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnEstoySeguro",By.id("bt-buyconfirmation"));</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -10735,14 +10695,14 @@
         <v>232</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>498</v>
+        <v>470</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
       <c r="E14" s="48" t="str">
-        <f>CONCATENATE("public By ",B14,C14,"=By.",IF(ISNUMBER(SEARCH("@id=",D14)),"xpath(""","id("""),D14,""");")</f>
-        <v>public By btnCambiarDeLinea=By.xpath("//*[@id="block-tieneinformaciondesaldoydeudadelmsisdn"]/div/div[2]/div/div/div/div[2]/div[1]/a");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnCambiarDeLinea",By.xpath("//*[@id='block-tieneinformaciondesaldoydeudadelmsisdn']/div/div[2]/div/div/div/div[2]/div[1]/a"));</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -10753,284 +10713,284 @@
         <v>232</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>500</v>
+        <v>471</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="E15" s="48" t="str">
-        <f>CONCATENATE("public By ",B15,C15,"=By.",IF(ISNUMBER(SEARCH("@id=",D15)),"xpath(""","id("""),D15,""");")</f>
-        <v>public By btnVerMisSuscripciones=By.xpath("//*[@id="suscriptions_trigger"]/a");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnVerMisSuscripciones",By.xpath("//*[@id='suscriptions_trigger']/a"));</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="94" t="s">
-        <v>437</v>
-      </c>
-      <c r="B16" s="133" t="s">
+        <v>436</v>
+      </c>
+      <c r="B16" s="104" t="s">
         <v>232</v>
       </c>
-      <c r="C16" s="134" t="s">
-        <v>441</v>
-      </c>
-      <c r="D16" s="133" t="s">
-        <v>442</v>
-      </c>
-      <c r="E16" s="133" t="str">
-        <f t="shared" ref="E16:E24" si="0">CONCATENATE("public By ",B16,C16,"=By.",IF(ISNUMBER(SEARCH("@id=",D16)),"xpath(""","id("""),D16,""");")</f>
-        <v>public By btnFlechaAtras=By.xpath("//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[1]");</v>
+      <c r="C16" s="105" t="s">
+        <v>438</v>
+      </c>
+      <c r="D16" s="104" t="s">
+        <v>479</v>
+      </c>
+      <c r="E16" s="104" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnFlechaAtras",By.xpath("//*[@id='tab_navegar']/div[1]/div[2]/div[2]/a[1]"));</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="94" t="s">
-        <v>437</v>
-      </c>
-      <c r="B17" s="133" t="s">
+        <v>436</v>
+      </c>
+      <c r="B17" s="104" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="133" t="s">
-        <v>443</v>
-      </c>
-      <c r="D17" s="133" t="s">
-        <v>444</v>
-      </c>
-      <c r="E17" s="133" t="str">
-        <f t="shared" si="0"/>
-        <v>public By btnFlechaAdelante=By.xpath("//*[@id="tab_navegar"]/div[1]/div[2]/div[2]/a[2]");</v>
+      <c r="C17" s="104" t="s">
+        <v>439</v>
+      </c>
+      <c r="D17" s="104" t="s">
+        <v>480</v>
+      </c>
+      <c r="E17" s="104" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnFlechaAdelante",By.xpath("//*[@id='tab_navegar']/div[1]/div[2]/div[2]/a[2]"));</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="94" t="s">
-        <v>437</v>
-      </c>
-      <c r="B18" s="133" t="s">
+        <v>436</v>
+      </c>
+      <c r="B18" s="104" t="s">
         <v>232</v>
       </c>
-      <c r="C18" s="133" t="s">
-        <v>445</v>
-      </c>
-      <c r="D18" s="133" t="s">
-        <v>456</v>
-      </c>
-      <c r="E18" s="133" t="str">
-        <f t="shared" si="0"/>
-        <v>public By btnComprar600MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[1]/div/div[2]/div/a");</v>
+      <c r="C18" s="104" t="s">
+        <v>440</v>
+      </c>
+      <c r="D18" s="104" t="s">
+        <v>481</v>
+      </c>
+      <c r="E18" s="104" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprar600MB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[1]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="94" t="s">
-        <v>437</v>
-      </c>
-      <c r="B19" s="135" t="s">
+        <v>436</v>
+      </c>
+      <c r="B19" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="C19" s="133" t="s">
-        <v>446</v>
-      </c>
-      <c r="D19" s="135" t="s">
-        <v>457</v>
-      </c>
-      <c r="E19" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>public By btnComprar350MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[2]/div/div[2]/div/a");</v>
+      <c r="C19" s="104" t="s">
+        <v>441</v>
+      </c>
+      <c r="D19" s="106" t="s">
+        <v>482</v>
+      </c>
+      <c r="E19" s="106" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprar350MB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[2]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="94" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B20" s="95" t="s">
         <v>232</v>
       </c>
       <c r="C20" s="95" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D20" s="95" t="s">
-        <v>458</v>
+        <v>483</v>
       </c>
       <c r="E20" s="95" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnComprar2GB30Dias=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[3]/div/div[2]/div/a");</v>
+        <v>ActionsUtil.objetosPut("btnComprar2GB30Dias",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[3]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="94" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B21" s="95" t="s">
         <v>232</v>
       </c>
       <c r="C21" s="95" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D21" s="95" t="s">
-        <v>459</v>
+        <v>484</v>
       </c>
       <c r="E21" s="95" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnComprar40MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[4]/div/div[2]/div/a");</v>
+        <v>ActionsUtil.objetosPut("btnComprar40MB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[4]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="94" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B22" s="95" t="s">
         <v>232</v>
       </c>
       <c r="C22" s="95" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D22" s="95" t="s">
-        <v>460</v>
+        <v>485</v>
       </c>
       <c r="E22" s="95" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnComprar100MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[5]/div/div[2]/div/a");</v>
+        <v>ActionsUtil.objetosPut("btnComprar100MB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[5]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="94" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B23" s="95" t="s">
         <v>232</v>
       </c>
       <c r="C23" s="95" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="D23" s="95" t="s">
-        <v>461</v>
+        <v>486</v>
       </c>
       <c r="E23" s="95" t="str">
         <f t="shared" si="0"/>
-        <v>public By btnComprar2GB15Dias=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[6]/div/div[2]/div/a");</v>
+        <v>ActionsUtil.objetosPut("btnComprar2GB15Dias",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[6]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="94" t="s">
-        <v>437</v>
-      </c>
-      <c r="B24" s="136" t="s">
+        <v>436</v>
+      </c>
+      <c r="B24" s="107" t="s">
         <v>232</v>
       </c>
       <c r="C24" s="95" t="s">
-        <v>451</v>
-      </c>
-      <c r="D24" s="136" t="s">
-        <v>462</v>
-      </c>
-      <c r="E24" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v>public By btnComprar150MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[7]/div/div[2]/div/a");</v>
+        <v>446</v>
+      </c>
+      <c r="D24" s="107" t="s">
+        <v>487</v>
+      </c>
+      <c r="E24" s="107" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprar150MB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[7]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="94" t="s">
-        <v>437</v>
-      </c>
-      <c r="B25" s="136" t="s">
+        <v>436</v>
+      </c>
+      <c r="B25" s="107" t="s">
         <v>232</v>
       </c>
       <c r="C25" s="95" t="s">
-        <v>452</v>
-      </c>
-      <c r="D25" s="136" t="s">
-        <v>463</v>
-      </c>
-      <c r="E25" s="136" t="str">
-        <f t="shared" ref="E25:E26" si="1">CONCATENATE("public By ",B25,C25,"=By.",IF(ISNUMBER(SEARCH("@id=",D25)),"xpath(""","id("""),D25,""");")</f>
-        <v>public By btnComprar120MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[8]/div/div[2]/div/a");</v>
+        <v>447</v>
+      </c>
+      <c r="D25" s="107" t="s">
+        <v>488</v>
+      </c>
+      <c r="E25" s="107" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprar120MB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[8]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="94" t="s">
-        <v>437</v>
-      </c>
-      <c r="B26" s="136" t="s">
+        <v>436</v>
+      </c>
+      <c r="B26" s="107" t="s">
         <v>232</v>
       </c>
       <c r="C26" s="95" t="s">
-        <v>453</v>
-      </c>
-      <c r="D26" s="136" t="s">
-        <v>464</v>
-      </c>
-      <c r="E26" s="136" t="str">
-        <f t="shared" si="1"/>
-        <v>public By btnComprar1GB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[9]/div/div[2]/div/a");</v>
+        <v>448</v>
+      </c>
+      <c r="D26" s="107" t="s">
+        <v>489</v>
+      </c>
+      <c r="E26" s="107" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprar1GB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[9]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="94" t="s">
+        <v>436</v>
+      </c>
+      <c r="B27" s="107" t="s">
+        <v>232</v>
+      </c>
+      <c r="C27" s="95" t="s">
+        <v>450</v>
+      </c>
+      <c r="D27" s="107" t="s">
+        <v>490</v>
+      </c>
+      <c r="E27" s="107" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprar50MB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[10]/div/div[2]/div/a"));</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="108" t="s">
+        <v>436</v>
+      </c>
+      <c r="B28" s="107" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="107" t="s">
+        <v>449</v>
+      </c>
+      <c r="D28" s="107" t="s">
+        <v>491</v>
+      </c>
+      <c r="E28" s="107" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprar500MB",By.xpath("//*[@id='tab_navegar']/div[1]/div[1]/ul/li[11]/div/div[2]/div/a"));</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="109" t="s">
         <v>437</v>
       </c>
-      <c r="B27" s="136" t="s">
+      <c r="B29" s="110" t="s">
         <v>232</v>
       </c>
-      <c r="C27" s="95" t="s">
-        <v>455</v>
-      </c>
-      <c r="D27" s="136" t="s">
-        <v>465</v>
-      </c>
-      <c r="E27" s="136" t="str">
-        <f t="shared" ref="E27" si="2">CONCATENATE("public By ",B27,C27,"=By.",IF(ISNUMBER(SEARCH("@id=",D27)),"xpath(""","id("""),D27,""");")</f>
-        <v>public By btnComprar50MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[10]/div/div[2]/div/a");</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="137" t="s">
+      <c r="C29" s="110" t="s">
+        <v>451</v>
+      </c>
+      <c r="D29" s="110" t="s">
+        <v>492</v>
+      </c>
+      <c r="E29" s="110" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprarSuscripcion1GB",By.xpath("//*[@id='tab_navegar']/div[2]/div[1]/ul/li[1]/div/div[2]/div/a"));</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="109" t="s">
         <v>437</v>
       </c>
-      <c r="B28" s="136" t="s">
+      <c r="B30" s="110" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="136" t="s">
-        <v>454</v>
-      </c>
-      <c r="D28" s="136" t="s">
-        <v>466</v>
-      </c>
-      <c r="E28" s="136" t="str">
-        <f t="shared" ref="E28" si="3">CONCATENATE("public By ",B28,C28,"=By.",IF(ISNUMBER(SEARCH("@id=",D28)),"xpath(""","id("""),D28,""");")</f>
-        <v>public By btnComprar500MB=By.xpath("//*[@id="tab_navegar"]/div[1]/div[1]/ul/li[11]/div/div[2]/div/a");</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="138" t="s">
-        <v>438</v>
-      </c>
-      <c r="B29" s="139" t="s">
-        <v>232</v>
-      </c>
-      <c r="C29" s="139" t="s">
-        <v>467</v>
-      </c>
-      <c r="D29" s="139" t="s">
-        <v>468</v>
-      </c>
-      <c r="E29" s="139" t="str">
-        <f t="shared" ref="E29" si="4">CONCATENATE("public By ",B29,C29,"=By.",IF(ISNUMBER(SEARCH("@id=",D29)),"xpath(""","id("""),D29,""");")</f>
-        <v>public By btnComprarSuscripcion1GB=By.xpath("//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[1]/div/div[2]/div/a");</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="138" t="s">
-        <v>438</v>
-      </c>
-      <c r="B30" s="139" t="s">
-        <v>232</v>
-      </c>
-      <c r="C30" s="139" t="s">
-        <v>469</v>
-      </c>
-      <c r="D30" s="139" t="s">
-        <v>470</v>
-      </c>
-      <c r="E30" s="139" t="str">
-        <f t="shared" ref="E30:E70" si="5">CONCATENATE("public By ",B30,C30,"=By.",IF(ISNUMBER(SEARCH("@id=",D30)),"xpath(""","id("""),D30,""");")</f>
-        <v>public By btnComprarSuscripcion2GB=By.xpath("//*[@id="tab_navegar"]/div[2]/div[1]/ul/li[2]/div/div[2]/div/a");</v>
+      <c r="C30" s="110" t="s">
+        <v>452</v>
+      </c>
+      <c r="D30" s="110" t="s">
+        <v>493</v>
+      </c>
+      <c r="E30" s="110" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnComprarSuscripcion2GB",By.xpath("//*[@id='tab_navegar']/div[2]/div[1]/ul/li[2]/div/div[2]/div/a"));</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -11044,11 +11004,11 @@
         <v>410</v>
       </c>
       <c r="D31" s="101" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="E31" s="101" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbResumenTransaccion=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbResumenTransaccion",By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div/div"));</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -11062,11 +11022,11 @@
         <v>412</v>
       </c>
       <c r="D32" s="101" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="E32" s="101" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbNumeroDelProducto=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[1]/b");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbNumeroDelProducto",By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div/div/div[1]/p[1]/b"));</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -11080,11 +11040,11 @@
         <v>280</v>
       </c>
       <c r="D33" s="103" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E33" s="103" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbValorPagar=By.xpath("//*[@id="block-tigo-theme-content"]/div/div[2]/div/div/div/div[1]/p[3]");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbValorPagar",By.xpath("//*[@id='block-tigo-theme-content']/div/div[2]/div/div/div/div[1]/p[3]"));</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -11098,11 +11058,11 @@
         <v>281</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="E34" s="34" t="str">
-        <f t="shared" si="5"/>
-        <v>public By linkTarjetaCredito=By.xpath("//*[@id="payment-method-type-label-credit-payu"]/label/div[1]/div[1]");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("linkTarjetaCredito",By.xpath("//*[@id='payment-method-type-label-credit-payu']/label/div[1]/div[1]"));</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -11116,29 +11076,29 @@
         <v>271</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="E35" s="34" t="str">
-        <f t="shared" si="5"/>
-        <v>public By linkDebitoBancarioPSE=By.xpath("//*[@id="payment-method-type-label-debit-payu"]/label/div[1]/div[1]");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("linkDebitoBancarioPSE",By.xpath("//*[@id='payment-method-type-label-debit-payu']/label/div[1]/div[1]"));</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="140" t="s">
+      <c r="A36" s="111" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>233</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>492</v>
+        <v>467</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="E36" s="34" t="str">
-        <f t="shared" si="5"/>
-        <v>public By linkAdelantaSaldo=By.xpath("//*[@id="payment-method-type-label-advance-balance"]/label/div[1]/div[1]");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("linkAdelantaSaldo",By.xpath("//*[@id='payment-method-type-label-advance-balance']/label/div[1]/div[1]"));</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -11155,8 +11115,8 @@
         <v>29</v>
       </c>
       <c r="E37" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtNumerodetarjeta=By.id("edit-cardnumber");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtNumerodetarjeta",By.id("edit-cardnumber"));</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -11173,8 +11133,8 @@
         <v>165</v>
       </c>
       <c r="E38" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbMensajedeerrortarjetainvalida=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbMensajedeerrortarjetainvalida",By.xpath("//*[@id='image-credit_card']/div/div[1]/p"));</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -11191,8 +11151,8 @@
         <v>165</v>
       </c>
       <c r="E39" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbMensajedeerrortarjetaconnumeronovalido=By.xpath("//*[@id='image-credit_card']/div/div[1]/p");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbMensajedeerrortarjetaconnumeronovalido",By.xpath("//*[@id='image-credit_card']/div/div[1]/p"));</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -11209,8 +11169,8 @@
         <v>31</v>
       </c>
       <c r="E40" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtCVV/CVC=By.id("edit-cvc");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtCVV/CVC",By.id("edit-cvc"));</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -11227,8 +11187,8 @@
         <v>33</v>
       </c>
       <c r="E41" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By listFechaVencimiento-MM=By.id("edit-buyer-card-month-expiration");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("listFechaVencimiento-MM",By.id("edit-buyer-card-month-expiration"));</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -11245,8 +11205,8 @@
         <v>34</v>
       </c>
       <c r="E42" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By listFechaVencimiento-AA=By.id("edit-buyer-card-year-expiration");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("listFechaVencimiento-AA",By.id("edit-buyer-card-year-expiration"));</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -11263,8 +11223,8 @@
         <v>37</v>
       </c>
       <c r="E43" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By listCuotas=By.id("edit-cardnumber-quota");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("listCuotas",By.id("edit-cardnumber-quota"));</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -11281,8 +11241,8 @@
         <v>38</v>
       </c>
       <c r="E44" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtNombre=By.id("edit-ccname");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtNombre",By.id("edit-ccname"));</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -11299,8 +11259,8 @@
         <v>40</v>
       </c>
       <c r="E45" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By listTipo=By.id("edit-buyer-document-type");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("listTipo",By.id("edit-buyer-document-type"));</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -11317,8 +11277,8 @@
         <v>41</v>
       </c>
       <c r="E46" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtNumerodedocumento=By.id("edit-buyer-document");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtNumerodedocumento",By.id("edit-buyer-document"));</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -11335,8 +11295,8 @@
         <v>166</v>
       </c>
       <c r="E47" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document']/div/p");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbMensajedeerrornumerodedocumento",By.xpath("//*[@id='edit-content-document']/div/p"));</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -11353,8 +11313,8 @@
         <v>43</v>
       </c>
       <c r="E48" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtTelefonocelular(Cargaunvalorpordefecto)=By.id("edit-buyer-phone");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtTelefonocelular(Cargaunvalorpordefecto)",By.id("edit-buyer-phone"));</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -11371,8 +11331,8 @@
         <v>167</v>
       </c>
       <c r="E49" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbMensajedeerrortelefonoinvalido=By.xpath("//*[@id='edit-show-phone']/div/p");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbMensajedeerrortelefonoinvalido",By.xpath("//*[@id='edit-show-phone']/div/p"));</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -11389,8 +11349,8 @@
         <v>45</v>
       </c>
       <c r="E50" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtCorreoElectronico=By.id("edit-buyer-mail");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtCorreoElectronico",By.id("edit-buyer-mail"));</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -11407,8 +11367,8 @@
         <v>168</v>
       </c>
       <c r="E51" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email']/div/p");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbMensajedeerrorcorreoelectronico",By.xpath("//*[@id='edit-show-email']/div/p"));</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -11425,8 +11385,8 @@
         <v>46</v>
       </c>
       <c r="E52" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By Check BoxAutorizoestatarjetaparafuturospagos=By.id("edit-buyer-check-authorize");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("Check BoxAutorizoestatarjetaparafuturospagos",By.id("edit-buyer-check-authorize"));</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -11443,8 +11403,8 @@
         <v>169</v>
       </c>
       <c r="E53" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms']/div/a");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("linkTerminosycondiciones",By.xpath("//*[@id='edit-terms']/div/a"));</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -11461,8 +11421,8 @@
         <v>49</v>
       </c>
       <c r="E54" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By btnCancelar=By.id("edit-cancel");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnCancelar",By.id("edit-cancel"));</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -11479,247 +11439,247 @@
         <v>50</v>
       </c>
       <c r="E55" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>public By btnPagar(Sehabilitaalllenarloscampossolicitados)=By.id("edit-submit");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnPagar(Sehabilitaalllenarloscampossolicitados)",By.id("edit-submit"));</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="141" t="s">
+      <c r="A56" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="142" t="s">
+      <c r="B56" s="113" t="s">
         <v>234</v>
       </c>
-      <c r="C56" s="142" t="s">
+      <c r="C56" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="142" t="s">
+      <c r="D56" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="E56" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By listBanco=By.id("edit-bank");</v>
+      <c r="E56" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("listBanco",By.id("edit-bank"));</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="141" t="s">
+      <c r="A57" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B57" s="142" t="s">
+      <c r="B57" s="113" t="s">
         <v>234</v>
       </c>
-      <c r="C57" s="142" t="s">
+      <c r="C57" s="113" t="s">
         <v>244</v>
       </c>
-      <c r="D57" s="142" t="s">
+      <c r="D57" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="E57" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By listTipodepersona=By.id("edit-buyer-type-person");</v>
+      <c r="E57" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("listTipodepersona",By.id("edit-buyer-type-person"));</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="141" t="s">
+      <c r="A58" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B58" s="142" t="s">
+      <c r="B58" s="113" t="s">
         <v>235</v>
       </c>
-      <c r="C58" s="142" t="s">
+      <c r="C58" s="113" t="s">
         <v>245</v>
       </c>
-      <c r="D58" s="142" t="s">
+      <c r="D58" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="E58" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtNombresyapellidos=By.id("edit-buyer-name");</v>
+      <c r="E58" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtNombresyapellidos",By.id("edit-buyer-name"));</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="141" t="s">
+      <c r="A59" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="142" t="s">
+      <c r="B59" s="113" t="s">
         <v>234</v>
       </c>
-      <c r="C59" s="142" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="142" t="s">
+      <c r="C59" s="113" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="E59" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By listTipo=By.id("edit-buyer-document-type--2");</v>
+      <c r="E59" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("listTipo",By.id("edit-buyer-document-type--2"));</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="141" t="s">
+      <c r="A60" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="142" t="s">
+      <c r="B60" s="113" t="s">
         <v>235</v>
       </c>
-      <c r="C60" s="142" t="s">
+      <c r="C60" s="113" t="s">
         <v>246</v>
       </c>
-      <c r="D60" s="142" t="s">
+      <c r="D60" s="113" t="s">
         <v>59</v>
       </c>
-      <c r="E60" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtNumerodedocumento=By.id("edit-buyer-document--2");</v>
+      <c r="E60" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtNumerodedocumento",By.id("edit-buyer-document--2"));</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="141" t="s">
+      <c r="A61" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="142" t="s">
+      <c r="B61" s="113" t="s">
         <v>236</v>
       </c>
-      <c r="C61" s="142" t="s">
+      <c r="C61" s="113" t="s">
         <v>264</v>
       </c>
-      <c r="D61" s="142" t="s">
+      <c r="D61" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="E61" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbMensajedeerrornumerodedocumento=By.xpath("//*[@id='edit-content-document--2']/div/p");</v>
+      <c r="E61" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbMensajedeerrornumerodedocumento",By.xpath("//*[@id='edit-content-document--2']/div/p"));</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="141" t="s">
+      <c r="A62" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="142" t="s">
+      <c r="B62" s="113" t="s">
         <v>235</v>
       </c>
-      <c r="C62" s="142" t="s">
+      <c r="C62" s="113" t="s">
         <v>257</v>
       </c>
-      <c r="D62" s="142" t="s">
+      <c r="D62" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="E62" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By txtCorreoElectronico(Cargaunvalorpordefecto)=By.id("edit-buyer-mail--2");</v>
+      <c r="E62" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("txtCorreoElectronico(Cargaunvalorpordefecto)",By.id("edit-buyer-mail--2"));</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="141" t="s">
+      <c r="A63" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B63" s="142" t="s">
+      <c r="B63" s="113" t="s">
         <v>236</v>
       </c>
-      <c r="C63" s="142" t="s">
+      <c r="C63" s="113" t="s">
         <v>256</v>
       </c>
-      <c r="D63" s="142" t="s">
+      <c r="D63" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="E63" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbMensajedeerrorcorreoelectronico=By.xpath("//*[@id='edit-show-email--2']/div/p");</v>
+      <c r="E63" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbMensajedeerrorcorreoelectronico",By.xpath("//*[@id='edit-show-email--2']/div/p"));</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="141" t="s">
+      <c r="A64" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="142" t="s">
+      <c r="B64" s="113" t="s">
         <v>233</v>
       </c>
-      <c r="C64" s="142" t="s">
+      <c r="C64" s="113" t="s">
         <v>270</v>
       </c>
-      <c r="D64" s="142" t="s">
+      <c r="D64" s="113" t="s">
         <v>288</v>
       </c>
-      <c r="E64" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By linkTerminosycondiciones=By.xpath("//*[@id='edit-terms--2']/div/a");</v>
+      <c r="E64" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("linkTerminosycondiciones",By.xpath("//*[@id='edit-terms--2']/div/a"));</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="141" t="s">
+      <c r="A65" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="142" t="s">
+      <c r="B65" s="113" t="s">
         <v>232</v>
       </c>
-      <c r="C65" s="142" t="s">
+      <c r="C65" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="142" t="s">
+      <c r="D65" s="113" t="s">
         <v>63</v>
       </c>
-      <c r="E65" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By btnCancelar=By.id("edit-cancel--2");</v>
+      <c r="E65" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnCancelar",By.id("edit-cancel--2"));</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="143" t="s">
+      <c r="A66" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="142" t="s">
+      <c r="B66" s="113" t="s">
         <v>232</v>
       </c>
-      <c r="C66" s="142" t="s">
+      <c r="C66" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="D66" s="142" t="s">
+      <c r="D66" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="E66" s="142" t="str">
-        <f t="shared" si="5"/>
-        <v>public By btnPagar(Sehabilitaalllenarloscampos)=By.id("edit-submit--2");</v>
+      <c r="E66" s="113" t="str">
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("btnPagar(Sehabilitaalllenarloscampos)",By.id("edit-submit--2"));</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="32" t="s">
-        <v>492</v>
+        <v>467</v>
       </c>
       <c r="B67" s="37" t="s">
         <v>236</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>494</v>
+        <v>468</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="E67" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v>public By lbTeQuedasteSinSaldo=By.xpath("//*[@id="modal"]/div/div/h1");</v>
+        <f t="shared" si="0"/>
+        <v>ActionsUtil.objetosPut("lbTeQuedasteSinSaldo",By.xpath("//*[@id='modal']/div/div/h1"));</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
-        <v>492</v>
+        <v>467</v>
       </c>
       <c r="B68" s="37" t="s">
         <v>232</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>496</v>
+        <v>469</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="E68" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v>public By btnAdelantarSaldo=By.xpath("//*[@id="modal"]/div/div/button");</v>
+        <f t="shared" ref="E68:E70" si="1">CONCATENATE("ActionsUtil.objetosPut(""",B68,C68,""",By.",IF(ISNUMBER(SEARCH("@id=",D68)),"xpath(""","id("""),D68,"""));")</f>
+        <v>ActionsUtil.objetosPut("btnAdelantarSaldo",By.xpath("//*[@id='modal']/div/div/button"));</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="32" t="s">
-        <v>492</v>
+        <v>467</v>
       </c>
       <c r="B69" s="37" t="s">
         <v>232</v>
@@ -11731,13 +11691,13 @@
         <v>68</v>
       </c>
       <c r="E69" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v>public By btnCancelar=By.id("tigoune-nequi-button-cancel");</v>
+        <f t="shared" si="1"/>
+        <v>ActionsUtil.objetosPut("btnCancelar",By.id("tigoune-nequi-button-cancel"));</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="144" t="s">
-        <v>492</v>
+      <c r="A70" s="115" t="s">
+        <v>467</v>
       </c>
       <c r="B70" s="37" t="s">
         <v>232</v>
@@ -11749,8 +11709,8 @@
         <v>69</v>
       </c>
       <c r="E70" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v>public By btnPagar=By.id("tigoune-nequi-button-submit");</v>
+        <f t="shared" si="1"/>
+        <v>ActionsUtil.objetosPut("btnPagar",By.id("tigoune-nequi-button-submit"));</v>
       </c>
     </row>
   </sheetData>

</xml_diff>